<commit_message>
Fixes to kV formulas
</commit_message>
<xml_diff>
--- a/MUSCMammoHologic.xlsx
+++ b/MUSCMammoHologic.xlsx
@@ -7175,18 +7175,93 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="153" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="55" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="131" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="131" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="55" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="23" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="131" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="132" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="133" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="134" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="135" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="130" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="99" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="55" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="23" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="131" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="55" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="23" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="131" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="25" fillId="14" borderId="55" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="25" fillId="14" borderId="23" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="25" fillId="14" borderId="131" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="55" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="23" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="131" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="175" fontId="25" fillId="14" borderId="55" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -7196,75 +7271,6 @@
     <xf numFmtId="175" fontId="25" fillId="14" borderId="131" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="25" fillId="14" borderId="55" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="25" fillId="14" borderId="23" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="25" fillId="14" borderId="131" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="55" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="23" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="131" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="132" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="133" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="134" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="135" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="130" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="99" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="55" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="23" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="131" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="55" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="131" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="131" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="15" borderId="55" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -7274,6 +7280,27 @@
     <xf numFmtId="0" fontId="24" fillId="15" borderId="131" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="55" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="23" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="131" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="111" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="136" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="112" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -7295,26 +7322,23 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="58" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="141" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="55" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="22" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="23" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="131" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="111" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="136" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="112" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="143" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -7346,9 +7370,6 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="141" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="141" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="143" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -7358,100 +7379,85 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="141" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="58" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="22" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="23" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="108" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="100" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="101" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="98" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="166" fontId="4" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="108" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="100" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="101" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="124" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -7460,12 +7466,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="153" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -7479,13 +7479,75 @@
   <dxfs count="94">
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial1"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+        <name val="Arial1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+        <name val="Arial1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+        <name val="Arial1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+        <name val="Arial1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+        <name val="Arial1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+        <name val="Arial1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+        <name val="Arial1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+        <name val="Arial1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+        <name val="Arial1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+        <name val="Arial1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+        <name val="Arial1"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -7494,6 +7556,16 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -8206,78 +8278,6 @@
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <name val="Arial1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <name val="Arial1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <name val="Arial1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <name val="Arial1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <name val="Arial1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <name val="Arial1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <name val="Arial1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <name val="Arial1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <name val="Arial1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <name val="Arial1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <name val="Arial1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <name val="Arial1"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -16590,40 +16590,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="26.25">
-      <c r="A1" s="595" t="s">
+      <c r="A1" s="623" t="s">
         <v>407</v>
       </c>
-      <c r="B1" s="595"/>
-      <c r="C1" s="595"/>
-      <c r="D1" s="595"/>
-      <c r="E1" s="595"/>
-      <c r="F1" s="595"/>
-      <c r="G1" s="595"/>
-      <c r="H1" s="595"/>
-      <c r="I1" s="595"/>
-      <c r="J1" s="595"/>
-      <c r="K1" s="595"/>
-      <c r="L1" s="595"/>
-      <c r="M1" s="595"/>
-      <c r="N1" s="595"/>
+      <c r="B1" s="623"/>
+      <c r="C1" s="623"/>
+      <c r="D1" s="623"/>
+      <c r="E1" s="623"/>
+      <c r="F1" s="623"/>
+      <c r="G1" s="623"/>
+      <c r="H1" s="623"/>
+      <c r="I1" s="623"/>
+      <c r="J1" s="623"/>
+      <c r="K1" s="623"/>
+      <c r="L1" s="623"/>
+      <c r="M1" s="623"/>
+      <c r="N1" s="623"/>
     </row>
     <row r="2" spans="1:15" ht="26.25">
-      <c r="A2" s="595" t="s">
+      <c r="A2" s="623" t="s">
         <v>651</v>
       </c>
-      <c r="B2" s="595"/>
-      <c r="C2" s="595"/>
-      <c r="D2" s="595"/>
-      <c r="E2" s="595"/>
-      <c r="F2" s="595"/>
-      <c r="G2" s="595"/>
-      <c r="H2" s="595"/>
-      <c r="I2" s="595"/>
-      <c r="J2" s="595"/>
-      <c r="K2" s="595"/>
-      <c r="L2" s="595"/>
-      <c r="M2" s="595"/>
-      <c r="N2" s="595"/>
+      <c r="B2" s="623"/>
+      <c r="C2" s="623"/>
+      <c r="D2" s="623"/>
+      <c r="E2" s="623"/>
+      <c r="F2" s="623"/>
+      <c r="G2" s="623"/>
+      <c r="H2" s="623"/>
+      <c r="I2" s="623"/>
+      <c r="J2" s="623"/>
+      <c r="K2" s="623"/>
+      <c r="L2" s="623"/>
+      <c r="M2" s="623"/>
+      <c r="N2" s="623"/>
     </row>
     <row r="3" spans="1:15" ht="16.5" customHeight="1">
       <c r="A3" s="471"/>
@@ -16646,43 +16646,43 @@
         <v>408</v>
       </c>
       <c r="B4" s="472"/>
-      <c r="C4" s="596"/>
-      <c r="D4" s="597"/>
-      <c r="E4" s="597"/>
-      <c r="F4" s="597"/>
-      <c r="G4" s="597"/>
-      <c r="H4" s="598"/>
+      <c r="C4" s="617"/>
+      <c r="D4" s="618"/>
+      <c r="E4" s="618"/>
+      <c r="F4" s="618"/>
+      <c r="G4" s="618"/>
+      <c r="H4" s="619"/>
       <c r="I4" s="473"/>
       <c r="J4" s="474" t="s">
         <v>409</v>
       </c>
-      <c r="K4" s="599"/>
-      <c r="L4" s="600"/>
-      <c r="M4" s="600"/>
-      <c r="N4" s="601"/>
+      <c r="K4" s="624"/>
+      <c r="L4" s="625"/>
+      <c r="M4" s="625"/>
+      <c r="N4" s="626"/>
     </row>
     <row r="5" spans="1:15" ht="16.5" customHeight="1">
       <c r="A5" s="472" t="s">
         <v>410</v>
       </c>
       <c r="B5" s="472"/>
-      <c r="C5" s="596"/>
-      <c r="D5" s="597"/>
-      <c r="E5" s="597"/>
-      <c r="F5" s="597"/>
-      <c r="G5" s="597"/>
-      <c r="H5" s="598"/>
+      <c r="C5" s="617"/>
+      <c r="D5" s="618"/>
+      <c r="E5" s="618"/>
+      <c r="F5" s="618"/>
+      <c r="G5" s="618"/>
+      <c r="H5" s="619"/>
       <c r="I5" s="473"/>
       <c r="J5" s="474" t="s">
         <v>411</v>
       </c>
-      <c r="K5" s="599">
+      <c r="K5" s="624">
         <f>Sheet1!P7</f>
         <v>0</v>
       </c>
-      <c r="L5" s="600"/>
-      <c r="M5" s="600"/>
-      <c r="N5" s="601"/>
+      <c r="L5" s="625"/>
+      <c r="M5" s="625"/>
+      <c r="N5" s="626"/>
     </row>
     <row r="6" spans="1:15" ht="16.5" customHeight="1">
       <c r="A6" s="472" t="s">
@@ -16690,21 +16690,21 @@
       </c>
       <c r="B6" s="472"/>
       <c r="C6" s="472"/>
-      <c r="D6" s="596" t="s">
+      <c r="D6" s="617" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="597"/>
-      <c r="F6" s="597"/>
-      <c r="G6" s="597"/>
-      <c r="H6" s="598"/>
+      <c r="E6" s="618"/>
+      <c r="F6" s="618"/>
+      <c r="G6" s="618"/>
+      <c r="H6" s="619"/>
       <c r="I6" s="473"/>
       <c r="J6" s="474" t="s">
         <v>413</v>
       </c>
-      <c r="K6" s="596"/>
-      <c r="L6" s="597"/>
-      <c r="M6" s="597"/>
-      <c r="N6" s="598"/>
+      <c r="K6" s="617"/>
+      <c r="L6" s="618"/>
+      <c r="M6" s="618"/>
+      <c r="N6" s="619"/>
     </row>
     <row r="7" spans="1:15" ht="16.5" customHeight="1">
       <c r="A7" s="472" t="s">
@@ -16712,21 +16712,21 @@
       </c>
       <c r="B7" s="472"/>
       <c r="C7" s="472"/>
-      <c r="D7" s="596" t="s">
+      <c r="D7" s="617" t="s">
         <v>415</v>
       </c>
-      <c r="E7" s="597"/>
-      <c r="F7" s="597"/>
-      <c r="G7" s="597"/>
-      <c r="H7" s="598"/>
+      <c r="E7" s="618"/>
+      <c r="F7" s="618"/>
+      <c r="G7" s="618"/>
+      <c r="H7" s="619"/>
       <c r="I7" s="473"/>
       <c r="J7" s="474" t="s">
         <v>416</v>
       </c>
-      <c r="K7" s="596"/>
-      <c r="L7" s="597"/>
-      <c r="M7" s="597"/>
-      <c r="N7" s="598"/>
+      <c r="K7" s="617"/>
+      <c r="L7" s="618"/>
+      <c r="M7" s="618"/>
+      <c r="N7" s="619"/>
     </row>
     <row r="8" spans="1:15" ht="16.5" customHeight="1">
       <c r="A8" s="472" t="s">
@@ -16734,22 +16734,22 @@
       </c>
       <c r="B8" s="472"/>
       <c r="C8" s="472"/>
-      <c r="D8" s="602" t="str">
+      <c r="D8" s="620" t="str">
         <f>Sheet1!K16</f>
         <v/>
       </c>
-      <c r="E8" s="603"/>
-      <c r="F8" s="603"/>
-      <c r="G8" s="603"/>
-      <c r="H8" s="604"/>
+      <c r="E8" s="621"/>
+      <c r="F8" s="621"/>
+      <c r="G8" s="621"/>
+      <c r="H8" s="622"/>
       <c r="I8" s="473"/>
       <c r="J8" s="474" t="s">
         <v>418</v>
       </c>
-      <c r="K8" s="596"/>
-      <c r="L8" s="597"/>
-      <c r="M8" s="597"/>
-      <c r="N8" s="598"/>
+      <c r="K8" s="617"/>
+      <c r="L8" s="618"/>
+      <c r="M8" s="618"/>
+      <c r="N8" s="619"/>
     </row>
     <row r="9" spans="1:15" ht="11.25" customHeight="1">
       <c r="A9" s="475"/>
@@ -16763,11 +16763,11 @@
       <c r="A10" s="475" t="s">
         <v>652</v>
       </c>
-      <c r="D10" s="606"/>
-      <c r="E10" s="607"/>
-      <c r="F10" s="607"/>
-      <c r="G10" s="607"/>
-      <c r="H10" s="608"/>
+      <c r="D10" s="604"/>
+      <c r="E10" s="605"/>
+      <c r="F10" s="605"/>
+      <c r="G10" s="605"/>
+      <c r="H10" s="606"/>
       <c r="I10" s="477" t="s">
         <v>653</v>
       </c>
@@ -16793,25 +16793,25 @@
       </c>
       <c r="B12" s="472"/>
       <c r="C12" s="472"/>
-      <c r="D12" s="609" t="s">
+      <c r="D12" s="607" t="s">
         <v>421</v>
       </c>
-      <c r="E12" s="609"/>
-      <c r="F12" s="609"/>
-      <c r="G12" s="609" t="s">
+      <c r="E12" s="607"/>
+      <c r="F12" s="607"/>
+      <c r="G12" s="607" t="s">
         <v>416</v>
       </c>
-      <c r="H12" s="609"/>
-      <c r="I12" s="609" t="s">
+      <c r="H12" s="607"/>
+      <c r="I12" s="607" t="s">
         <v>8</v>
       </c>
-      <c r="J12" s="609"/>
-      <c r="K12" s="609" t="s">
+      <c r="J12" s="607"/>
+      <c r="K12" s="607" t="s">
         <v>419</v>
       </c>
-      <c r="L12" s="609"/>
-      <c r="M12" s="609"/>
-      <c r="N12" s="609"/>
+      <c r="L12" s="607"/>
+      <c r="M12" s="607"/>
+      <c r="N12" s="607"/>
     </row>
     <row r="13" spans="1:15" ht="16.5" customHeight="1" thickTop="1">
       <c r="A13" s="472"/>
@@ -16819,63 +16819,63 @@
       <c r="C13" s="479" t="s">
         <v>422</v>
       </c>
-      <c r="D13" s="610" t="s">
+      <c r="D13" s="608" t="s">
         <v>689</v>
       </c>
-      <c r="E13" s="611"/>
-      <c r="F13" s="612"/>
-      <c r="G13" s="610" t="s">
+      <c r="E13" s="609"/>
+      <c r="F13" s="610"/>
+      <c r="G13" s="608" t="s">
         <v>690</v>
       </c>
-      <c r="H13" s="612"/>
-      <c r="I13" s="613"/>
-      <c r="J13" s="614"/>
-      <c r="K13" s="610" t="s">
+      <c r="H13" s="610"/>
+      <c r="I13" s="611"/>
+      <c r="J13" s="612"/>
+      <c r="K13" s="608" t="s">
         <v>691</v>
       </c>
-      <c r="L13" s="611"/>
-      <c r="M13" s="611"/>
-      <c r="N13" s="612"/>
+      <c r="L13" s="609"/>
+      <c r="M13" s="609"/>
+      <c r="N13" s="610"/>
     </row>
     <row r="14" spans="1:15" ht="16.5" customHeight="1">
       <c r="C14" s="479" t="s">
         <v>423</v>
       </c>
-      <c r="D14" s="615" t="s">
+      <c r="D14" s="613" t="s">
         <v>689</v>
       </c>
-      <c r="E14" s="616"/>
-      <c r="F14" s="617"/>
-      <c r="G14" s="615" t="s">
+      <c r="E14" s="614"/>
+      <c r="F14" s="615"/>
+      <c r="G14" s="613" t="s">
         <v>692</v>
       </c>
-      <c r="H14" s="617"/>
-      <c r="I14" s="606"/>
-      <c r="J14" s="608"/>
-      <c r="K14" s="615" t="s">
+      <c r="H14" s="615"/>
+      <c r="I14" s="604"/>
+      <c r="J14" s="606"/>
+      <c r="K14" s="613" t="s">
         <v>693</v>
       </c>
-      <c r="L14" s="616"/>
-      <c r="M14" s="616"/>
-      <c r="N14" s="617"/>
+      <c r="L14" s="614"/>
+      <c r="M14" s="614"/>
+      <c r="N14" s="615"/>
     </row>
     <row r="15" spans="1:15" s="480" customFormat="1" ht="36" customHeight="1">
-      <c r="A15" s="618" t="s">
+      <c r="A15" s="616" t="s">
         <v>654</v>
       </c>
-      <c r="B15" s="618"/>
-      <c r="C15" s="618"/>
-      <c r="D15" s="618"/>
-      <c r="E15" s="618"/>
-      <c r="F15" s="618"/>
-      <c r="G15" s="618"/>
-      <c r="H15" s="618"/>
-      <c r="I15" s="618"/>
-      <c r="J15" s="618"/>
-      <c r="K15" s="618"/>
-      <c r="L15" s="618"/>
-      <c r="M15" s="618"/>
-      <c r="N15" s="618"/>
+      <c r="B15" s="616"/>
+      <c r="C15" s="616"/>
+      <c r="D15" s="616"/>
+      <c r="E15" s="616"/>
+      <c r="F15" s="616"/>
+      <c r="G15" s="616"/>
+      <c r="H15" s="616"/>
+      <c r="I15" s="616"/>
+      <c r="J15" s="616"/>
+      <c r="K15" s="616"/>
+      <c r="L15" s="616"/>
+      <c r="M15" s="616"/>
+      <c r="N15" s="616"/>
     </row>
     <row r="16" spans="1:15" ht="16.5" customHeight="1">
       <c r="A16" s="475" t="s">
@@ -16937,46 +16937,46 @@
       <c r="L18" s="496"/>
     </row>
     <row r="19" spans="1:15" ht="21" customHeight="1">
-      <c r="A19" s="605" t="s">
+      <c r="A19" s="603" t="s">
         <v>426</v>
       </c>
-      <c r="B19" s="605"/>
-      <c r="C19" s="605"/>
-      <c r="D19" s="605"/>
-      <c r="E19" s="605"/>
-      <c r="F19" s="605"/>
-      <c r="G19" s="605"/>
-      <c r="H19" s="605"/>
-      <c r="I19" s="605"/>
-      <c r="J19" s="605"/>
-      <c r="K19" s="605"/>
-      <c r="L19" s="605"/>
-      <c r="M19" s="605"/>
-      <c r="N19" s="605"/>
+      <c r="B19" s="603"/>
+      <c r="C19" s="603"/>
+      <c r="D19" s="603"/>
+      <c r="E19" s="603"/>
+      <c r="F19" s="603"/>
+      <c r="G19" s="603"/>
+      <c r="H19" s="603"/>
+      <c r="I19" s="603"/>
+      <c r="J19" s="603"/>
+      <c r="K19" s="603"/>
+      <c r="L19" s="603"/>
+      <c r="M19" s="603"/>
+      <c r="N19" s="603"/>
     </row>
     <row r="20" spans="1:15" ht="15" customHeight="1">
-      <c r="A20" s="621" t="s">
+      <c r="A20" s="601" t="s">
         <v>427</v>
       </c>
-      <c r="B20" s="621"/>
-      <c r="C20" s="621"/>
-      <c r="D20" s="621"/>
-      <c r="E20" s="621"/>
-      <c r="F20" s="621"/>
-      <c r="G20" s="621"/>
-      <c r="H20" s="621"/>
-      <c r="I20" s="621"/>
-      <c r="J20" s="621"/>
-      <c r="K20" s="621"/>
-      <c r="L20" s="621"/>
-      <c r="M20" s="621"/>
-      <c r="N20" s="621"/>
+      <c r="B20" s="601"/>
+      <c r="C20" s="601"/>
+      <c r="D20" s="601"/>
+      <c r="E20" s="601"/>
+      <c r="F20" s="601"/>
+      <c r="G20" s="601"/>
+      <c r="H20" s="601"/>
+      <c r="I20" s="601"/>
+      <c r="J20" s="601"/>
+      <c r="K20" s="601"/>
+      <c r="L20" s="601"/>
+      <c r="M20" s="601"/>
+      <c r="N20" s="601"/>
     </row>
     <row r="21" spans="1:15" ht="15" customHeight="1">
-      <c r="M21" s="622" t="s">
+      <c r="M21" s="602" t="s">
         <v>428</v>
       </c>
-      <c r="N21" s="622"/>
+      <c r="N21" s="602"/>
     </row>
     <row r="22" spans="1:15" ht="15.75" customHeight="1">
       <c r="A22" s="497" t="s">
@@ -16993,8 +16993,8 @@
       <c r="J22" s="472"/>
       <c r="K22" s="472"/>
       <c r="L22" s="472"/>
-      <c r="M22" s="619"/>
-      <c r="N22" s="620"/>
+      <c r="M22" s="598"/>
+      <c r="N22" s="599"/>
     </row>
     <row r="23" spans="1:15" ht="15.75" customHeight="1">
       <c r="A23" s="497" t="s">
@@ -17011,8 +17011,8 @@
       <c r="J23" s="472"/>
       <c r="K23" s="472"/>
       <c r="L23" s="472"/>
-      <c r="M23" s="619"/>
-      <c r="N23" s="620"/>
+      <c r="M23" s="598"/>
+      <c r="N23" s="599"/>
     </row>
     <row r="24" spans="1:15" ht="15.75" customHeight="1">
       <c r="A24" s="497" t="s">
@@ -17029,8 +17029,8 @@
       <c r="J24" s="473"/>
       <c r="K24" s="473"/>
       <c r="L24" s="473"/>
-      <c r="M24" s="619"/>
-      <c r="N24" s="620"/>
+      <c r="M24" s="598"/>
+      <c r="N24" s="599"/>
     </row>
     <row r="25" spans="1:15" ht="15.75" customHeight="1">
       <c r="A25" s="497" t="s">
@@ -17047,8 +17047,8 @@
       <c r="J25" s="472"/>
       <c r="K25" s="472"/>
       <c r="L25" s="472"/>
-      <c r="M25" s="619"/>
-      <c r="N25" s="620"/>
+      <c r="M25" s="598"/>
+      <c r="N25" s="599"/>
     </row>
     <row r="26" spans="1:15" ht="15.75" customHeight="1">
       <c r="A26" s="497" t="s">
@@ -17065,8 +17065,8 @@
       <c r="J26" s="472"/>
       <c r="K26" s="472"/>
       <c r="L26" s="472"/>
-      <c r="M26" s="619"/>
-      <c r="N26" s="620"/>
+      <c r="M26" s="598"/>
+      <c r="N26" s="599"/>
     </row>
     <row r="27" spans="1:15" ht="15.75" customHeight="1">
       <c r="A27" s="497" t="s">
@@ -17083,8 +17083,8 @@
       <c r="J27" s="472"/>
       <c r="K27" s="472"/>
       <c r="L27" s="472"/>
-      <c r="M27" s="619"/>
-      <c r="N27" s="620"/>
+      <c r="M27" s="598"/>
+      <c r="N27" s="599"/>
     </row>
     <row r="28" spans="1:15" ht="15.75" customHeight="1">
       <c r="A28" s="497" t="s">
@@ -17101,8 +17101,8 @@
       <c r="J28" s="472"/>
       <c r="K28" s="472"/>
       <c r="L28" s="472"/>
-      <c r="M28" s="619"/>
-      <c r="N28" s="620"/>
+      <c r="M28" s="598"/>
+      <c r="N28" s="599"/>
     </row>
     <row r="29" spans="1:15" ht="15.75" customHeight="1">
       <c r="A29" s="497" t="s">
@@ -17134,8 +17134,8 @@
       <c r="L30" s="502" t="s">
         <v>329</v>
       </c>
-      <c r="M30" s="619"/>
-      <c r="N30" s="620"/>
+      <c r="M30" s="598"/>
+      <c r="N30" s="599"/>
     </row>
     <row r="31" spans="1:15" ht="15.75" customHeight="1">
       <c r="A31" s="472"/>
@@ -17157,8 +17157,8 @@
       <c r="L31" s="502" t="s">
         <v>329</v>
       </c>
-      <c r="M31" s="619"/>
-      <c r="N31" s="620"/>
+      <c r="M31" s="598"/>
+      <c r="N31" s="599"/>
     </row>
     <row r="32" spans="1:15" ht="15.75" customHeight="1">
       <c r="A32" s="472" t="s">
@@ -17175,8 +17175,8 @@
       <c r="J32" s="472"/>
       <c r="K32" s="472"/>
       <c r="L32" s="472"/>
-      <c r="M32" s="619"/>
-      <c r="N32" s="620"/>
+      <c r="M32" s="598"/>
+      <c r="N32" s="599"/>
     </row>
     <row r="33" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
       <c r="A33" s="472" t="s">
@@ -17221,8 +17221,8 @@
       </c>
       <c r="K34" s="476"/>
       <c r="L34" s="476"/>
-      <c r="M34" s="619"/>
-      <c r="N34" s="620"/>
+      <c r="M34" s="598"/>
+      <c r="N34" s="599"/>
     </row>
     <row r="35" spans="1:14" ht="15.75" customHeight="1">
       <c r="C35" s="503" t="s">
@@ -17244,8 +17244,8 @@
         <v>0</v>
       </c>
       <c r="L35" s="476"/>
-      <c r="M35" s="619"/>
-      <c r="N35" s="620"/>
+      <c r="M35" s="598"/>
+      <c r="N35" s="599"/>
     </row>
     <row r="36" spans="1:14" ht="15.75" customHeight="1">
       <c r="A36" s="472" t="s">
@@ -17283,8 +17283,8 @@
       <c r="J37" s="508"/>
       <c r="K37" s="514"/>
       <c r="L37" s="514"/>
-      <c r="M37" s="619"/>
-      <c r="N37" s="620"/>
+      <c r="M37" s="598"/>
+      <c r="N37" s="599"/>
     </row>
     <row r="38" spans="1:14" ht="15.75" customHeight="1">
       <c r="A38" s="472"/>
@@ -17324,8 +17324,8 @@
       <c r="J39" s="508"/>
       <c r="K39" s="514"/>
       <c r="L39" s="514"/>
-      <c r="M39" s="619"/>
-      <c r="N39" s="620"/>
+      <c r="M39" s="598"/>
+      <c r="N39" s="599"/>
     </row>
     <row r="40" spans="1:14" ht="15.75" customHeight="1">
       <c r="A40" s="472" t="s">
@@ -17342,8 +17342,8 @@
       <c r="J40" s="472"/>
       <c r="K40" s="472"/>
       <c r="L40" s="472"/>
-      <c r="M40" s="619"/>
-      <c r="N40" s="620"/>
+      <c r="M40" s="598"/>
+      <c r="N40" s="599"/>
     </row>
     <row r="41" spans="1:14" ht="15.75" customHeight="1">
       <c r="A41" s="472" t="s">
@@ -17360,8 +17360,8 @@
       <c r="J41" s="472"/>
       <c r="K41" s="472"/>
       <c r="L41" s="472"/>
-      <c r="M41" s="619"/>
-      <c r="N41" s="620"/>
+      <c r="M41" s="598"/>
+      <c r="N41" s="599"/>
     </row>
     <row r="42" spans="1:14" ht="15.75" customHeight="1">
       <c r="A42" s="472" t="s">
@@ -17378,8 +17378,8 @@
       <c r="J42" s="472"/>
       <c r="K42" s="472"/>
       <c r="L42" s="472"/>
-      <c r="M42" s="619"/>
-      <c r="N42" s="620"/>
+      <c r="M42" s="598"/>
+      <c r="N42" s="599"/>
     </row>
     <row r="43" spans="1:14" ht="15.75" customHeight="1">
       <c r="A43" s="497" t="s">
@@ -17396,8 +17396,8 @@
       <c r="J43" s="497"/>
       <c r="K43" s="497"/>
       <c r="L43" s="472"/>
-      <c r="M43" s="619"/>
-      <c r="N43" s="624"/>
+      <c r="M43" s="598"/>
+      <c r="N43" s="600"/>
     </row>
     <row r="44" spans="1:14" ht="15.75" customHeight="1">
       <c r="A44" s="472" t="s">
@@ -17414,8 +17414,8 @@
       <c r="J44" s="472"/>
       <c r="K44" s="472"/>
       <c r="L44" s="472"/>
-      <c r="M44" s="619"/>
-      <c r="N44" s="620"/>
+      <c r="M44" s="598"/>
+      <c r="N44" s="599"/>
     </row>
     <row r="45" spans="1:14" ht="15.75" customHeight="1">
       <c r="A45" s="472" t="s">
@@ -17432,8 +17432,8 @@
       <c r="J45" s="472"/>
       <c r="K45" s="472"/>
       <c r="L45" s="472"/>
-      <c r="M45" s="619"/>
-      <c r="N45" s="620"/>
+      <c r="M45" s="598"/>
+      <c r="N45" s="599"/>
     </row>
     <row r="46" spans="1:14" ht="15.75" customHeight="1">
       <c r="A46" s="472" t="s">
@@ -17450,8 +17450,8 @@
       <c r="J46" s="472"/>
       <c r="K46" s="472"/>
       <c r="L46" s="472"/>
-      <c r="M46" s="619"/>
-      <c r="N46" s="620"/>
+      <c r="M46" s="598"/>
+      <c r="N46" s="599"/>
     </row>
     <row r="47" spans="1:14" ht="15.75" customHeight="1">
       <c r="A47" s="472"/>
@@ -17470,49 +17470,37 @@
       <c r="N47" s="514"/>
     </row>
     <row r="48" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A48" s="623" t="s">
+      <c r="A48" s="597" t="s">
         <v>676</v>
       </c>
-      <c r="B48" s="623"/>
-      <c r="C48" s="623"/>
-      <c r="D48" s="623"/>
-      <c r="E48" s="623"/>
-      <c r="F48" s="623"/>
-      <c r="G48" s="623"/>
-      <c r="H48" s="623"/>
-      <c r="I48" s="623"/>
-      <c r="J48" s="623"/>
-      <c r="K48" s="623"/>
-      <c r="L48" s="623"/>
-      <c r="M48" s="623"/>
-      <c r="N48" s="623"/>
+      <c r="B48" s="597"/>
+      <c r="C48" s="597"/>
+      <c r="D48" s="597"/>
+      <c r="E48" s="597"/>
+      <c r="F48" s="597"/>
+      <c r="G48" s="597"/>
+      <c r="H48" s="597"/>
+      <c r="I48" s="597"/>
+      <c r="J48" s="597"/>
+      <c r="K48" s="597"/>
+      <c r="L48" s="597"/>
+      <c r="M48" s="597"/>
+      <c r="N48" s="597"/>
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="A48:N48"/>
-    <mergeCell ref="M34:N34"/>
-    <mergeCell ref="M35:N35"/>
-    <mergeCell ref="M37:N37"/>
-    <mergeCell ref="M39:N39"/>
-    <mergeCell ref="M40:N40"/>
-    <mergeCell ref="M41:N41"/>
-    <mergeCell ref="M42:N42"/>
-    <mergeCell ref="M43:N43"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="M45:N45"/>
-    <mergeCell ref="M46:N46"/>
-    <mergeCell ref="M32:N32"/>
-    <mergeCell ref="A20:N20"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="M31:N31"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="A2:N2"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="K4:N4"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="K7:N7"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="K8:N8"/>
     <mergeCell ref="A19:N19"/>
     <mergeCell ref="D10:H10"/>
     <mergeCell ref="D12:F12"/>
@@ -17528,18 +17516,30 @@
     <mergeCell ref="I14:J14"/>
     <mergeCell ref="K14:N14"/>
     <mergeCell ref="A15:N15"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="K6:N6"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="K7:N7"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="K8:N8"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="A2:N2"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="K4:N4"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="M32:N32"/>
+    <mergeCell ref="A20:N20"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="M31:N31"/>
+    <mergeCell ref="A48:N48"/>
+    <mergeCell ref="M34:N34"/>
+    <mergeCell ref="M35:N35"/>
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="M39:N39"/>
+    <mergeCell ref="M40:N40"/>
+    <mergeCell ref="M41:N41"/>
+    <mergeCell ref="M42:N42"/>
+    <mergeCell ref="M43:N43"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="M45:N45"/>
+    <mergeCell ref="M46:N46"/>
   </mergeCells>
   <conditionalFormatting sqref="M22:N28 M32:N32 M37:N37 M39:N40 M42:N42 M44:N45 M43">
     <cfRule type="cellIs" dxfId="93" priority="7" stopIfTrue="1" operator="equal">
@@ -17815,69 +17815,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="27" customHeight="1">
-      <c r="A1" s="628" t="s">
+      <c r="A1" s="637" t="s">
         <v>407</v>
       </c>
-      <c r="B1" s="628"/>
-      <c r="C1" s="628"/>
-      <c r="D1" s="628"/>
-      <c r="E1" s="628"/>
-      <c r="F1" s="628"/>
-      <c r="G1" s="628"/>
-      <c r="H1" s="628"/>
-      <c r="I1" s="628"/>
-      <c r="J1" s="628"/>
-      <c r="K1" s="628"/>
-      <c r="L1" s="628"/>
+      <c r="B1" s="637"/>
+      <c r="C1" s="637"/>
+      <c r="D1" s="637"/>
+      <c r="E1" s="637"/>
+      <c r="F1" s="637"/>
+      <c r="G1" s="637"/>
+      <c r="H1" s="637"/>
+      <c r="I1" s="637"/>
+      <c r="J1" s="637"/>
+      <c r="K1" s="637"/>
+      <c r="L1" s="637"/>
     </row>
     <row r="2" spans="1:12" ht="18" customHeight="1">
-      <c r="A2" s="629" t="s">
+      <c r="A2" s="638" t="s">
         <v>677</v>
       </c>
-      <c r="B2" s="630"/>
-      <c r="C2" s="630"/>
-      <c r="D2" s="630"/>
-      <c r="E2" s="630"/>
-      <c r="F2" s="630"/>
-      <c r="G2" s="630"/>
-      <c r="H2" s="630"/>
-      <c r="I2" s="630"/>
-      <c r="J2" s="630"/>
-      <c r="K2" s="630"/>
-      <c r="L2" s="630"/>
+      <c r="B2" s="639"/>
+      <c r="C2" s="639"/>
+      <c r="D2" s="639"/>
+      <c r="E2" s="639"/>
+      <c r="F2" s="639"/>
+      <c r="G2" s="639"/>
+      <c r="H2" s="639"/>
+      <c r="I2" s="639"/>
+      <c r="J2" s="639"/>
+      <c r="K2" s="639"/>
+      <c r="L2" s="639"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1"/>
     <row r="4" spans="1:12" ht="24" customHeight="1">
-      <c r="A4" s="631" t="s">
+      <c r="A4" s="640" t="s">
         <v>442</v>
       </c>
-      <c r="B4" s="631"/>
-      <c r="C4" s="631"/>
-      <c r="D4" s="631"/>
-      <c r="E4" s="631"/>
-      <c r="F4" s="631"/>
-      <c r="G4" s="631"/>
-      <c r="H4" s="631"/>
-      <c r="I4" s="631"/>
-      <c r="J4" s="631"/>
-      <c r="K4" s="631"/>
-      <c r="L4" s="631"/>
+      <c r="B4" s="640"/>
+      <c r="C4" s="640"/>
+      <c r="D4" s="640"/>
+      <c r="E4" s="640"/>
+      <c r="F4" s="640"/>
+      <c r="G4" s="640"/>
+      <c r="H4" s="640"/>
+      <c r="I4" s="640"/>
+      <c r="J4" s="640"/>
+      <c r="K4" s="640"/>
+      <c r="L4" s="640"/>
     </row>
     <row r="5" spans="1:12" ht="42" customHeight="1">
-      <c r="A5" s="632" t="s">
+      <c r="A5" s="641" t="s">
         <v>678</v>
       </c>
-      <c r="B5" s="632"/>
-      <c r="C5" s="632"/>
-      <c r="D5" s="632"/>
-      <c r="E5" s="632"/>
-      <c r="F5" s="632"/>
-      <c r="G5" s="632"/>
-      <c r="H5" s="632"/>
-      <c r="I5" s="632"/>
-      <c r="J5" s="632"/>
-      <c r="K5" s="632"/>
-      <c r="L5" s="632"/>
+      <c r="B5" s="641"/>
+      <c r="C5" s="641"/>
+      <c r="D5" s="641"/>
+      <c r="E5" s="641"/>
+      <c r="F5" s="641"/>
+      <c r="G5" s="641"/>
+      <c r="H5" s="641"/>
+      <c r="I5" s="641"/>
+      <c r="J5" s="641"/>
+      <c r="K5" s="641"/>
+      <c r="L5" s="641"/>
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1">
       <c r="A6" s="517" t="s">
@@ -17912,9 +17912,9 @@
       <c r="L7" s="524"/>
     </row>
     <row r="8" spans="1:12" ht="15" customHeight="1">
-      <c r="J8" s="633"/>
-      <c r="K8" s="633"/>
-      <c r="L8" s="633"/>
+      <c r="J8" s="642"/>
+      <c r="K8" s="642"/>
+      <c r="L8" s="642"/>
     </row>
     <row r="9" spans="1:12" ht="15" customHeight="1">
       <c r="A9" s="476"/>
@@ -17923,11 +17923,11 @@
         <v>443</v>
       </c>
       <c r="I9" s="493"/>
-      <c r="J9" s="634" t="s">
+      <c r="J9" s="643" t="s">
         <v>428</v>
       </c>
-      <c r="K9" s="634"/>
-      <c r="L9" s="634"/>
+      <c r="K9" s="643"/>
+      <c r="L9" s="643"/>
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1">
       <c r="A10" s="526" t="s">
@@ -17939,9 +17939,9 @@
       <c r="H10" s="528" t="s">
         <v>445</v>
       </c>
-      <c r="J10" s="625"/>
-      <c r="K10" s="626"/>
-      <c r="L10" s="627"/>
+      <c r="J10" s="627"/>
+      <c r="K10" s="628"/>
+      <c r="L10" s="629"/>
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1">
       <c r="A11" s="529" t="s">
@@ -17953,9 +17953,9 @@
       <c r="H11" s="528" t="s">
         <v>445</v>
       </c>
-      <c r="J11" s="625"/>
-      <c r="K11" s="626"/>
-      <c r="L11" s="627"/>
+      <c r="J11" s="627"/>
+      <c r="K11" s="628"/>
+      <c r="L11" s="629"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1">
       <c r="A12" s="529" t="s">
@@ -17967,9 +17967,9 @@
       <c r="H12" s="528" t="s">
         <v>445</v>
       </c>
-      <c r="J12" s="625"/>
-      <c r="K12" s="626"/>
-      <c r="L12" s="627"/>
+      <c r="J12" s="627"/>
+      <c r="K12" s="628"/>
+      <c r="L12" s="629"/>
     </row>
     <row r="13" spans="1:12" ht="15.75" customHeight="1">
       <c r="A13" s="529" t="s">
@@ -17981,9 +17981,9 @@
       <c r="H13" s="528" t="s">
         <v>445</v>
       </c>
-      <c r="J13" s="625"/>
-      <c r="K13" s="626"/>
-      <c r="L13" s="627"/>
+      <c r="J13" s="627"/>
+      <c r="K13" s="628"/>
+      <c r="L13" s="629"/>
     </row>
     <row r="14" spans="1:12" ht="15.75" customHeight="1">
       <c r="A14" s="529" t="s">
@@ -17995,9 +17995,9 @@
       <c r="H14" s="528" t="s">
         <v>445</v>
       </c>
-      <c r="J14" s="625"/>
-      <c r="K14" s="626"/>
-      <c r="L14" s="627"/>
+      <c r="J14" s="627"/>
+      <c r="K14" s="628"/>
+      <c r="L14" s="629"/>
     </row>
     <row r="15" spans="1:12" ht="15.75" customHeight="1">
       <c r="A15" s="529" t="s">
@@ -18009,9 +18009,9 @@
       <c r="H15" s="528" t="s">
         <v>445</v>
       </c>
-      <c r="J15" s="625"/>
-      <c r="K15" s="626"/>
-      <c r="L15" s="627"/>
+      <c r="J15" s="627"/>
+      <c r="K15" s="628"/>
+      <c r="L15" s="629"/>
     </row>
     <row r="16" spans="1:12" ht="15.75" customHeight="1">
       <c r="A16" s="529" t="s">
@@ -18023,9 +18023,9 @@
       <c r="H16" s="528" t="s">
         <v>456</v>
       </c>
-      <c r="J16" s="625"/>
-      <c r="K16" s="626"/>
-      <c r="L16" s="627"/>
+      <c r="J16" s="627"/>
+      <c r="K16" s="628"/>
+      <c r="L16" s="629"/>
     </row>
     <row r="17" spans="1:12" ht="15.75" customHeight="1">
       <c r="A17" s="529" t="s">
@@ -18037,9 +18037,9 @@
       <c r="H17" s="528" t="s">
         <v>459</v>
       </c>
-      <c r="J17" s="625"/>
-      <c r="K17" s="626"/>
-      <c r="L17" s="627"/>
+      <c r="J17" s="627"/>
+      <c r="K17" s="628"/>
+      <c r="L17" s="629"/>
     </row>
     <row r="18" spans="1:12" ht="15.75" customHeight="1">
       <c r="A18" s="526" t="s">
@@ -18051,9 +18051,9 @@
       <c r="H18" s="528" t="s">
         <v>462</v>
       </c>
-      <c r="J18" s="625"/>
-      <c r="K18" s="626"/>
-      <c r="L18" s="627"/>
+      <c r="J18" s="627"/>
+      <c r="K18" s="628"/>
+      <c r="L18" s="629"/>
     </row>
     <row r="19" spans="1:12" ht="15.75" customHeight="1">
       <c r="A19" s="526" t="s">
@@ -18065,9 +18065,9 @@
       <c r="H19" s="531" t="s">
         <v>465</v>
       </c>
-      <c r="J19" s="625"/>
-      <c r="K19" s="626"/>
-      <c r="L19" s="627"/>
+      <c r="J19" s="627"/>
+      <c r="K19" s="628"/>
+      <c r="L19" s="629"/>
     </row>
     <row r="20" spans="1:12" ht="15.75" customHeight="1">
       <c r="A20" s="532" t="s">
@@ -18084,9 +18084,9 @@
       <c r="H20" s="533" t="s">
         <v>465</v>
       </c>
-      <c r="J20" s="625"/>
-      <c r="K20" s="626"/>
-      <c r="L20" s="627"/>
+      <c r="J20" s="627"/>
+      <c r="K20" s="628"/>
+      <c r="L20" s="629"/>
     </row>
     <row r="21" spans="1:12" ht="15.75" customHeight="1">
       <c r="A21" s="526" t="s">
@@ -18098,9 +18098,9 @@
       <c r="H21" s="531" t="s">
         <v>684</v>
       </c>
-      <c r="J21" s="625"/>
-      <c r="K21" s="626"/>
-      <c r="L21" s="627"/>
+      <c r="J21" s="627"/>
+      <c r="K21" s="628"/>
+      <c r="L21" s="629"/>
     </row>
     <row r="22" spans="1:12" ht="15.75" customHeight="1">
       <c r="A22" s="526" t="s">
@@ -18112,58 +18112,58 @@
       <c r="H22" s="528" t="s">
         <v>687</v>
       </c>
-      <c r="J22" s="625"/>
-      <c r="K22" s="626"/>
-      <c r="L22" s="627"/>
+      <c r="J22" s="627"/>
+      <c r="K22" s="628"/>
+      <c r="L22" s="629"/>
     </row>
     <row r="23" spans="1:12" ht="15.75" customHeight="1"/>
     <row r="24" spans="1:12" ht="24" customHeight="1">
-      <c r="A24" s="635" t="s">
+      <c r="A24" s="630" t="s">
         <v>468</v>
       </c>
-      <c r="B24" s="635"/>
-      <c r="C24" s="635"/>
-      <c r="D24" s="635"/>
-      <c r="E24" s="635"/>
-      <c r="F24" s="635"/>
-      <c r="G24" s="635"/>
-      <c r="H24" s="635"/>
-      <c r="I24" s="635"/>
-      <c r="J24" s="635"/>
-      <c r="K24" s="635"/>
-      <c r="L24" s="635"/>
+      <c r="B24" s="630"/>
+      <c r="C24" s="630"/>
+      <c r="D24" s="630"/>
+      <c r="E24" s="630"/>
+      <c r="F24" s="630"/>
+      <c r="G24" s="630"/>
+      <c r="H24" s="630"/>
+      <c r="I24" s="630"/>
+      <c r="J24" s="630"/>
+      <c r="K24" s="630"/>
+      <c r="L24" s="630"/>
     </row>
     <row r="25" spans="1:12" ht="15" customHeight="1"/>
     <row r="26" spans="1:12" ht="241.5" customHeight="1">
-      <c r="A26" s="636"/>
-      <c r="B26" s="637"/>
-      <c r="C26" s="637"/>
-      <c r="D26" s="637"/>
-      <c r="E26" s="637"/>
-      <c r="F26" s="637"/>
-      <c r="G26" s="637"/>
-      <c r="H26" s="637"/>
-      <c r="I26" s="637"/>
-      <c r="J26" s="637"/>
-      <c r="K26" s="637"/>
-      <c r="L26" s="638"/>
+      <c r="A26" s="631"/>
+      <c r="B26" s="632"/>
+      <c r="C26" s="632"/>
+      <c r="D26" s="632"/>
+      <c r="E26" s="632"/>
+      <c r="F26" s="632"/>
+      <c r="G26" s="632"/>
+      <c r="H26" s="632"/>
+      <c r="I26" s="632"/>
+      <c r="J26" s="632"/>
+      <c r="K26" s="632"/>
+      <c r="L26" s="633"/>
     </row>
     <row r="27" spans="1:12" ht="15" customHeight="1" thickBot="1"/>
     <row r="28" spans="1:12" ht="204.75" customHeight="1" thickBot="1">
-      <c r="A28" s="639" t="s">
+      <c r="A28" s="634" t="s">
         <v>688</v>
       </c>
-      <c r="B28" s="640"/>
-      <c r="C28" s="640"/>
-      <c r="D28" s="640"/>
-      <c r="E28" s="640"/>
-      <c r="F28" s="640"/>
-      <c r="G28" s="640"/>
-      <c r="H28" s="640"/>
-      <c r="I28" s="640"/>
-      <c r="J28" s="640"/>
-      <c r="K28" s="640"/>
-      <c r="L28" s="641"/>
+      <c r="B28" s="635"/>
+      <c r="C28" s="635"/>
+      <c r="D28" s="635"/>
+      <c r="E28" s="635"/>
+      <c r="F28" s="635"/>
+      <c r="G28" s="635"/>
+      <c r="H28" s="635"/>
+      <c r="I28" s="635"/>
+      <c r="J28" s="635"/>
+      <c r="K28" s="635"/>
+      <c r="L28" s="636"/>
     </row>
     <row r="33" spans="2:12" ht="18" customHeight="1">
       <c r="B33" s="472"/>
@@ -18180,16 +18180,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="J22:L22"/>
-    <mergeCell ref="A24:L24"/>
-    <mergeCell ref="A26:L26"/>
-    <mergeCell ref="A28:L28"/>
-    <mergeCell ref="J16:L16"/>
-    <mergeCell ref="J17:L17"/>
-    <mergeCell ref="J18:L18"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="J20:L20"/>
-    <mergeCell ref="J21:L21"/>
     <mergeCell ref="J15:L15"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A2:L2"/>
@@ -18202,6 +18192,16 @@
     <mergeCell ref="J12:L12"/>
     <mergeCell ref="J13:L13"/>
     <mergeCell ref="J14:L14"/>
+    <mergeCell ref="J22:L22"/>
+    <mergeCell ref="A24:L24"/>
+    <mergeCell ref="A26:L26"/>
+    <mergeCell ref="A28:L28"/>
+    <mergeCell ref="J16:L16"/>
+    <mergeCell ref="J17:L17"/>
+    <mergeCell ref="J18:L18"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="J20:L20"/>
+    <mergeCell ref="J21:L21"/>
   </mergeCells>
   <conditionalFormatting sqref="J22:L22 J20 J10:L19">
     <cfRule type="cellIs" dxfId="86" priority="2" stopIfTrue="1" operator="equal">
@@ -18756,13 +18756,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33" customHeight="1">
-      <c r="A1" s="657" t="s">
+      <c r="A1" s="646" t="s">
         <v>469</v>
       </c>
-      <c r="B1" s="658"/>
-      <c r="C1" s="658"/>
-      <c r="D1" s="658"/>
-      <c r="E1" s="658"/>
+      <c r="B1" s="647"/>
+      <c r="C1" s="647"/>
+      <c r="D1" s="647"/>
+      <c r="E1" s="647"/>
     </row>
     <row r="2" spans="1:5" ht="18" customHeight="1">
       <c r="A2" s="534"/>
@@ -18775,23 +18775,23 @@
       <c r="A3" s="535" t="s">
         <v>470</v>
       </c>
-      <c r="B3" s="659">
+      <c r="B3" s="648">
         <f>'QC Test Summary-Hologic'!C4</f>
         <v>0</v>
       </c>
-      <c r="C3" s="659"/>
-      <c r="D3" s="659"/>
-      <c r="E3" s="659"/>
+      <c r="C3" s="648"/>
+      <c r="D3" s="648"/>
+      <c r="E3" s="648"/>
     </row>
     <row r="4" spans="1:5" ht="16.5" customHeight="1">
       <c r="A4" s="535" t="s">
         <v>471</v>
       </c>
-      <c r="B4" s="660" t="str">
+      <c r="B4" s="649" t="str">
         <f>Sheet1!R17</f>
         <v/>
       </c>
-      <c r="C4" s="660"/>
+      <c r="C4" s="649"/>
       <c r="D4" s="536" t="s">
         <v>23</v>
       </c>
@@ -18821,11 +18821,11 @@
       <c r="A6" s="535" t="s">
         <v>474</v>
       </c>
-      <c r="B6" s="660" t="str">
+      <c r="B6" s="649" t="str">
         <f>Sheet1!X7</f>
         <v>Eugene Mah</v>
       </c>
-      <c r="C6" s="660"/>
+      <c r="C6" s="649"/>
       <c r="D6" s="536" t="s">
         <v>475</v>
       </c>
@@ -18838,8 +18838,8 @@
       <c r="A7" s="535" t="s">
         <v>476</v>
       </c>
-      <c r="B7" s="660"/>
-      <c r="C7" s="660"/>
+      <c r="B7" s="649"/>
+      <c r="C7" s="649"/>
       <c r="D7" s="536" t="s">
         <v>477</v>
       </c>
@@ -18867,7 +18867,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="33" customHeight="1" thickTop="1">
-      <c r="A10" s="656" t="s">
+      <c r="A10" s="644" t="s">
         <v>482</v>
       </c>
       <c r="B10" s="543" t="s">
@@ -18882,7 +18882,7 @@
       <c r="E10" s="546"/>
     </row>
     <row r="11" spans="1:5" ht="25.5" customHeight="1" thickBot="1">
-      <c r="A11" s="652"/>
+      <c r="A11" s="645"/>
       <c r="B11" s="547" t="s">
         <v>486</v>
       </c>
@@ -18895,7 +18895,7 @@
       <c r="E11" s="550"/>
     </row>
     <row r="12" spans="1:5" ht="33.75" customHeight="1">
-      <c r="A12" s="647" t="s">
+      <c r="A12" s="655" t="s">
         <v>488</v>
       </c>
       <c r="B12" s="551" t="s">
@@ -18910,7 +18910,7 @@
       <c r="E12" s="554"/>
     </row>
     <row r="13" spans="1:5" ht="33.75" customHeight="1">
-      <c r="A13" s="648"/>
+      <c r="A13" s="656"/>
       <c r="B13" s="555" t="s">
         <v>492</v>
       </c>
@@ -18923,7 +18923,7 @@
       <c r="E13" s="558"/>
     </row>
     <row r="14" spans="1:5" ht="34.5" customHeight="1" thickBot="1">
-      <c r="A14" s="649"/>
+      <c r="A14" s="657"/>
       <c r="B14" s="559" t="s">
         <v>494</v>
       </c>
@@ -18936,7 +18936,7 @@
       <c r="E14" s="561"/>
     </row>
     <row r="15" spans="1:5" ht="56.25">
-      <c r="A15" s="650" t="s">
+      <c r="A15" s="658" t="s">
         <v>496</v>
       </c>
       <c r="B15" s="562" t="s">
@@ -18951,7 +18951,7 @@
       <c r="E15" s="564"/>
     </row>
     <row r="16" spans="1:5" ht="54.75" customHeight="1" thickBot="1">
-      <c r="A16" s="651"/>
+      <c r="A16" s="659"/>
       <c r="B16" s="547" t="s">
         <v>499</v>
       </c>
@@ -18964,7 +18964,7 @@
       <c r="E16" s="566"/>
     </row>
     <row r="17" spans="1:5" ht="33.75" customHeight="1">
-      <c r="A17" s="642" t="s">
+      <c r="A17" s="650" t="s">
         <v>502</v>
       </c>
       <c r="B17" s="567" t="s">
@@ -18979,7 +18979,7 @@
       <c r="E17" s="568"/>
     </row>
     <row r="18" spans="1:5" ht="33.75" customHeight="1" thickBot="1">
-      <c r="A18" s="652"/>
+      <c r="A18" s="645"/>
       <c r="B18" s="569" t="s">
         <v>505</v>
       </c>
@@ -18992,7 +18992,7 @@
       <c r="E18" s="550"/>
     </row>
     <row r="19" spans="1:5" ht="33.75">
-      <c r="A19" s="653" t="s">
+      <c r="A19" s="660" t="s">
         <v>507</v>
       </c>
       <c r="B19" s="567" t="s">
@@ -19007,7 +19007,7 @@
       <c r="E19" s="568"/>
     </row>
     <row r="20" spans="1:5" ht="33.75" customHeight="1">
-      <c r="A20" s="654"/>
+      <c r="A20" s="661"/>
       <c r="B20" s="571" t="s">
         <v>510</v>
       </c>
@@ -19020,7 +19020,7 @@
       <c r="E20" s="573"/>
     </row>
     <row r="21" spans="1:5" ht="54.75" customHeight="1" thickBot="1">
-      <c r="A21" s="655"/>
+      <c r="A21" s="662"/>
       <c r="B21" s="569" t="s">
         <v>512</v>
       </c>
@@ -19033,7 +19033,7 @@
       <c r="E21" s="550"/>
     </row>
     <row r="22" spans="1:5" ht="33.75" customHeight="1">
-      <c r="A22" s="642" t="s">
+      <c r="A22" s="650" t="s">
         <v>514</v>
       </c>
       <c r="B22" s="567" t="s">
@@ -19048,7 +19048,7 @@
       <c r="E22" s="568"/>
     </row>
     <row r="23" spans="1:5" ht="25.5" customHeight="1" thickBot="1">
-      <c r="A23" s="652"/>
+      <c r="A23" s="645"/>
       <c r="B23" s="547" t="s">
         <v>517</v>
       </c>
@@ -19061,7 +19061,7 @@
       <c r="E23" s="566"/>
     </row>
     <row r="24" spans="1:5" ht="33.75">
-      <c r="A24" s="653" t="s">
+      <c r="A24" s="660" t="s">
         <v>519</v>
       </c>
       <c r="B24" s="567" t="s">
@@ -19076,7 +19076,7 @@
       <c r="E24" s="568"/>
     </row>
     <row r="25" spans="1:5" ht="45.75" customHeight="1">
-      <c r="A25" s="654"/>
+      <c r="A25" s="661"/>
       <c r="B25" s="571" t="s">
         <v>522</v>
       </c>
@@ -19089,7 +19089,7 @@
       <c r="E25" s="573"/>
     </row>
     <row r="26" spans="1:5" ht="46.5" customHeight="1">
-      <c r="A26" s="654"/>
+      <c r="A26" s="661"/>
       <c r="B26" s="574" t="s">
         <v>524</v>
       </c>
@@ -19102,7 +19102,7 @@
       <c r="E26" s="573"/>
     </row>
     <row r="27" spans="1:5" ht="22.5">
-      <c r="A27" s="654"/>
+      <c r="A27" s="661"/>
       <c r="B27" s="574" t="s">
         <v>526</v>
       </c>
@@ -19115,7 +19115,7 @@
       <c r="E27" s="573"/>
     </row>
     <row r="28" spans="1:5" ht="23.25" thickBot="1">
-      <c r="A28" s="655"/>
+      <c r="A28" s="662"/>
       <c r="B28" s="575" t="s">
         <v>528</v>
       </c>
@@ -19128,7 +19128,7 @@
       <c r="E28" s="566"/>
     </row>
     <row r="29" spans="1:5" ht="22.5">
-      <c r="A29" s="642" t="s">
+      <c r="A29" s="650" t="s">
         <v>530</v>
       </c>
       <c r="B29" s="576" t="s">
@@ -19143,7 +19143,7 @@
       <c r="E29" s="568"/>
     </row>
     <row r="30" spans="1:5" ht="54.75" customHeight="1">
-      <c r="A30" s="643"/>
+      <c r="A30" s="651"/>
       <c r="B30" s="574" t="s">
         <v>533</v>
       </c>
@@ -19156,7 +19156,7 @@
       <c r="E30" s="573"/>
     </row>
     <row r="31" spans="1:5" ht="34.5" thickBot="1">
-      <c r="A31" s="644"/>
+      <c r="A31" s="652"/>
       <c r="B31" s="575" t="s">
         <v>535</v>
       </c>
@@ -19169,7 +19169,7 @@
       <c r="E31" s="566"/>
     </row>
     <row r="32" spans="1:5" ht="46.5" customHeight="1">
-      <c r="A32" s="642" t="s">
+      <c r="A32" s="650" t="s">
         <v>537</v>
       </c>
       <c r="B32" s="576" t="s">
@@ -19184,7 +19184,7 @@
       <c r="E32" s="568"/>
     </row>
     <row r="33" spans="1:5" ht="66.75" customHeight="1">
-      <c r="A33" s="643"/>
+      <c r="A33" s="651"/>
       <c r="B33" s="574" t="s">
         <v>540</v>
       </c>
@@ -19197,7 +19197,7 @@
       <c r="E33" s="573"/>
     </row>
     <row r="34" spans="1:5" ht="34.5" thickBot="1">
-      <c r="A34" s="644"/>
+      <c r="A34" s="652"/>
       <c r="B34" s="575" t="s">
         <v>541</v>
       </c>
@@ -19285,13 +19285,13 @@
       <c r="E39" s="550"/>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="645" t="s">
+      <c r="A40" s="653" t="s">
         <v>701</v>
       </c>
-      <c r="B40" s="646"/>
-      <c r="C40" s="646"/>
-      <c r="D40" s="646"/>
-      <c r="E40" s="646"/>
+      <c r="B40" s="654"/>
+      <c r="C40" s="654"/>
+      <c r="D40" s="654"/>
+      <c r="E40" s="654"/>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="585"/>
@@ -19988,12 +19988,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
     <mergeCell ref="A29:A31"/>
     <mergeCell ref="A32:A34"/>
     <mergeCell ref="A40:E40"/>
@@ -20003,6 +19997,12 @@
     <mergeCell ref="A19:A21"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="A24:A28"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation showInputMessage="1" showErrorMessage="1" sqref="E10 JA10 SW10 ACS10 AMO10 AWK10 BGG10 BQC10 BZY10 CJU10 CTQ10 DDM10 DNI10 DXE10 EHA10 EQW10 FAS10 FKO10 FUK10 GEG10 GOC10 GXY10 HHU10 HRQ10 IBM10 ILI10 IVE10 JFA10 JOW10 JYS10 KIO10 KSK10 LCG10 LMC10 LVY10 MFU10 MPQ10 MZM10 NJI10 NTE10 ODA10 OMW10 OWS10 PGO10 PQK10 QAG10 QKC10 QTY10 RDU10 RNQ10 RXM10 SHI10 SRE10 TBA10 TKW10 TUS10 UEO10 UOK10 UYG10 VIC10 VRY10 WBU10 WLQ10 WVM10 E65546 JA65546 SW65546 ACS65546 AMO65546 AWK65546 BGG65546 BQC65546 BZY65546 CJU65546 CTQ65546 DDM65546 DNI65546 DXE65546 EHA65546 EQW65546 FAS65546 FKO65546 FUK65546 GEG65546 GOC65546 GXY65546 HHU65546 HRQ65546 IBM65546 ILI65546 IVE65546 JFA65546 JOW65546 JYS65546 KIO65546 KSK65546 LCG65546 LMC65546 LVY65546 MFU65546 MPQ65546 MZM65546 NJI65546 NTE65546 ODA65546 OMW65546 OWS65546 PGO65546 PQK65546 QAG65546 QKC65546 QTY65546 RDU65546 RNQ65546 RXM65546 SHI65546 SRE65546 TBA65546 TKW65546 TUS65546 UEO65546 UOK65546 UYG65546 VIC65546 VRY65546 WBU65546 WLQ65546 WVM65546 E131082 JA131082 SW131082 ACS131082 AMO131082 AWK131082 BGG131082 BQC131082 BZY131082 CJU131082 CTQ131082 DDM131082 DNI131082 DXE131082 EHA131082 EQW131082 FAS131082 FKO131082 FUK131082 GEG131082 GOC131082 GXY131082 HHU131082 HRQ131082 IBM131082 ILI131082 IVE131082 JFA131082 JOW131082 JYS131082 KIO131082 KSK131082 LCG131082 LMC131082 LVY131082 MFU131082 MPQ131082 MZM131082 NJI131082 NTE131082 ODA131082 OMW131082 OWS131082 PGO131082 PQK131082 QAG131082 QKC131082 QTY131082 RDU131082 RNQ131082 RXM131082 SHI131082 SRE131082 TBA131082 TKW131082 TUS131082 UEO131082 UOK131082 UYG131082 VIC131082 VRY131082 WBU131082 WLQ131082 WVM131082 E196618 JA196618 SW196618 ACS196618 AMO196618 AWK196618 BGG196618 BQC196618 BZY196618 CJU196618 CTQ196618 DDM196618 DNI196618 DXE196618 EHA196618 EQW196618 FAS196618 FKO196618 FUK196618 GEG196618 GOC196618 GXY196618 HHU196618 HRQ196618 IBM196618 ILI196618 IVE196618 JFA196618 JOW196618 JYS196618 KIO196618 KSK196618 LCG196618 LMC196618 LVY196618 MFU196618 MPQ196618 MZM196618 NJI196618 NTE196618 ODA196618 OMW196618 OWS196618 PGO196618 PQK196618 QAG196618 QKC196618 QTY196618 RDU196618 RNQ196618 RXM196618 SHI196618 SRE196618 TBA196618 TKW196618 TUS196618 UEO196618 UOK196618 UYG196618 VIC196618 VRY196618 WBU196618 WLQ196618 WVM196618 E262154 JA262154 SW262154 ACS262154 AMO262154 AWK262154 BGG262154 BQC262154 BZY262154 CJU262154 CTQ262154 DDM262154 DNI262154 DXE262154 EHA262154 EQW262154 FAS262154 FKO262154 FUK262154 GEG262154 GOC262154 GXY262154 HHU262154 HRQ262154 IBM262154 ILI262154 IVE262154 JFA262154 JOW262154 JYS262154 KIO262154 KSK262154 LCG262154 LMC262154 LVY262154 MFU262154 MPQ262154 MZM262154 NJI262154 NTE262154 ODA262154 OMW262154 OWS262154 PGO262154 PQK262154 QAG262154 QKC262154 QTY262154 RDU262154 RNQ262154 RXM262154 SHI262154 SRE262154 TBA262154 TKW262154 TUS262154 UEO262154 UOK262154 UYG262154 VIC262154 VRY262154 WBU262154 WLQ262154 WVM262154 E327690 JA327690 SW327690 ACS327690 AMO327690 AWK327690 BGG327690 BQC327690 BZY327690 CJU327690 CTQ327690 DDM327690 DNI327690 DXE327690 EHA327690 EQW327690 FAS327690 FKO327690 FUK327690 GEG327690 GOC327690 GXY327690 HHU327690 HRQ327690 IBM327690 ILI327690 IVE327690 JFA327690 JOW327690 JYS327690 KIO327690 KSK327690 LCG327690 LMC327690 LVY327690 MFU327690 MPQ327690 MZM327690 NJI327690 NTE327690 ODA327690 OMW327690 OWS327690 PGO327690 PQK327690 QAG327690 QKC327690 QTY327690 RDU327690 RNQ327690 RXM327690 SHI327690 SRE327690 TBA327690 TKW327690 TUS327690 UEO327690 UOK327690 UYG327690 VIC327690 VRY327690 WBU327690 WLQ327690 WVM327690 E393226 JA393226 SW393226 ACS393226 AMO393226 AWK393226 BGG393226 BQC393226 BZY393226 CJU393226 CTQ393226 DDM393226 DNI393226 DXE393226 EHA393226 EQW393226 FAS393226 FKO393226 FUK393226 GEG393226 GOC393226 GXY393226 HHU393226 HRQ393226 IBM393226 ILI393226 IVE393226 JFA393226 JOW393226 JYS393226 KIO393226 KSK393226 LCG393226 LMC393226 LVY393226 MFU393226 MPQ393226 MZM393226 NJI393226 NTE393226 ODA393226 OMW393226 OWS393226 PGO393226 PQK393226 QAG393226 QKC393226 QTY393226 RDU393226 RNQ393226 RXM393226 SHI393226 SRE393226 TBA393226 TKW393226 TUS393226 UEO393226 UOK393226 UYG393226 VIC393226 VRY393226 WBU393226 WLQ393226 WVM393226 E458762 JA458762 SW458762 ACS458762 AMO458762 AWK458762 BGG458762 BQC458762 BZY458762 CJU458762 CTQ458762 DDM458762 DNI458762 DXE458762 EHA458762 EQW458762 FAS458762 FKO458762 FUK458762 GEG458762 GOC458762 GXY458762 HHU458762 HRQ458762 IBM458762 ILI458762 IVE458762 JFA458762 JOW458762 JYS458762 KIO458762 KSK458762 LCG458762 LMC458762 LVY458762 MFU458762 MPQ458762 MZM458762 NJI458762 NTE458762 ODA458762 OMW458762 OWS458762 PGO458762 PQK458762 QAG458762 QKC458762 QTY458762 RDU458762 RNQ458762 RXM458762 SHI458762 SRE458762 TBA458762 TKW458762 TUS458762 UEO458762 UOK458762 UYG458762 VIC458762 VRY458762 WBU458762 WLQ458762 WVM458762 E524298 JA524298 SW524298 ACS524298 AMO524298 AWK524298 BGG524298 BQC524298 BZY524298 CJU524298 CTQ524298 DDM524298 DNI524298 DXE524298 EHA524298 EQW524298 FAS524298 FKO524298 FUK524298 GEG524298 GOC524298 GXY524298 HHU524298 HRQ524298 IBM524298 ILI524298 IVE524298 JFA524298 JOW524298 JYS524298 KIO524298 KSK524298 LCG524298 LMC524298 LVY524298 MFU524298 MPQ524298 MZM524298 NJI524298 NTE524298 ODA524298 OMW524298 OWS524298 PGO524298 PQK524298 QAG524298 QKC524298 QTY524298 RDU524298 RNQ524298 RXM524298 SHI524298 SRE524298 TBA524298 TKW524298 TUS524298 UEO524298 UOK524298 UYG524298 VIC524298 VRY524298 WBU524298 WLQ524298 WVM524298 E589834 JA589834 SW589834 ACS589834 AMO589834 AWK589834 BGG589834 BQC589834 BZY589834 CJU589834 CTQ589834 DDM589834 DNI589834 DXE589834 EHA589834 EQW589834 FAS589834 FKO589834 FUK589834 GEG589834 GOC589834 GXY589834 HHU589834 HRQ589834 IBM589834 ILI589834 IVE589834 JFA589834 JOW589834 JYS589834 KIO589834 KSK589834 LCG589834 LMC589834 LVY589834 MFU589834 MPQ589834 MZM589834 NJI589834 NTE589834 ODA589834 OMW589834 OWS589834 PGO589834 PQK589834 QAG589834 QKC589834 QTY589834 RDU589834 RNQ589834 RXM589834 SHI589834 SRE589834 TBA589834 TKW589834 TUS589834 UEO589834 UOK589834 UYG589834 VIC589834 VRY589834 WBU589834 WLQ589834 WVM589834 E655370 JA655370 SW655370 ACS655370 AMO655370 AWK655370 BGG655370 BQC655370 BZY655370 CJU655370 CTQ655370 DDM655370 DNI655370 DXE655370 EHA655370 EQW655370 FAS655370 FKO655370 FUK655370 GEG655370 GOC655370 GXY655370 HHU655370 HRQ655370 IBM655370 ILI655370 IVE655370 JFA655370 JOW655370 JYS655370 KIO655370 KSK655370 LCG655370 LMC655370 LVY655370 MFU655370 MPQ655370 MZM655370 NJI655370 NTE655370 ODA655370 OMW655370 OWS655370 PGO655370 PQK655370 QAG655370 QKC655370 QTY655370 RDU655370 RNQ655370 RXM655370 SHI655370 SRE655370 TBA655370 TKW655370 TUS655370 UEO655370 UOK655370 UYG655370 VIC655370 VRY655370 WBU655370 WLQ655370 WVM655370 E720906 JA720906 SW720906 ACS720906 AMO720906 AWK720906 BGG720906 BQC720906 BZY720906 CJU720906 CTQ720906 DDM720906 DNI720906 DXE720906 EHA720906 EQW720906 FAS720906 FKO720906 FUK720906 GEG720906 GOC720906 GXY720906 HHU720906 HRQ720906 IBM720906 ILI720906 IVE720906 JFA720906 JOW720906 JYS720906 KIO720906 KSK720906 LCG720906 LMC720906 LVY720906 MFU720906 MPQ720906 MZM720906 NJI720906 NTE720906 ODA720906 OMW720906 OWS720906 PGO720906 PQK720906 QAG720906 QKC720906 QTY720906 RDU720906 RNQ720906 RXM720906 SHI720906 SRE720906 TBA720906 TKW720906 TUS720906 UEO720906 UOK720906 UYG720906 VIC720906 VRY720906 WBU720906 WLQ720906 WVM720906 E786442 JA786442 SW786442 ACS786442 AMO786442 AWK786442 BGG786442 BQC786442 BZY786442 CJU786442 CTQ786442 DDM786442 DNI786442 DXE786442 EHA786442 EQW786442 FAS786442 FKO786442 FUK786442 GEG786442 GOC786442 GXY786442 HHU786442 HRQ786442 IBM786442 ILI786442 IVE786442 JFA786442 JOW786442 JYS786442 KIO786442 KSK786442 LCG786442 LMC786442 LVY786442 MFU786442 MPQ786442 MZM786442 NJI786442 NTE786442 ODA786442 OMW786442 OWS786442 PGO786442 PQK786442 QAG786442 QKC786442 QTY786442 RDU786442 RNQ786442 RXM786442 SHI786442 SRE786442 TBA786442 TKW786442 TUS786442 UEO786442 UOK786442 UYG786442 VIC786442 VRY786442 WBU786442 WLQ786442 WVM786442 E851978 JA851978 SW851978 ACS851978 AMO851978 AWK851978 BGG851978 BQC851978 BZY851978 CJU851978 CTQ851978 DDM851978 DNI851978 DXE851978 EHA851978 EQW851978 FAS851978 FKO851978 FUK851978 GEG851978 GOC851978 GXY851978 HHU851978 HRQ851978 IBM851978 ILI851978 IVE851978 JFA851978 JOW851978 JYS851978 KIO851978 KSK851978 LCG851978 LMC851978 LVY851978 MFU851978 MPQ851978 MZM851978 NJI851978 NTE851978 ODA851978 OMW851978 OWS851978 PGO851978 PQK851978 QAG851978 QKC851978 QTY851978 RDU851978 RNQ851978 RXM851978 SHI851978 SRE851978 TBA851978 TKW851978 TUS851978 UEO851978 UOK851978 UYG851978 VIC851978 VRY851978 WBU851978 WLQ851978 WVM851978 E917514 JA917514 SW917514 ACS917514 AMO917514 AWK917514 BGG917514 BQC917514 BZY917514 CJU917514 CTQ917514 DDM917514 DNI917514 DXE917514 EHA917514 EQW917514 FAS917514 FKO917514 FUK917514 GEG917514 GOC917514 GXY917514 HHU917514 HRQ917514 IBM917514 ILI917514 IVE917514 JFA917514 JOW917514 JYS917514 KIO917514 KSK917514 LCG917514 LMC917514 LVY917514 MFU917514 MPQ917514 MZM917514 NJI917514 NTE917514 ODA917514 OMW917514 OWS917514 PGO917514 PQK917514 QAG917514 QKC917514 QTY917514 RDU917514 RNQ917514 RXM917514 SHI917514 SRE917514 TBA917514 TKW917514 TUS917514 UEO917514 UOK917514 UYG917514 VIC917514 VRY917514 WBU917514 WLQ917514 WVM917514 E983050 JA983050 SW983050 ACS983050 AMO983050 AWK983050 BGG983050 BQC983050 BZY983050 CJU983050 CTQ983050 DDM983050 DNI983050 DXE983050 EHA983050 EQW983050 FAS983050 FKO983050 FUK983050 GEG983050 GOC983050 GXY983050 HHU983050 HRQ983050 IBM983050 ILI983050 IVE983050 JFA983050 JOW983050 JYS983050 KIO983050 KSK983050 LCG983050 LMC983050 LVY983050 MFU983050 MPQ983050 MZM983050 NJI983050 NTE983050 ODA983050 OMW983050 OWS983050 PGO983050 PQK983050 QAG983050 QKC983050 QTY983050 RDU983050 RNQ983050 RXM983050 SHI983050 SRE983050 TBA983050 TKW983050 TUS983050 UEO983050 UOK983050 UYG983050 VIC983050 VRY983050 WBU983050 WLQ983050 WVM983050"/>
@@ -22447,21 +22447,21 @@
       <c r="E10" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="661" t="str">
+      <c r="F10" s="686" t="str">
         <f>IF(R10="","",R10)</f>
         <v/>
       </c>
-      <c r="G10" s="661"/>
+      <c r="G10" s="686"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="K10" s="661" t="str">
+      <c r="K10" s="686" t="str">
         <f>IF(V10="","",V10)</f>
         <v/>
       </c>
-      <c r="L10" s="661"/>
+      <c r="L10" s="686"/>
       <c r="M10" s="42"/>
       <c r="N10" s="5"/>
       <c r="O10" s="13"/>
@@ -22531,21 +22531,21 @@
       <c r="E11" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="662" t="str">
+      <c r="F11" s="688" t="str">
         <f>IF(R11="","",R11)</f>
         <v/>
       </c>
-      <c r="G11" s="662"/>
+      <c r="G11" s="688"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="K11" s="661" t="str">
+      <c r="K11" s="686" t="str">
         <f>IF(V11="","",V11)</f>
         <v/>
       </c>
-      <c r="L11" s="661"/>
+      <c r="L11" s="686"/>
       <c r="M11" s="42"/>
       <c r="N11" s="5"/>
       <c r="O11" s="13"/>
@@ -22615,21 +22615,21 @@
       <c r="E12" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="662" t="str">
+      <c r="F12" s="688" t="str">
         <f>IF(R12="","",R12)</f>
         <v/>
       </c>
-      <c r="G12" s="662"/>
+      <c r="G12" s="688"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="K12" s="663" t="str">
+      <c r="K12" s="687" t="str">
         <f>IF(V12="","",V12)</f>
         <v/>
       </c>
-      <c r="L12" s="663"/>
+      <c r="L12" s="687"/>
       <c r="M12" s="42"/>
       <c r="N12" s="5"/>
       <c r="O12" s="13"/>
@@ -22699,21 +22699,21 @@
       <c r="E13" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="662" t="str">
+      <c r="F13" s="688" t="str">
         <f>IF(R13="","",R13)</f>
         <v/>
       </c>
-      <c r="G13" s="662"/>
+      <c r="G13" s="688"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="K13" s="661" t="str">
+      <c r="K13" s="686" t="str">
         <f>IF(V13="","",V13)</f>
         <v/>
       </c>
-      <c r="L13" s="661"/>
+      <c r="L13" s="686"/>
       <c r="M13" s="42"/>
       <c r="N13" s="5"/>
       <c r="O13" s="13"/>
@@ -22923,21 +22923,21 @@
       <c r="E16" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="F16" s="661" t="str">
+      <c r="F16" s="686" t="str">
         <f>IF(R17="","",R17)</f>
         <v/>
       </c>
-      <c r="G16" s="661"/>
+      <c r="G16" s="686"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="K16" s="663" t="str">
+      <c r="K16" s="687" t="str">
         <f>IF(V17="","",V17)</f>
         <v/>
       </c>
-      <c r="L16" s="663"/>
+      <c r="L16" s="687"/>
       <c r="M16" s="42"/>
       <c r="N16" s="5"/>
       <c r="O16" s="13"/>
@@ -22999,21 +22999,21 @@
       <c r="E17" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="F17" s="661" t="str">
+      <c r="F17" s="686" t="str">
         <f>IF(R18="","",R18)</f>
         <v/>
       </c>
-      <c r="G17" s="661"/>
+      <c r="G17" s="686"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="K17" s="661" t="str">
+      <c r="K17" s="686" t="str">
         <f>IF(V18="","",V18)</f>
         <v/>
       </c>
-      <c r="L17" s="661"/>
+      <c r="L17" s="686"/>
       <c r="M17" s="42"/>
       <c r="N17" s="5"/>
       <c r="O17" s="13"/>
@@ -23083,21 +23083,21 @@
       <c r="E18" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="F18" s="661" t="str">
+      <c r="F18" s="686" t="str">
         <f>IF(R19="","",R19)</f>
         <v/>
       </c>
-      <c r="G18" s="661"/>
+      <c r="G18" s="686"/>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="K18" s="661" t="str">
+      <c r="K18" s="686" t="str">
         <f>IF(V19="","",V19)</f>
         <v/>
       </c>
-      <c r="L18" s="661"/>
+      <c r="L18" s="686"/>
       <c r="M18" s="42"/>
       <c r="N18" s="5"/>
       <c r="O18" s="13"/>
@@ -23301,21 +23301,21 @@
       <c r="E21" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="F21" s="661" t="str">
+      <c r="F21" s="686" t="str">
         <f>IF(R22="","",R22)</f>
         <v/>
       </c>
-      <c r="G21" s="661"/>
+      <c r="G21" s="686"/>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
       <c r="J21" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="K21" s="661" t="str">
+      <c r="K21" s="686" t="str">
         <f>IF(V21="","",V21)</f>
         <v/>
       </c>
-      <c r="L21" s="661"/>
+      <c r="L21" s="686"/>
       <c r="M21" s="42"/>
       <c r="N21" s="5"/>
       <c r="O21" s="13"/>
@@ -23382,19 +23382,19 @@
       <c r="E22" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="F22" s="663" t="str">
+      <c r="F22" s="687" t="str">
         <f>IF(R23="","",R23)</f>
         <v/>
       </c>
-      <c r="G22" s="663"/>
+      <c r="G22" s="687"/>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="41"/>
-      <c r="K22" s="661" t="str">
+      <c r="K22" s="686" t="str">
         <f>IF(V22="","",V22)</f>
         <v/>
       </c>
-      <c r="L22" s="661"/>
+      <c r="L22" s="686"/>
       <c r="M22" s="42"/>
       <c r="N22" s="5"/>
       <c r="O22" s="13"/>
@@ -23469,11 +23469,11 @@
       <c r="J23" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="K23" s="661" t="str">
+      <c r="K23" s="686" t="str">
         <f>IF(V24="","",V24)</f>
         <v/>
       </c>
-      <c r="L23" s="661"/>
+      <c r="L23" s="686"/>
       <c r="M23" s="42"/>
       <c r="N23" s="5"/>
       <c r="O23" s="13"/>
@@ -23538,19 +23538,19 @@
       <c r="E24" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="F24" s="661" t="str">
+      <c r="F24" s="686" t="str">
         <f>IF(R25="","",R25)</f>
         <v/>
       </c>
-      <c r="G24" s="661"/>
+      <c r="G24" s="686"/>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
-      <c r="K24" s="661" t="str">
+      <c r="K24" s="686" t="str">
         <f>IF(V25="","",V25)</f>
         <v/>
       </c>
-      <c r="L24" s="661"/>
+      <c r="L24" s="686"/>
       <c r="M24" s="42"/>
       <c r="N24" s="5"/>
       <c r="O24" s="13"/>
@@ -23617,11 +23617,11 @@
       <c r="E25" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="F25" s="661" t="str">
+      <c r="F25" s="686" t="str">
         <f>IF(R26="","",R26)</f>
         <v/>
       </c>
-      <c r="G25" s="661"/>
+      <c r="G25" s="686"/>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
       <c r="J25" s="47"/>
@@ -23694,11 +23694,11 @@
       <c r="E26" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="F26" s="661" t="str">
+      <c r="F26" s="686" t="str">
         <f>IF(R27="","",R27)</f>
         <v/>
       </c>
-      <c r="G26" s="661"/>
+      <c r="G26" s="686"/>
       <c r="H26" s="5"/>
       <c r="I26" s="45" t="s">
         <v>32</v>
@@ -23780,11 +23780,11 @@
       <c r="J27" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="K27" s="661" t="str">
+      <c r="K27" s="686" t="str">
         <f>IF(V28="","",V28)</f>
         <v/>
       </c>
-      <c r="L27" s="661"/>
+      <c r="L27" s="686"/>
       <c r="M27" s="42"/>
       <c r="N27" s="5"/>
       <c r="O27" s="13"/>
@@ -23845,21 +23845,21 @@
       <c r="E28" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="F28" s="661" t="str">
+      <c r="F28" s="686" t="str">
         <f>IF(R29="","",R29)</f>
         <v/>
       </c>
-      <c r="G28" s="661"/>
+      <c r="G28" s="686"/>
       <c r="H28" s="5"/>
       <c r="I28" s="47"/>
       <c r="J28" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="K28" s="661" t="str">
+      <c r="K28" s="686" t="str">
         <f>IF(V29="","",V29)</f>
         <v/>
       </c>
-      <c r="L28" s="661"/>
+      <c r="L28" s="686"/>
       <c r="M28" s="42"/>
       <c r="N28" s="5"/>
       <c r="O28" s="13"/>
@@ -23926,11 +23926,11 @@
       <c r="E29" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="F29" s="661" t="str">
+      <c r="F29" s="686" t="str">
         <f>IF(R30="","",R30)</f>
         <v/>
       </c>
-      <c r="G29" s="661"/>
+      <c r="G29" s="686"/>
       <c r="H29" s="5"/>
       <c r="I29" s="45" t="s">
         <v>36</v>
@@ -23938,11 +23938,11 @@
       <c r="J29" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="K29" s="661" t="str">
+      <c r="K29" s="686" t="str">
         <f>IF(V32="","",V32)</f>
         <v/>
       </c>
-      <c r="L29" s="661"/>
+      <c r="L29" s="686"/>
       <c r="M29" s="42"/>
       <c r="N29" s="5"/>
       <c r="O29" s="13"/>
@@ -24012,21 +24012,21 @@
       <c r="E30" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="F30" s="661" t="str">
+      <c r="F30" s="686" t="str">
         <f>IF(R31="","",R31)</f>
         <v/>
       </c>
-      <c r="G30" s="661"/>
+      <c r="G30" s="686"/>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
       <c r="J30" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="K30" s="661" t="str">
+      <c r="K30" s="686" t="str">
         <f>IF(V33="","",V33)</f>
         <v/>
       </c>
-      <c r="L30" s="661"/>
+      <c r="L30" s="686"/>
       <c r="M30" s="42"/>
       <c r="N30" s="5"/>
       <c r="O30" s="13"/>
@@ -24309,7 +24309,9 @@
       <c r="L34" s="33"/>
       <c r="M34" s="35"/>
       <c r="N34" s="5"/>
-      <c r="O34" s="51"/>
+      <c r="O34" s="51">
+        <v>1</v>
+      </c>
       <c r="P34" s="5" t="s">
         <v>40</v>
       </c>
@@ -24366,24 +24368,26 @@
       <c r="C35" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="D35" s="664" t="s">
+      <c r="D35" s="683" t="s">
         <v>42</v>
       </c>
-      <c r="E35" s="664"/>
-      <c r="F35" s="664"/>
-      <c r="G35" s="665" t="s">
+      <c r="E35" s="683"/>
+      <c r="F35" s="683"/>
+      <c r="G35" s="684" t="s">
         <v>43</v>
       </c>
-      <c r="H35" s="665"/>
-      <c r="I35" s="665"/>
-      <c r="J35" s="664" t="s">
+      <c r="H35" s="684"/>
+      <c r="I35" s="684"/>
+      <c r="J35" s="683" t="s">
         <v>44</v>
       </c>
-      <c r="K35" s="664"/>
-      <c r="L35" s="664"/>
+      <c r="K35" s="683"/>
+      <c r="L35" s="683"/>
       <c r="M35" s="42"/>
       <c r="N35" s="5"/>
-      <c r="O35" s="53"/>
+      <c r="O35" s="53">
+        <v>2</v>
+      </c>
       <c r="P35" s="21" t="s">
         <v>45</v>
       </c>
@@ -24440,15 +24444,15 @@
       <c r="C36" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="D36" s="664"/>
-      <c r="E36" s="664"/>
-      <c r="F36" s="664"/>
-      <c r="G36" s="665"/>
-      <c r="H36" s="665"/>
-      <c r="I36" s="665"/>
-      <c r="J36" s="664"/>
-      <c r="K36" s="664"/>
-      <c r="L36" s="664"/>
+      <c r="D36" s="683"/>
+      <c r="E36" s="683"/>
+      <c r="F36" s="683"/>
+      <c r="G36" s="684"/>
+      <c r="H36" s="684"/>
+      <c r="I36" s="684"/>
+      <c r="J36" s="683"/>
+      <c r="K36" s="683"/>
+      <c r="L36" s="683"/>
       <c r="M36" s="42"/>
       <c r="N36" s="5"/>
       <c r="O36" s="5"/>
@@ -25113,10 +25117,10 @@
       <c r="I44" s="5"/>
       <c r="J44" s="5"/>
       <c r="K44" s="5"/>
-      <c r="L44" s="666" t="s">
+      <c r="L44" s="685" t="s">
         <v>63</v>
       </c>
-      <c r="M44" s="666"/>
+      <c r="M44" s="685"/>
       <c r="N44" s="5"/>
       <c r="O44" s="13"/>
       <c r="P44" s="5"/>
@@ -28896,21 +28900,21 @@
       <c r="O97" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="P97" s="664" t="s">
+      <c r="P97" s="683" t="s">
         <v>42</v>
       </c>
-      <c r="Q97" s="664"/>
-      <c r="R97" s="664"/>
-      <c r="S97" s="665" t="s">
+      <c r="Q97" s="683"/>
+      <c r="R97" s="683"/>
+      <c r="S97" s="684" t="s">
         <v>43</v>
       </c>
-      <c r="T97" s="665"/>
-      <c r="U97" s="665"/>
-      <c r="V97" s="664" t="s">
+      <c r="T97" s="684"/>
+      <c r="U97" s="684"/>
+      <c r="V97" s="683" t="s">
         <v>44</v>
       </c>
-      <c r="W97" s="664"/>
-      <c r="X97" s="664"/>
+      <c r="W97" s="683"/>
+      <c r="X97" s="683"/>
       <c r="Y97" s="15"/>
       <c r="AA97" s="177"/>
       <c r="AB97" s="177"/>
@@ -28968,15 +28972,15 @@
       <c r="O98" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="P98" s="664"/>
-      <c r="Q98" s="664"/>
-      <c r="R98" s="664"/>
-      <c r="S98" s="665"/>
-      <c r="T98" s="665"/>
-      <c r="U98" s="665"/>
-      <c r="V98" s="664"/>
-      <c r="W98" s="664"/>
-      <c r="X98" s="664"/>
+      <c r="P98" s="683"/>
+      <c r="Q98" s="683"/>
+      <c r="R98" s="683"/>
+      <c r="S98" s="684"/>
+      <c r="T98" s="684"/>
+      <c r="U98" s="684"/>
+      <c r="V98" s="683"/>
+      <c r="W98" s="683"/>
+      <c r="X98" s="683"/>
       <c r="Y98" s="15"/>
       <c r="AA98" s="45" t="s">
         <v>394</v>
@@ -29592,21 +29596,21 @@
       <c r="O105" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="P105" s="664" t="s">
+      <c r="P105" s="683" t="s">
         <v>42</v>
       </c>
-      <c r="Q105" s="664"/>
-      <c r="R105" s="664"/>
-      <c r="S105" s="665" t="s">
+      <c r="Q105" s="683"/>
+      <c r="R105" s="683"/>
+      <c r="S105" s="684" t="s">
         <v>43</v>
       </c>
-      <c r="T105" s="665"/>
-      <c r="U105" s="665"/>
-      <c r="V105" s="664" t="s">
+      <c r="T105" s="684"/>
+      <c r="U105" s="684"/>
+      <c r="V105" s="683" t="s">
         <v>44</v>
       </c>
-      <c r="W105" s="664"/>
-      <c r="X105" s="664"/>
+      <c r="W105" s="683"/>
+      <c r="X105" s="683"/>
       <c r="Y105" s="15"/>
       <c r="AA105" s="41" t="s">
         <v>274</v>
@@ -29664,15 +29668,15 @@
       <c r="O106" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="P106" s="664"/>
-      <c r="Q106" s="664"/>
-      <c r="R106" s="664"/>
-      <c r="S106" s="665"/>
-      <c r="T106" s="665"/>
-      <c r="U106" s="665"/>
-      <c r="V106" s="664"/>
-      <c r="W106" s="664"/>
-      <c r="X106" s="664"/>
+      <c r="P106" s="683"/>
+      <c r="Q106" s="683"/>
+      <c r="R106" s="683"/>
+      <c r="S106" s="684"/>
+      <c r="T106" s="684"/>
+      <c r="U106" s="684"/>
+      <c r="V106" s="683"/>
+      <c r="W106" s="683"/>
+      <c r="X106" s="683"/>
       <c r="Y106" s="15"/>
       <c r="AA106" s="41" t="s">
         <v>277</v>
@@ -32237,17 +32241,17 @@
       <c r="M150" s="42"/>
       <c r="N150" s="5"/>
       <c r="O150" s="13"/>
-      <c r="P150" s="667" t="s">
+      <c r="P150" s="672" t="s">
         <v>187</v>
       </c>
-      <c r="Q150" s="667"/>
-      <c r="R150" s="667"/>
-      <c r="S150" s="667"/>
+      <c r="Q150" s="672"/>
+      <c r="R150" s="672"/>
+      <c r="S150" s="672"/>
       <c r="T150" s="133"/>
-      <c r="U150" s="667" t="s">
+      <c r="U150" s="672" t="s">
         <v>188</v>
       </c>
-      <c r="V150" s="667"/>
+      <c r="V150" s="672"/>
       <c r="W150" s="5"/>
       <c r="X150" s="5"/>
       <c r="Y150" s="15"/>
@@ -32296,10 +32300,10 @@
         <v>192</v>
       </c>
       <c r="T151" s="133"/>
-      <c r="U151" s="668" t="s">
+      <c r="U151" s="681" t="s">
         <v>193</v>
       </c>
-      <c r="V151" s="668"/>
+      <c r="V151" s="681"/>
       <c r="W151" s="5"/>
       <c r="X151" s="5"/>
       <c r="Y151" s="15"/>
@@ -32339,11 +32343,11 @@
       <c r="R152" s="136"/>
       <c r="S152" s="137"/>
       <c r="T152" s="133"/>
-      <c r="U152" s="669" t="str">
+      <c r="U152" s="682" t="str">
         <f>IF(OR(R149=2,R149=3),"NA",IF(OR(P152="",Q152="",R152="",S152=""),"",AVERAGE(P152:S152)))</f>
         <v/>
       </c>
-      <c r="V152" s="669"/>
+      <c r="V152" s="682"/>
       <c r="W152" s="5"/>
       <c r="X152" s="41" t="s">
         <v>180</v>
@@ -32459,7 +32463,7 @@
       </c>
       <c r="P155" s="114">
         <f>IF($O$34=1,70,65)</f>
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="Q155" s="5"/>
       <c r="R155" s="5"/>
@@ -32489,18 +32493,18 @@
       <c r="M156" s="141"/>
       <c r="N156" s="5"/>
       <c r="O156" s="13"/>
-      <c r="P156" s="670" t="s">
+      <c r="P156" s="675" t="s">
         <v>196</v>
       </c>
-      <c r="Q156" s="671" t="s">
+      <c r="Q156" s="679" t="s">
         <v>197</v>
       </c>
-      <c r="R156" s="671"/>
-      <c r="S156" s="671"/>
+      <c r="R156" s="679"/>
+      <c r="S156" s="679"/>
       <c r="T156" s="142" t="s">
         <v>197</v>
       </c>
-      <c r="U156" s="672" t="s">
+      <c r="U156" s="677" t="s">
         <v>198</v>
       </c>
       <c r="V156" s="77"/>
@@ -32528,7 +32532,7 @@
       <c r="M157" s="42"/>
       <c r="N157" s="5"/>
       <c r="O157" s="13"/>
-      <c r="P157" s="670" t="s">
+      <c r="P157" s="675" t="s">
         <v>196</v>
       </c>
       <c r="Q157" s="142" t="s">
@@ -32543,7 +32547,7 @@
       <c r="T157" s="142" t="s">
         <v>202</v>
       </c>
-      <c r="U157" s="672" t="s">
+      <c r="U157" s="677" t="s">
         <v>196</v>
       </c>
       <c r="V157" s="77"/>
@@ -32893,14 +32897,14 @@
       <c r="M164" s="42"/>
       <c r="N164" s="5"/>
       <c r="O164" s="156"/>
-      <c r="P164" s="670" t="s">
+      <c r="P164" s="675" t="s">
         <v>209</v>
       </c>
-      <c r="Q164" s="670"/>
-      <c r="R164" s="670"/>
-      <c r="S164" s="670"/>
-      <c r="T164" s="670"/>
-      <c r="U164" s="670"/>
+      <c r="Q164" s="675"/>
+      <c r="R164" s="675"/>
+      <c r="S164" s="675"/>
+      <c r="T164" s="675"/>
+      <c r="U164" s="675"/>
       <c r="V164" s="77"/>
       <c r="W164" s="77"/>
       <c r="X164" s="77"/>
@@ -32944,18 +32948,18 @@
       <c r="M165" s="42"/>
       <c r="N165" s="5"/>
       <c r="O165" s="156"/>
-      <c r="P165" s="670" t="s">
+      <c r="P165" s="675" t="s">
         <v>196</v>
       </c>
-      <c r="Q165" s="673" t="s">
+      <c r="Q165" s="676" t="s">
         <v>197</v>
       </c>
-      <c r="R165" s="673"/>
-      <c r="S165" s="673"/>
+      <c r="R165" s="676"/>
+      <c r="S165" s="676"/>
       <c r="T165" s="143" t="s">
         <v>197</v>
       </c>
-      <c r="U165" s="672" t="s">
+      <c r="U165" s="677" t="s">
         <v>198</v>
       </c>
       <c r="V165" s="77"/>
@@ -32985,7 +32989,7 @@
       <c r="M166" s="42"/>
       <c r="N166" s="5"/>
       <c r="O166" s="156"/>
-      <c r="P166" s="670" t="s">
+      <c r="P166" s="675" t="s">
         <v>196</v>
       </c>
       <c r="Q166" s="143" t="s">
@@ -33000,7 +33004,7 @@
       <c r="T166" s="143" t="s">
         <v>202</v>
       </c>
-      <c r="U166" s="672" t="s">
+      <c r="U166" s="677" t="s">
         <v>196</v>
       </c>
       <c r="V166" s="77"/>
@@ -33273,17 +33277,17 @@
       </c>
       <c r="B172" s="39"/>
       <c r="C172" s="5"/>
-      <c r="D172" s="667" t="s">
+      <c r="D172" s="672" t="s">
         <v>187</v>
       </c>
-      <c r="E172" s="667"/>
-      <c r="F172" s="667"/>
-      <c r="G172" s="667"/>
+      <c r="E172" s="672"/>
+      <c r="F172" s="672"/>
+      <c r="G172" s="672"/>
       <c r="H172" s="133"/>
-      <c r="I172" s="667" t="s">
+      <c r="I172" s="672" t="s">
         <v>188</v>
       </c>
-      <c r="J172" s="667"/>
+      <c r="J172" s="672"/>
       <c r="K172" s="5"/>
       <c r="L172" s="5"/>
       <c r="M172" s="42"/>
@@ -33339,10 +33343,10 @@
         <v>192</v>
       </c>
       <c r="H173" s="133"/>
-      <c r="I173" s="668" t="s">
+      <c r="I173" s="681" t="s">
         <v>193</v>
       </c>
-      <c r="J173" s="668"/>
+      <c r="J173" s="681"/>
       <c r="K173" s="5"/>
       <c r="L173" s="5"/>
       <c r="M173" s="42"/>
@@ -33386,11 +33390,11 @@
         <v/>
       </c>
       <c r="H174" s="133"/>
-      <c r="I174" s="675" t="str">
+      <c r="I174" s="674" t="str">
         <f>IF(U152="","",U152)</f>
         <v/>
       </c>
-      <c r="J174" s="675"/>
+      <c r="J174" s="674"/>
       <c r="K174" s="5"/>
       <c r="L174" s="41" t="s">
         <v>180</v>
@@ -33533,18 +33537,18 @@
       <c r="M178" s="42"/>
       <c r="N178" s="5"/>
       <c r="O178" s="13"/>
-      <c r="P178" s="670" t="s">
+      <c r="P178" s="675" t="s">
         <v>196</v>
       </c>
-      <c r="Q178" s="673" t="s">
+      <c r="Q178" s="676" t="s">
         <v>197</v>
       </c>
-      <c r="R178" s="673"/>
-      <c r="S178" s="673"/>
+      <c r="R178" s="676"/>
+      <c r="S178" s="676"/>
       <c r="T178" s="143" t="s">
         <v>196</v>
       </c>
-      <c r="U178" s="672" t="s">
+      <c r="U178" s="677" t="s">
         <v>198</v>
       </c>
       <c r="V178" s="77"/>
@@ -33559,23 +33563,23 @@
       <c r="B179" s="39"/>
       <c r="C179" s="119">
         <f>IF(P155="","",P155)</f>
-        <v>65</v>
-      </c>
-      <c r="D179" s="676" t="s">
+        <v>70</v>
+      </c>
+      <c r="D179" s="678" t="s">
         <v>219</v>
       </c>
-      <c r="E179" s="676"/>
-      <c r="F179" s="676"/>
-      <c r="G179" s="676"/>
-      <c r="H179" s="676"/>
-      <c r="I179" s="676"/>
+      <c r="E179" s="678"/>
+      <c r="F179" s="678"/>
+      <c r="G179" s="678"/>
+      <c r="H179" s="678"/>
+      <c r="I179" s="678"/>
       <c r="J179" s="77"/>
       <c r="K179" s="77"/>
       <c r="L179" s="77"/>
       <c r="M179" s="42"/>
       <c r="N179" s="5"/>
       <c r="O179" s="13"/>
-      <c r="P179" s="670" t="s">
+      <c r="P179" s="675" t="s">
         <v>196</v>
       </c>
       <c r="Q179" s="143" t="s">
@@ -33590,7 +33594,7 @@
       <c r="T179" s="143" t="s">
         <v>202</v>
       </c>
-      <c r="U179" s="672" t="s">
+      <c r="U179" s="677" t="s">
         <v>196</v>
       </c>
       <c r="V179" s="77"/>
@@ -33604,18 +33608,18 @@
       </c>
       <c r="B180" s="39"/>
       <c r="C180" s="47"/>
-      <c r="D180" s="670" t="s">
+      <c r="D180" s="675" t="s">
         <v>196</v>
       </c>
-      <c r="E180" s="671" t="s">
+      <c r="E180" s="679" t="s">
         <v>197</v>
       </c>
-      <c r="F180" s="671"/>
-      <c r="G180" s="671"/>
+      <c r="F180" s="679"/>
+      <c r="G180" s="679"/>
       <c r="H180" s="142" t="s">
         <v>196</v>
       </c>
-      <c r="I180" s="677" t="s">
+      <c r="I180" s="680" t="s">
         <v>198</v>
       </c>
       <c r="J180" s="77"/>
@@ -33643,7 +33647,7 @@
       </c>
       <c r="B181" s="39"/>
       <c r="C181" s="47"/>
-      <c r="D181" s="670" t="s">
+      <c r="D181" s="675" t="s">
         <v>196</v>
       </c>
       <c r="E181" s="142" t="s">
@@ -33658,7 +33662,7 @@
       <c r="H181" s="142" t="s">
         <v>202</v>
       </c>
-      <c r="I181" s="677" t="s">
+      <c r="I181" s="680" t="s">
         <v>202</v>
       </c>
       <c r="J181" s="77"/>
@@ -33971,14 +33975,14 @@
       <c r="M187" s="42"/>
       <c r="N187" s="5"/>
       <c r="O187" s="156"/>
-      <c r="P187" s="678" t="s">
+      <c r="P187" s="663" t="s">
         <v>209</v>
       </c>
-      <c r="Q187" s="678"/>
-      <c r="R187" s="678"/>
-      <c r="S187" s="678"/>
-      <c r="T187" s="678"/>
-      <c r="U187" s="678"/>
+      <c r="Q187" s="663"/>
+      <c r="R187" s="663"/>
+      <c r="S187" s="663"/>
+      <c r="T187" s="663"/>
+      <c r="U187" s="663"/>
       <c r="V187" s="77"/>
       <c r="W187" s="77"/>
       <c r="X187" s="77"/>
@@ -34022,18 +34026,18 @@
       <c r="M188" s="42"/>
       <c r="N188" s="5"/>
       <c r="O188" s="156"/>
-      <c r="P188" s="670" t="s">
+      <c r="P188" s="675" t="s">
         <v>196</v>
       </c>
-      <c r="Q188" s="673" t="s">
+      <c r="Q188" s="676" t="s">
         <v>197</v>
       </c>
-      <c r="R188" s="673"/>
-      <c r="S188" s="673"/>
+      <c r="R188" s="676"/>
+      <c r="S188" s="676"/>
       <c r="T188" s="143" t="s">
         <v>196</v>
       </c>
-      <c r="U188" s="672" t="s">
+      <c r="U188" s="677" t="s">
         <v>198</v>
       </c>
       <c r="V188" s="77"/>
@@ -34047,21 +34051,21 @@
       </c>
       <c r="B189" s="175"/>
       <c r="C189" s="47"/>
-      <c r="D189" s="676" t="s">
+      <c r="D189" s="678" t="s">
         <v>224</v>
       </c>
-      <c r="E189" s="676"/>
-      <c r="F189" s="676"/>
-      <c r="G189" s="676"/>
-      <c r="H189" s="676"/>
-      <c r="I189" s="676"/>
+      <c r="E189" s="678"/>
+      <c r="F189" s="678"/>
+      <c r="G189" s="678"/>
+      <c r="H189" s="678"/>
+      <c r="I189" s="678"/>
       <c r="J189" s="77"/>
       <c r="K189" s="77"/>
       <c r="L189" s="77"/>
       <c r="M189" s="78"/>
       <c r="N189" s="5"/>
       <c r="O189" s="156"/>
-      <c r="P189" s="670" t="s">
+      <c r="P189" s="675" t="s">
         <v>196</v>
       </c>
       <c r="Q189" s="143" t="s">
@@ -34076,7 +34080,7 @@
       <c r="T189" s="143" t="s">
         <v>202</v>
       </c>
-      <c r="U189" s="672"/>
+      <c r="U189" s="677"/>
       <c r="V189" s="77"/>
       <c r="W189" s="77"/>
       <c r="X189" s="77"/>
@@ -36635,7 +36639,7 @@
         <v/>
       </c>
       <c r="V241" s="5"/>
-      <c r="W241" s="690" t="str">
+      <c r="W241" s="595" t="str">
         <f>IF(W234="","",IF(MAX(W234:W240)&gt;0.1,"Fail","Pass"))</f>
         <v/>
       </c>
@@ -36889,11 +36893,11 @@
       <c r="U246" s="47"/>
       <c r="V246" s="5"/>
       <c r="W246" s="5"/>
-      <c r="X246" s="674" t="str">
+      <c r="X246" s="673" t="str">
         <f>IF($O$34=1,AB246,Z246)</f>
-        <v>Selenia</v>
-      </c>
-      <c r="Y246" s="674"/>
+        <v>Selenia Dimensions</v>
+      </c>
+      <c r="Y246" s="673"/>
       <c r="Z246" s="435" t="s">
         <v>602</v>
       </c>
@@ -37015,11 +37019,11 @@
       <c r="W248" s="5"/>
       <c r="X248" s="216">
         <f t="shared" ref="X248:Y250" si="40">IF($O$34=1,AB248,Z248)</f>
-        <v>0.5</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="Y248" s="217">
         <f t="shared" si="40"/>
-        <v>0.61</v>
+        <v>0.66</v>
       </c>
       <c r="Z248" s="435">
         <v>0.5</v>
@@ -37067,11 +37071,11 @@
       <c r="W249" s="5"/>
       <c r="X249" s="216">
         <f t="shared" si="40"/>
-        <v>0.63</v>
+        <v>0.66</v>
       </c>
       <c r="Y249" s="217">
         <f t="shared" si="40"/>
-        <v>0.77</v>
+        <v>0.78</v>
       </c>
       <c r="Z249" s="435">
         <v>0.63</v>
@@ -37129,11 +37133,11 @@
       <c r="W250" s="5"/>
       <c r="X250" s="216">
         <f t="shared" si="40"/>
-        <v>0.77</v>
+        <v>0.78</v>
       </c>
       <c r="Y250" s="217">
         <f t="shared" si="40"/>
-        <v>0.94</v>
+        <v>0.92</v>
       </c>
       <c r="Z250" s="435">
         <v>0.77</v>
@@ -37253,11 +37257,11 @@
       <c r="W252" s="5"/>
       <c r="X252" s="216">
         <f t="shared" ref="X252:Y255" si="42">IF($O$34=1,AB252,Z252)</f>
-        <v>1.04</v>
+        <v>1.06</v>
       </c>
       <c r="Y252" s="217">
         <f t="shared" si="42"/>
-        <v>1.27</v>
+        <v>1.24</v>
       </c>
       <c r="Z252" s="435">
         <v>1.04</v>
@@ -37323,7 +37327,7 @@
       <c r="W253" s="5"/>
       <c r="X253" s="216">
         <f t="shared" si="42"/>
-        <v>1.17</v>
+        <v>1.22</v>
       </c>
       <c r="Y253" s="217">
         <f t="shared" si="42"/>
@@ -37389,11 +37393,11 @@
       <c r="W254" s="5"/>
       <c r="X254" s="216">
         <f t="shared" si="42"/>
-        <v>1.31</v>
+        <v>1.4</v>
       </c>
       <c r="Y254" s="217">
         <f t="shared" si="42"/>
-        <v>1.6</v>
+        <v>1.64</v>
       </c>
       <c r="Z254" s="435">
         <v>1.31</v>
@@ -37455,11 +37459,11 @@
       <c r="W255" s="5"/>
       <c r="X255" s="216">
         <f t="shared" si="42"/>
-        <v>1.44</v>
+        <v>1.61</v>
       </c>
       <c r="Y255" s="217">
         <f t="shared" si="42"/>
-        <v>1.76</v>
+        <v>1.89</v>
       </c>
       <c r="Z255" s="435">
         <v>1.44</v>
@@ -37578,21 +37582,21 @@
       </c>
       <c r="B259" s="39"/>
       <c r="C259" s="5"/>
-      <c r="D259" s="681" t="s">
+      <c r="D259" s="668" t="s">
         <v>263</v>
       </c>
-      <c r="E259" s="681"/>
+      <c r="E259" s="668"/>
       <c r="F259" s="47"/>
-      <c r="G259" s="681" t="s">
+      <c r="G259" s="668" t="s">
         <v>264</v>
       </c>
-      <c r="H259" s="681"/>
+      <c r="H259" s="668"/>
       <c r="I259" s="5"/>
       <c r="J259" s="47"/>
-      <c r="K259" s="682" t="s">
+      <c r="K259" s="669" t="s">
         <v>265</v>
       </c>
-      <c r="L259" s="682"/>
+      <c r="L259" s="669"/>
       <c r="M259" s="78"/>
       <c r="N259" s="5"/>
       <c r="O259" s="110" t="s">
@@ -39870,14 +39874,14 @@
       <c r="B305" s="175"/>
       <c r="C305" s="77"/>
       <c r="D305" s="77"/>
-      <c r="E305" s="683" t="str">
+      <c r="E305" s="670" t="str">
         <f>O294&amp;" "&amp;P295&amp;" "&amp;Q295</f>
         <v xml:space="preserve">Combo Mode 2D Target/Filter: </v>
       </c>
-      <c r="F305" s="683"/>
-      <c r="G305" s="683"/>
-      <c r="H305" s="683"/>
-      <c r="I305" s="683"/>
+      <c r="F305" s="670"/>
+      <c r="G305" s="670"/>
+      <c r="H305" s="670"/>
+      <c r="I305" s="670"/>
       <c r="J305" s="77"/>
       <c r="K305" s="77"/>
       <c r="L305" s="77"/>
@@ -40438,14 +40442,14 @@
       <c r="B316" s="175"/>
       <c r="C316" s="77"/>
       <c r="D316" s="77"/>
-      <c r="E316" s="684" t="str">
+      <c r="E316" s="671" t="str">
         <f>O306&amp;" "&amp;P307&amp;" "&amp;Q307</f>
         <v xml:space="preserve">Combo Mode 3D Target/Filter: </v>
       </c>
-      <c r="F316" s="684"/>
-      <c r="G316" s="684"/>
-      <c r="H316" s="684"/>
-      <c r="I316" s="684"/>
+      <c r="F316" s="671"/>
+      <c r="G316" s="671"/>
+      <c r="H316" s="671"/>
+      <c r="I316" s="671"/>
       <c r="J316" s="77"/>
       <c r="K316" s="77"/>
       <c r="L316" s="77"/>
@@ -40725,10 +40729,10 @@
       <c r="S321" s="41" t="s">
         <v>305</v>
       </c>
-      <c r="T321" s="685">
+      <c r="T321" s="665">
         <v>43014</v>
       </c>
-      <c r="U321" s="685"/>
+      <c r="U321" s="665"/>
       <c r="V321" s="5"/>
       <c r="W321" s="5"/>
       <c r="X321" s="5"/>
@@ -40782,10 +40786,10 @@
       <c r="S322" s="41" t="s">
         <v>307</v>
       </c>
-      <c r="T322" s="685">
+      <c r="T322" s="665">
         <v>43744</v>
       </c>
-      <c r="U322" s="685"/>
+      <c r="U322" s="665"/>
       <c r="V322" s="5"/>
       <c r="W322" s="5"/>
       <c r="X322" s="5"/>
@@ -40881,13 +40885,13 @@
       <c r="Q324" s="5"/>
       <c r="R324" s="5"/>
       <c r="S324" s="5"/>
-      <c r="T324" s="678" t="s">
+      <c r="T324" s="663" t="s">
         <v>308</v>
       </c>
-      <c r="U324" s="678"/>
-      <c r="V324" s="678"/>
-      <c r="W324" s="678"/>
-      <c r="X324" s="678"/>
+      <c r="U324" s="663"/>
+      <c r="V324" s="663"/>
+      <c r="W324" s="663"/>
+      <c r="X324" s="663"/>
       <c r="Y324" s="15"/>
     </row>
     <row r="325" spans="1:25">
@@ -41492,13 +41496,13 @@
       <c r="Q335" s="5"/>
       <c r="R335" s="5"/>
       <c r="S335" s="41"/>
-      <c r="T335" s="678" t="s">
+      <c r="T335" s="663" t="s">
         <v>308</v>
       </c>
-      <c r="U335" s="678"/>
-      <c r="V335" s="678"/>
-      <c r="W335" s="678"/>
-      <c r="X335" s="678"/>
+      <c r="U335" s="663"/>
+      <c r="V335" s="663"/>
+      <c r="W335" s="663"/>
+      <c r="X335" s="663"/>
       <c r="Y335" s="15"/>
     </row>
     <row r="336" spans="1:25">
@@ -41840,11 +41844,11 @@
         <v/>
       </c>
       <c r="U341" s="211" t="str">
-        <f>IF(AN90="","",AVERAGE(AN90:AN91))</f>
+        <f>IF(AN90="","",AN90)</f>
         <v/>
       </c>
       <c r="V341" s="209" t="str">
-        <f>IF(AO90="","",AVERAGE(AO90:AO91))</f>
+        <f>IF(AO90="","",AO90)</f>
         <v/>
       </c>
       <c r="W341" s="237" t="str">
@@ -41901,11 +41905,11 @@
         <v/>
       </c>
       <c r="U342" s="211" t="str">
-        <f>IF(AN91="","",AVERAGE(AN91:AN92))</f>
+        <f>IF(AN91="","",AN91)</f>
         <v/>
       </c>
       <c r="V342" s="209" t="str">
-        <f>IF(AO91="","",AVERAGE(AO91:AO92))</f>
+        <f>IF(AO91="","",AO91)</f>
         <v/>
       </c>
       <c r="W342" s="237" t="str">
@@ -41936,11 +41940,11 @@
       <c r="H343" s="279" t="s">
         <v>305</v>
       </c>
-      <c r="I343" s="679">
+      <c r="I343" s="666">
         <f>IF(T321="","",T321)</f>
         <v>43014</v>
       </c>
-      <c r="J343" s="679"/>
+      <c r="J343" s="666"/>
       <c r="K343" s="33"/>
       <c r="L343" s="33"/>
       <c r="M343" s="35"/>
@@ -41979,11 +41983,11 @@
       <c r="H344" s="228" t="s">
         <v>307</v>
       </c>
-      <c r="I344" s="680">
+      <c r="I344" s="667">
         <f>IF(T322="","",T322)</f>
         <v>43744</v>
       </c>
-      <c r="J344" s="680"/>
+      <c r="J344" s="667"/>
       <c r="K344" s="47"/>
       <c r="L344" s="5"/>
       <c r="M344" s="42"/>
@@ -42024,13 +42028,13 @@
       <c r="Q345" s="5"/>
       <c r="R345" s="5"/>
       <c r="S345" s="41"/>
-      <c r="T345" s="678" t="s">
+      <c r="T345" s="663" t="s">
         <v>308</v>
       </c>
-      <c r="U345" s="678"/>
-      <c r="V345" s="678"/>
-      <c r="W345" s="678"/>
-      <c r="X345" s="678"/>
+      <c r="U345" s="663"/>
+      <c r="V345" s="663"/>
+      <c r="W345" s="663"/>
+      <c r="X345" s="663"/>
       <c r="Y345" s="15"/>
     </row>
     <row r="346" spans="1:25">
@@ -42145,15 +42149,15 @@
         <v>50</v>
       </c>
       <c r="T347" s="209" t="str">
-        <f>IF(AM92="","",AM92)</f>
+        <f>IF(AM92="","",AVERAGE(AM92:AM93))</f>
         <v/>
       </c>
       <c r="U347" s="211" t="str">
-        <f>IF(AN92="","",AN92)</f>
+        <f>IF(AN92="","",AVERAGE(AN92:AN93))</f>
         <v/>
       </c>
       <c r="V347" s="209" t="str">
-        <f>IF(AO92="","",AO92)</f>
+        <f>IF(AO92="","",AVERAGE(AO92:AO93))</f>
         <v/>
       </c>
       <c r="W347" s="237" t="str">
@@ -42216,15 +42220,15 @@
         <v>50</v>
       </c>
       <c r="T348" s="209" t="str">
-        <f>IF(AM100="","",AM100)</f>
+        <f>IF(AM100="","",AVERAGE(AM100:AM101))</f>
         <v/>
       </c>
       <c r="U348" s="211" t="str">
-        <f>IF(AN100="","",AN100)</f>
+        <f>IF(AN100="","",AVERAGE(AN100:AN101))</f>
         <v/>
       </c>
       <c r="V348" s="209" t="str">
-        <f>IF(AO100="","",AO100)</f>
+        <f>IF(AO100="","",AVERAGE(AO100:AO101))</f>
         <v/>
       </c>
       <c r="W348" s="237" t="str">
@@ -42284,15 +42288,15 @@
         <v>50</v>
       </c>
       <c r="T349" s="209" t="str">
-        <f>IF(AM108="","",AM108)</f>
+        <f>IF(AM108="","",AVERAGE(AM108:AM109))</f>
         <v/>
       </c>
       <c r="U349" s="211" t="str">
-        <f>IF(AN108="","",AN108)</f>
+        <f>IF(AN108="","",AVERAGE(AN108:AN109))</f>
         <v/>
       </c>
       <c r="V349" s="209" t="str">
-        <f>IF(AO108="","",AO108)</f>
+        <f>IF(AO108="","",AVERAGE(AO108:AO109))</f>
         <v/>
       </c>
       <c r="W349" s="237" t="str">
@@ -42358,15 +42362,15 @@
         <v>50</v>
       </c>
       <c r="T350" s="209" t="str">
-        <f>IF(AM116="","",AM116)</f>
+        <f>IF(AM116="","",AVERAGE(AM116:AM117))</f>
         <v/>
       </c>
       <c r="U350" s="211" t="str">
-        <f>IF(AN116="","",AN116)</f>
+        <f>IF(AN116="","",AVERAGE(AN116:AN117))</f>
         <v/>
       </c>
       <c r="V350" s="209" t="str">
-        <f>IF(AO116="","",AO116)</f>
+        <f>IF(AO116="","",AVERAGE(AO116:AO117))</f>
         <v/>
       </c>
       <c r="W350" s="237" t="str">
@@ -42441,15 +42445,15 @@
         <v>50</v>
       </c>
       <c r="T351" s="209" t="str">
-        <f>IF(AM124="","",AM124)</f>
+        <f>IF(AM124="","",AVERAGE(AM124:AM125))</f>
         <v/>
       </c>
       <c r="U351" s="211" t="str">
-        <f>IF(AN124="","",AN124)</f>
+        <f>IF(AN124="","",AVERAGE(AN124:AN125))</f>
         <v/>
       </c>
       <c r="V351" s="209" t="str">
-        <f>IF(AO124="","",AO124)</f>
+        <f>IF(AO124="","",AVERAGE(AO124:AO125))</f>
         <v/>
       </c>
       <c r="W351" s="237" t="str">
@@ -42732,13 +42736,13 @@
       <c r="Q356" s="5"/>
       <c r="R356" s="5"/>
       <c r="S356" s="41"/>
-      <c r="T356" s="678" t="s">
+      <c r="T356" s="663" t="s">
         <v>308</v>
       </c>
-      <c r="U356" s="678"/>
-      <c r="V356" s="678"/>
-      <c r="W356" s="678"/>
-      <c r="X356" s="678"/>
+      <c r="U356" s="663"/>
+      <c r="V356" s="663"/>
+      <c r="W356" s="663"/>
+      <c r="X356" s="663"/>
       <c r="Y356" s="15"/>
     </row>
     <row r="357" spans="1:25" ht="16.5" thickBot="1">
@@ -43225,7 +43229,7 @@
       </c>
       <c r="T365" s="288"/>
       <c r="U365" s="288"/>
-      <c r="V365" s="691"/>
+      <c r="V365" s="596"/>
       <c r="W365" s="591" t="str">
         <f>IF(AB87="","",AB87)</f>
         <v/>
@@ -43445,13 +43449,13 @@
       <c r="Q370" s="5"/>
       <c r="R370" s="5"/>
       <c r="S370" s="5"/>
-      <c r="T370" s="678" t="s">
+      <c r="T370" s="663" t="s">
         <v>308</v>
       </c>
-      <c r="U370" s="678"/>
-      <c r="V370" s="678"/>
-      <c r="W370" s="678"/>
-      <c r="X370" s="678"/>
+      <c r="U370" s="663"/>
+      <c r="V370" s="663"/>
+      <c r="W370" s="663"/>
+      <c r="X370" s="663"/>
       <c r="Y370" s="15"/>
     </row>
     <row r="371" spans="1:25">
@@ -44122,16 +44126,16 @@
       <c r="P383" s="299" t="s">
         <v>340</v>
       </c>
-      <c r="Q383" s="686" t="s">
+      <c r="Q383" s="664" t="s">
         <v>341</v>
       </c>
-      <c r="R383" s="686"/>
-      <c r="S383" s="686"/>
-      <c r="T383" s="686"/>
-      <c r="U383" s="686"/>
-      <c r="V383" s="686"/>
-      <c r="W383" s="686"/>
-      <c r="X383" s="686"/>
+      <c r="R383" s="664"/>
+      <c r="S383" s="664"/>
+      <c r="T383" s="664"/>
+      <c r="U383" s="664"/>
+      <c r="V383" s="664"/>
+      <c r="W383" s="664"/>
+      <c r="X383" s="664"/>
       <c r="Y383" s="15"/>
     </row>
     <row r="384" spans="1:25">
@@ -44935,13 +44939,13 @@
       <c r="P396" s="299" t="s">
         <v>340</v>
       </c>
-      <c r="Q396" s="686" t="s">
+      <c r="Q396" s="664" t="s">
         <v>341</v>
       </c>
-      <c r="R396" s="686"/>
-      <c r="S396" s="686"/>
-      <c r="T396" s="686"/>
-      <c r="U396" s="686"/>
+      <c r="R396" s="664"/>
+      <c r="S396" s="664"/>
+      <c r="T396" s="664"/>
+      <c r="U396" s="664"/>
       <c r="V396" s="77"/>
       <c r="W396" s="77"/>
       <c r="X396" s="77"/>
@@ -47491,22 +47495,58 @@
     </row>
   </sheetData>
   <mergeCells count="84">
-    <mergeCell ref="T356:X356"/>
-    <mergeCell ref="T370:X370"/>
-    <mergeCell ref="Q383:X383"/>
-    <mergeCell ref="Q396:U396"/>
-    <mergeCell ref="T322:U322"/>
-    <mergeCell ref="T324:X324"/>
-    <mergeCell ref="T335:X335"/>
-    <mergeCell ref="I343:J343"/>
-    <mergeCell ref="I344:J344"/>
-    <mergeCell ref="T345:X345"/>
-    <mergeCell ref="D259:E259"/>
-    <mergeCell ref="G259:H259"/>
-    <mergeCell ref="K259:L259"/>
-    <mergeCell ref="E305:I305"/>
-    <mergeCell ref="E316:I316"/>
-    <mergeCell ref="T321:U321"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="D35:F36"/>
+    <mergeCell ref="G35:I36"/>
+    <mergeCell ref="J35:L36"/>
+    <mergeCell ref="L44:M44"/>
+    <mergeCell ref="P97:R98"/>
+    <mergeCell ref="V97:X98"/>
+    <mergeCell ref="P105:R106"/>
+    <mergeCell ref="S105:U106"/>
+    <mergeCell ref="V105:X106"/>
+    <mergeCell ref="P150:S150"/>
+    <mergeCell ref="U150:V150"/>
+    <mergeCell ref="S97:U98"/>
+    <mergeCell ref="I173:J173"/>
+    <mergeCell ref="U151:V151"/>
+    <mergeCell ref="U152:V152"/>
+    <mergeCell ref="P156:P157"/>
+    <mergeCell ref="Q156:S156"/>
+    <mergeCell ref="U156:U157"/>
+    <mergeCell ref="P164:U164"/>
+    <mergeCell ref="P165:P166"/>
+    <mergeCell ref="Q165:S165"/>
+    <mergeCell ref="U165:U166"/>
     <mergeCell ref="D172:G172"/>
     <mergeCell ref="I172:J172"/>
     <mergeCell ref="X246:Y246"/>
@@ -47523,401 +47563,365 @@
     <mergeCell ref="Q188:S188"/>
     <mergeCell ref="U188:U189"/>
     <mergeCell ref="D189:I189"/>
-    <mergeCell ref="I173:J173"/>
-    <mergeCell ref="U151:V151"/>
-    <mergeCell ref="U152:V152"/>
-    <mergeCell ref="P156:P157"/>
-    <mergeCell ref="Q156:S156"/>
-    <mergeCell ref="U156:U157"/>
-    <mergeCell ref="P164:U164"/>
-    <mergeCell ref="P165:P166"/>
-    <mergeCell ref="Q165:S165"/>
-    <mergeCell ref="U165:U166"/>
-    <mergeCell ref="V97:X98"/>
-    <mergeCell ref="P105:R106"/>
-    <mergeCell ref="S105:U106"/>
-    <mergeCell ref="V105:X106"/>
-    <mergeCell ref="P150:S150"/>
-    <mergeCell ref="U150:V150"/>
-    <mergeCell ref="S97:U98"/>
-    <mergeCell ref="D35:F36"/>
-    <mergeCell ref="G35:I36"/>
-    <mergeCell ref="J35:L36"/>
-    <mergeCell ref="L44:M44"/>
-    <mergeCell ref="P97:R98"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="I343:J343"/>
+    <mergeCell ref="I344:J344"/>
+    <mergeCell ref="T345:X345"/>
+    <mergeCell ref="D259:E259"/>
+    <mergeCell ref="G259:H259"/>
+    <mergeCell ref="K259:L259"/>
+    <mergeCell ref="E305:I305"/>
+    <mergeCell ref="E316:I316"/>
+    <mergeCell ref="T321:U321"/>
+    <mergeCell ref="T356:X356"/>
+    <mergeCell ref="T370:X370"/>
+    <mergeCell ref="Q383:X383"/>
+    <mergeCell ref="Q396:U396"/>
+    <mergeCell ref="T322:U322"/>
+    <mergeCell ref="T324:X324"/>
+    <mergeCell ref="T335:X335"/>
   </mergeCells>
   <conditionalFormatting sqref="P171:U172">
-    <cfRule type="cellIs" dxfId="72" priority="87" operator="lessThan">
+    <cfRule type="cellIs" dxfId="84" priority="87" operator="lessThan">
       <formula>0.02</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="88" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="83" priority="88" operator="greaterThan">
       <formula>0.02</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P190:U193">
-    <cfRule type="cellIs" dxfId="70" priority="84" operator="between">
+    <cfRule type="cellIs" dxfId="82" priority="84" operator="between">
       <formula>0.02</formula>
       <formula>-0.02</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="85" operator="lessThan">
+    <cfRule type="cellIs" dxfId="81" priority="85" operator="lessThan">
       <formula>-0.02</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="86" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="80" priority="86" operator="greaterThan">
       <formula>0.02</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P194:U194">
-    <cfRule type="cellIs" dxfId="67" priority="81" operator="lessThan">
+    <cfRule type="cellIs" dxfId="79" priority="81" operator="lessThan">
       <formula>-0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="82" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="78" priority="82" operator="greaterThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="83" operator="between">
+    <cfRule type="cellIs" dxfId="77" priority="83" operator="between">
       <formula>-0.01</formula>
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W219:W226">
-    <cfRule type="cellIs" dxfId="64" priority="79" operator="lessThan">
+    <cfRule type="cellIs" dxfId="76" priority="79" operator="lessThan">
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="80" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="75" priority="80" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W234:W240">
-    <cfRule type="cellIs" dxfId="62" priority="77" operator="lessThan">
+    <cfRule type="cellIs" dxfId="74" priority="77" operator="lessThan">
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="78" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="73" priority="78" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U248">
-    <cfRule type="cellIs" dxfId="60" priority="76" operator="between">
+    <cfRule type="cellIs" dxfId="72" priority="76" operator="between">
       <formula>$X$248</formula>
       <formula>$Y$248</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U249">
-    <cfRule type="cellIs" dxfId="59" priority="75" operator="between">
+    <cfRule type="cellIs" dxfId="71" priority="75" operator="between">
       <formula>$X$249</formula>
       <formula>$Y$249</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U250">
-    <cfRule type="cellIs" dxfId="58" priority="74" operator="between">
+    <cfRule type="cellIs" dxfId="70" priority="74" operator="between">
       <formula>$X$250</formula>
       <formula>$Y$250</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U252">
-    <cfRule type="cellIs" dxfId="57" priority="73" operator="between">
+    <cfRule type="cellIs" dxfId="69" priority="73" operator="between">
       <formula>$X$252</formula>
       <formula>$Y$252</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U253">
-    <cfRule type="cellIs" dxfId="56" priority="72" operator="between">
+    <cfRule type="cellIs" dxfId="68" priority="72" operator="between">
       <formula>$X$253</formula>
       <formula>$Y$253</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U254">
-    <cfRule type="cellIs" dxfId="55" priority="71" operator="between">
+    <cfRule type="cellIs" dxfId="67" priority="71" operator="between">
       <formula>$X$254</formula>
       <formula>$Y$254</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U255">
-    <cfRule type="cellIs" dxfId="54" priority="70" operator="between">
+    <cfRule type="cellIs" dxfId="66" priority="70" operator="between">
       <formula>$X$255</formula>
       <formula>$Y$255</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X266 X281 X301 X313">
-    <cfRule type="cellIs" dxfId="53" priority="69" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="65" priority="69" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X271 X286 X305 X317">
-    <cfRule type="cellIs" dxfId="52" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="64" priority="3" operator="lessThan">
       <formula>0.15</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="68" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="63" priority="68" operator="greaterThan">
       <formula>0.15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X318">
-    <cfRule type="cellIs" dxfId="50" priority="67" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="62" priority="67" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T364:X364">
-    <cfRule type="cellIs" dxfId="49" priority="64" operator="lessThan">
+    <cfRule type="cellIs" dxfId="61" priority="64" operator="lessThan">
       <formula>-0.02</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="65" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="60" priority="65" operator="greaterThan">
       <formula>0.02</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="66" operator="between">
+    <cfRule type="cellIs" dxfId="59" priority="66" operator="between">
       <formula>0.02</formula>
       <formula>-0.02</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W376">
-    <cfRule type="cellIs" dxfId="46" priority="62" operator="lessThan">
+    <cfRule type="cellIs" dxfId="58" priority="62" operator="lessThan">
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="63" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="57" priority="63" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U410 P429 R429 Q420:R420 U420:V420">
-    <cfRule type="cellIs" dxfId="44" priority="47" operator="lessThan">
+    <cfRule type="cellIs" dxfId="56" priority="47" operator="lessThan">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="48" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="55" priority="48" operator="greaterThanOrEqual">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U411 Q421:R421 U421:V421 P430 R430">
-    <cfRule type="cellIs" dxfId="42" priority="45" operator="lessThan">
+    <cfRule type="cellIs" dxfId="54" priority="45" operator="lessThan">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="46" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="53" priority="46" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U412 Q422:R422 U422:V422 P431 R431">
-    <cfRule type="cellIs" dxfId="40" priority="43" operator="lessThan">
+    <cfRule type="cellIs" dxfId="52" priority="43" operator="lessThan">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="44" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="51" priority="44" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T429">
-    <cfRule type="cellIs" dxfId="38" priority="41" operator="lessThan">
+    <cfRule type="cellIs" dxfId="50" priority="41" operator="lessThan">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="42" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="49" priority="42" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T430:T431">
-    <cfRule type="cellIs" dxfId="36" priority="39" operator="lessThan">
+    <cfRule type="cellIs" dxfId="48" priority="39" operator="lessThan">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="40" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="47" priority="40" operator="greaterThanOrEqual">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T441">
-    <cfRule type="cellIs" dxfId="34" priority="37" operator="lessThan">
+    <cfRule type="cellIs" dxfId="46" priority="37" operator="lessThan">
       <formula>40</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="38" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="45" priority="38" operator="greaterThanOrEqual">
       <formula>40</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V442">
-    <cfRule type="cellIs" dxfId="32" priority="34" operator="lessThan">
+    <cfRule type="cellIs" dxfId="44" priority="34" operator="lessThan">
       <formula>-0.15</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="35" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="43" priority="35" operator="greaterThan">
       <formula>0.15</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="36" operator="between">
+    <cfRule type="cellIs" dxfId="42" priority="36" operator="between">
       <formula>0.15</formula>
       <formula>-0.15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T326">
-    <cfRule type="cellIs" dxfId="29" priority="31" operator="between">
+    <cfRule type="cellIs" dxfId="41" priority="31" operator="between">
       <formula>$R$326*0.95</formula>
       <formula>$R$326*1.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T327">
-    <cfRule type="cellIs" dxfId="28" priority="30" operator="between">
+    <cfRule type="cellIs" dxfId="40" priority="30" operator="between">
       <formula>$R$327*0.95</formula>
       <formula>$R$327*1.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T328">
-    <cfRule type="cellIs" dxfId="27" priority="29" operator="between">
+    <cfRule type="cellIs" dxfId="39" priority="29" operator="between">
       <formula>$R$328*0.95</formula>
       <formula>$R$328*1.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T329">
-    <cfRule type="cellIs" dxfId="26" priority="28" operator="between">
+    <cfRule type="cellIs" dxfId="38" priority="28" operator="between">
       <formula>$R$329*0.95</formula>
       <formula>$R$329*1.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T330">
-    <cfRule type="cellIs" dxfId="25" priority="27" operator="between">
+    <cfRule type="cellIs" dxfId="37" priority="27" operator="between">
       <formula>$R$330*0.95</formula>
       <formula>$R$330*1.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T331">
-    <cfRule type="cellIs" dxfId="24" priority="26" operator="between">
+    <cfRule type="cellIs" dxfId="36" priority="26" operator="between">
       <formula>$R$331*0.95</formula>
       <formula>$R$331*1.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T332">
-    <cfRule type="cellIs" dxfId="23" priority="25" operator="between">
+    <cfRule type="cellIs" dxfId="35" priority="25" operator="between">
       <formula>$R$332*0.95</formula>
       <formula>$R$332*1.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T337">
-    <cfRule type="cellIs" dxfId="22" priority="24" operator="between">
+    <cfRule type="cellIs" dxfId="34" priority="24" operator="between">
       <formula>$R$337*0.95</formula>
       <formula>$R$337*1.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T338">
-    <cfRule type="cellIs" dxfId="21" priority="23" operator="between">
+    <cfRule type="cellIs" dxfId="33" priority="23" operator="between">
       <formula>$R$338*0.95</formula>
       <formula>$R$338*1.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T339">
-    <cfRule type="cellIs" dxfId="20" priority="22" operator="between">
+    <cfRule type="cellIs" dxfId="32" priority="22" operator="between">
       <formula>$R$339*0.95</formula>
       <formula>$R$339*1.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T340">
-    <cfRule type="cellIs" dxfId="19" priority="21" operator="between">
+    <cfRule type="cellIs" dxfId="31" priority="21" operator="between">
       <formula>$R$340*0.95</formula>
       <formula>$R$340*1.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T341">
-    <cfRule type="cellIs" dxfId="18" priority="20" operator="between">
+    <cfRule type="cellIs" dxfId="30" priority="20" operator="between">
       <formula>$R$341*0.95</formula>
       <formula>$R$341*1.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T342">
-    <cfRule type="cellIs" dxfId="17" priority="19" operator="between">
+    <cfRule type="cellIs" dxfId="29" priority="19" operator="between">
       <formula>$R$342*0.95</formula>
       <formula>$R$342*1.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T347">
-    <cfRule type="cellIs" dxfId="16" priority="18" operator="between">
+    <cfRule type="cellIs" dxfId="28" priority="18" operator="between">
       <formula>$R$347*0.95</formula>
       <formula>$R$347*1.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T348">
-    <cfRule type="cellIs" dxfId="15" priority="17" operator="between">
+    <cfRule type="cellIs" dxfId="27" priority="17" operator="between">
       <formula>$R$348*0.95</formula>
       <formula>$R$348*1.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T349">
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="between">
+    <cfRule type="cellIs" dxfId="26" priority="16" operator="between">
       <formula>$R$349*0.95</formula>
       <formula>$R$349*1.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T350">
-    <cfRule type="cellIs" dxfId="13" priority="15" operator="between">
+    <cfRule type="cellIs" dxfId="25" priority="15" operator="between">
       <formula>$R$350*0.95</formula>
       <formula>$R$350*1.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T351">
-    <cfRule type="cellIs" dxfId="12" priority="14" operator="between">
+    <cfRule type="cellIs" dxfId="24" priority="14" operator="between">
       <formula>$R$351*0.95</formula>
       <formula>$R$351*1.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R123:R130">
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="23" priority="11" operator="lessThan">
       <formula>-0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="22" priority="12" operator="greaterThan">
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="13" operator="between">
+    <cfRule type="cellIs" dxfId="21" priority="13" operator="between">
       <formula>0.5</formula>
       <formula>-0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U152:V152">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="20" priority="9" operator="lessThan">
       <formula>160</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="10" operator="greaterThan">
       <formula>160</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q142:V142">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="7" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="8" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q210:T210">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X266 X281 X301 X313 X318">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="4" operator="lessThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q390:X390 Q403:U403">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -47955,39 +47959,39 @@
       </c>
     </row>
     <row r="2" spans="1:30" ht="16.5" thickBot="1">
-      <c r="B2" s="689" t="s">
+      <c r="B2" s="691" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="689"/>
-      <c r="D2" s="689"/>
-      <c r="E2" s="689"/>
-      <c r="F2" s="689"/>
-      <c r="G2" s="689"/>
-      <c r="H2" s="689"/>
-      <c r="I2" s="689"/>
-      <c r="J2" s="689"/>
-      <c r="L2" s="689" t="s">
+      <c r="C2" s="691"/>
+      <c r="D2" s="691"/>
+      <c r="E2" s="691"/>
+      <c r="F2" s="691"/>
+      <c r="G2" s="691"/>
+      <c r="H2" s="691"/>
+      <c r="I2" s="691"/>
+      <c r="J2" s="691"/>
+      <c r="L2" s="691" t="s">
         <v>49</v>
       </c>
-      <c r="M2" s="689"/>
-      <c r="N2" s="689"/>
-      <c r="O2" s="689"/>
-      <c r="P2" s="689"/>
-      <c r="Q2" s="689"/>
-      <c r="R2" s="689"/>
-      <c r="S2" s="689"/>
-      <c r="T2" s="689"/>
-      <c r="V2" s="689" t="s">
+      <c r="M2" s="691"/>
+      <c r="N2" s="691"/>
+      <c r="O2" s="691"/>
+      <c r="P2" s="691"/>
+      <c r="Q2" s="691"/>
+      <c r="R2" s="691"/>
+      <c r="S2" s="691"/>
+      <c r="T2" s="691"/>
+      <c r="V2" s="691" t="s">
         <v>49</v>
       </c>
-      <c r="W2" s="689"/>
-      <c r="X2" s="689"/>
-      <c r="Y2" s="689"/>
-      <c r="Z2" s="689"/>
-      <c r="AA2" s="689"/>
-      <c r="AB2" s="689"/>
-      <c r="AC2" s="689"/>
-      <c r="AD2" s="689"/>
+      <c r="W2" s="691"/>
+      <c r="X2" s="691"/>
+      <c r="Y2" s="691"/>
+      <c r="Z2" s="691"/>
+      <c r="AA2" s="691"/>
+      <c r="AB2" s="691"/>
+      <c r="AC2" s="691"/>
+      <c r="AD2" s="691"/>
     </row>
     <row r="3" spans="1:30" ht="16.5" thickTop="1">
       <c r="A3" s="424" t="s">
@@ -49448,36 +49452,36 @@
     </row>
     <row r="26" spans="1:30" ht="16.5" thickTop="1">
       <c r="A26" s="424"/>
-      <c r="B26" s="687" t="s">
+      <c r="B26" s="689" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="687"/>
-      <c r="D26" s="687"/>
-      <c r="E26" s="687"/>
-      <c r="F26" s="687"/>
-      <c r="G26" s="687"/>
-      <c r="H26" s="687"/>
-      <c r="I26" s="687"/>
-      <c r="J26" s="687"/>
-      <c r="K26" s="687"/>
-      <c r="L26" s="687"/>
-      <c r="M26" s="688"/>
+      <c r="C26" s="689"/>
+      <c r="D26" s="689"/>
+      <c r="E26" s="689"/>
+      <c r="F26" s="689"/>
+      <c r="G26" s="689"/>
+      <c r="H26" s="689"/>
+      <c r="I26" s="689"/>
+      <c r="J26" s="689"/>
+      <c r="K26" s="689"/>
+      <c r="L26" s="689"/>
+      <c r="M26" s="690"/>
       <c r="N26" s="424"/>
-      <c r="O26" s="687" t="s">
+      <c r="O26" s="689" t="s">
         <v>49</v>
       </c>
-      <c r="P26" s="687"/>
-      <c r="Q26" s="687"/>
-      <c r="R26" s="687"/>
-      <c r="S26" s="687"/>
-      <c r="T26" s="687"/>
-      <c r="U26" s="687"/>
-      <c r="V26" s="687"/>
-      <c r="W26" s="687"/>
-      <c r="X26" s="687"/>
-      <c r="Y26" s="687"/>
-      <c r="Z26" s="687"/>
-      <c r="AA26" s="688"/>
+      <c r="P26" s="689"/>
+      <c r="Q26" s="689"/>
+      <c r="R26" s="689"/>
+      <c r="S26" s="689"/>
+      <c r="T26" s="689"/>
+      <c r="U26" s="689"/>
+      <c r="V26" s="689"/>
+      <c r="W26" s="689"/>
+      <c r="X26" s="689"/>
+      <c r="Y26" s="689"/>
+      <c r="Z26" s="689"/>
+      <c r="AA26" s="690"/>
     </row>
     <row r="27" spans="1:30">
       <c r="A27" s="427" t="s">
@@ -51313,33 +51317,33 @@
     </row>
     <row r="51" spans="1:26" ht="16.5" thickTop="1">
       <c r="A51" s="424"/>
-      <c r="B51" s="687" t="s">
+      <c r="B51" s="689" t="s">
         <v>49</v>
       </c>
-      <c r="C51" s="687"/>
-      <c r="D51" s="687"/>
-      <c r="E51" s="687"/>
-      <c r="F51" s="687"/>
-      <c r="G51" s="687"/>
-      <c r="H51" s="687"/>
-      <c r="I51" s="687"/>
-      <c r="J51" s="687"/>
-      <c r="K51" s="687"/>
-      <c r="L51" s="687"/>
-      <c r="M51" s="687"/>
-      <c r="N51" s="687"/>
-      <c r="O51" s="687"/>
-      <c r="P51" s="687"/>
-      <c r="Q51" s="687"/>
-      <c r="R51" s="687"/>
-      <c r="S51" s="687"/>
-      <c r="T51" s="687"/>
-      <c r="U51" s="687"/>
-      <c r="V51" s="687"/>
-      <c r="W51" s="687"/>
-      <c r="X51" s="687"/>
-      <c r="Y51" s="687"/>
-      <c r="Z51" s="688"/>
+      <c r="C51" s="689"/>
+      <c r="D51" s="689"/>
+      <c r="E51" s="689"/>
+      <c r="F51" s="689"/>
+      <c r="G51" s="689"/>
+      <c r="H51" s="689"/>
+      <c r="I51" s="689"/>
+      <c r="J51" s="689"/>
+      <c r="K51" s="689"/>
+      <c r="L51" s="689"/>
+      <c r="M51" s="689"/>
+      <c r="N51" s="689"/>
+      <c r="O51" s="689"/>
+      <c r="P51" s="689"/>
+      <c r="Q51" s="689"/>
+      <c r="R51" s="689"/>
+      <c r="S51" s="689"/>
+      <c r="T51" s="689"/>
+      <c r="U51" s="689"/>
+      <c r="V51" s="689"/>
+      <c r="W51" s="689"/>
+      <c r="X51" s="689"/>
+      <c r="Y51" s="689"/>
+      <c r="Z51" s="690"/>
     </row>
     <row r="52" spans="1:26">
       <c r="A52" s="427" t="s">
@@ -54048,11 +54052,11 @@
         <f>"DGN values (mrad/R) for "&amp;Sheet1!$T$260&amp;" kV and HVL="&amp;ROUND(Sheet1!$X$263,2)&amp;" mm Al"</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G100" s="689" t="s">
+      <c r="G100" s="691" t="s">
         <v>441</v>
       </c>
-      <c r="H100" s="689"/>
-      <c r="I100" s="689"/>
+      <c r="H100" s="691"/>
+      <c r="I100" s="691"/>
       <c r="T100" t="s">
         <v>604</v>
       </c>
@@ -60374,50 +60378,50 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C12">
-    <cfRule type="cellIs" dxfId="84" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="lessThan">
       <formula>21.8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="between">
       <formula>24</formula>
       <formula>27</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="3" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="greaterThanOrEqual">
       <formula>40</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="cellIs" dxfId="81" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="lessThan">
       <formula>21.8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="between">
       <formula>25.35</formula>
       <formula>31.55</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="6" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="greaterThanOrEqual">
       <formula>40</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="cellIs" dxfId="78" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="lessThan">
       <formula>21.8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="8" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="between">
       <formula>24</formula>
       <formula>27</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="9" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="3" priority="9" operator="greaterThanOrEqual">
       <formula>40</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="cellIs" dxfId="75" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="10" operator="lessThan">
       <formula>21.8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="11" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="11" operator="between">
       <formula>25.35</formula>
       <formula>31.55</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="12" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="12" operator="greaterThanOrEqual">
       <formula>40</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update formulas in HVL section of Tables sheet
</commit_message>
<xml_diff>
--- a/MUSCMammoHologic.xlsx
+++ b/MUSCMammoHologic.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8190" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8190" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="QC Test Summary-Hologic" sheetId="11" r:id="rId1"/>
@@ -5467,7 +5467,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="692">
+  <cellXfs count="693">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -7181,96 +7181,96 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="153" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="55" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="23" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="131" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="25" fillId="14" borderId="55" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="25" fillId="14" borderId="23" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="25" fillId="14" borderId="131" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="25" fillId="14" borderId="55" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="25" fillId="14" borderId="23" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="25" fillId="14" borderId="131" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="55" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="23" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="131" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="132" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="133" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="134" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="135" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="130" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="99" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="55" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="23" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="131" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="55" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="131" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="55" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="131" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="131" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="55" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="23" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="131" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="132" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="133" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="134" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="135" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="130" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="99" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="55" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="23" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="131" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="55" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="23" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="131" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="25" fillId="14" borderId="55" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="25" fillId="14" borderId="23" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="25" fillId="14" borderId="131" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="25" fillId="14" borderId="55" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="25" fillId="14" borderId="23" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="25" fillId="14" borderId="131" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="15" borderId="55" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -7280,6 +7280,27 @@
     <xf numFmtId="0" fontId="24" fillId="15" borderId="131" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="14" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -7301,33 +7322,51 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="112" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="143" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="58" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="141" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="14" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="143" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="58" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="141" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="143" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="141" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="141" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="143" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="58" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="141" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="58" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="141" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -7340,124 +7379,85 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="23" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="143" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="58" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="141" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="143" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="58" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="141" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="143" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="141" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="143" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="58" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="141" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="108" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="100" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="101" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="98" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="108" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="100" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="101" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="124" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -7466,6 +7466,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -16590,40 +16593,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="26.25">
-      <c r="A1" s="623" t="s">
+      <c r="A1" s="597" t="s">
         <v>407</v>
       </c>
-      <c r="B1" s="623"/>
-      <c r="C1" s="623"/>
-      <c r="D1" s="623"/>
-      <c r="E1" s="623"/>
-      <c r="F1" s="623"/>
-      <c r="G1" s="623"/>
-      <c r="H1" s="623"/>
-      <c r="I1" s="623"/>
-      <c r="J1" s="623"/>
-      <c r="K1" s="623"/>
-      <c r="L1" s="623"/>
-      <c r="M1" s="623"/>
-      <c r="N1" s="623"/>
+      <c r="B1" s="597"/>
+      <c r="C1" s="597"/>
+      <c r="D1" s="597"/>
+      <c r="E1" s="597"/>
+      <c r="F1" s="597"/>
+      <c r="G1" s="597"/>
+      <c r="H1" s="597"/>
+      <c r="I1" s="597"/>
+      <c r="J1" s="597"/>
+      <c r="K1" s="597"/>
+      <c r="L1" s="597"/>
+      <c r="M1" s="597"/>
+      <c r="N1" s="597"/>
     </row>
     <row r="2" spans="1:15" ht="26.25">
-      <c r="A2" s="623" t="s">
+      <c r="A2" s="597" t="s">
         <v>651</v>
       </c>
-      <c r="B2" s="623"/>
-      <c r="C2" s="623"/>
-      <c r="D2" s="623"/>
-      <c r="E2" s="623"/>
-      <c r="F2" s="623"/>
-      <c r="G2" s="623"/>
-      <c r="H2" s="623"/>
-      <c r="I2" s="623"/>
-      <c r="J2" s="623"/>
-      <c r="K2" s="623"/>
-      <c r="L2" s="623"/>
-      <c r="M2" s="623"/>
-      <c r="N2" s="623"/>
+      <c r="B2" s="597"/>
+      <c r="C2" s="597"/>
+      <c r="D2" s="597"/>
+      <c r="E2" s="597"/>
+      <c r="F2" s="597"/>
+      <c r="G2" s="597"/>
+      <c r="H2" s="597"/>
+      <c r="I2" s="597"/>
+      <c r="J2" s="597"/>
+      <c r="K2" s="597"/>
+      <c r="L2" s="597"/>
+      <c r="M2" s="597"/>
+      <c r="N2" s="597"/>
     </row>
     <row r="3" spans="1:15" ht="16.5" customHeight="1">
       <c r="A3" s="471"/>
@@ -16646,43 +16649,43 @@
         <v>408</v>
       </c>
       <c r="B4" s="472"/>
-      <c r="C4" s="617"/>
-      <c r="D4" s="618"/>
-      <c r="E4" s="618"/>
-      <c r="F4" s="618"/>
-      <c r="G4" s="618"/>
-      <c r="H4" s="619"/>
+      <c r="C4" s="598"/>
+      <c r="D4" s="599"/>
+      <c r="E4" s="599"/>
+      <c r="F4" s="599"/>
+      <c r="G4" s="599"/>
+      <c r="H4" s="600"/>
       <c r="I4" s="473"/>
       <c r="J4" s="474" t="s">
         <v>409</v>
       </c>
-      <c r="K4" s="624"/>
-      <c r="L4" s="625"/>
-      <c r="M4" s="625"/>
-      <c r="N4" s="626"/>
+      <c r="K4" s="601"/>
+      <c r="L4" s="602"/>
+      <c r="M4" s="602"/>
+      <c r="N4" s="603"/>
     </row>
     <row r="5" spans="1:15" ht="16.5" customHeight="1">
       <c r="A5" s="472" t="s">
         <v>410</v>
       </c>
       <c r="B5" s="472"/>
-      <c r="C5" s="617"/>
-      <c r="D5" s="618"/>
-      <c r="E5" s="618"/>
-      <c r="F5" s="618"/>
-      <c r="G5" s="618"/>
-      <c r="H5" s="619"/>
+      <c r="C5" s="598"/>
+      <c r="D5" s="599"/>
+      <c r="E5" s="599"/>
+      <c r="F5" s="599"/>
+      <c r="G5" s="599"/>
+      <c r="H5" s="600"/>
       <c r="I5" s="473"/>
       <c r="J5" s="474" t="s">
         <v>411</v>
       </c>
-      <c r="K5" s="624">
+      <c r="K5" s="601">
         <f>Sheet1!P7</f>
         <v>0</v>
       </c>
-      <c r="L5" s="625"/>
-      <c r="M5" s="625"/>
-      <c r="N5" s="626"/>
+      <c r="L5" s="602"/>
+      <c r="M5" s="602"/>
+      <c r="N5" s="603"/>
     </row>
     <row r="6" spans="1:15" ht="16.5" customHeight="1">
       <c r="A6" s="472" t="s">
@@ -16690,21 +16693,21 @@
       </c>
       <c r="B6" s="472"/>
       <c r="C6" s="472"/>
-      <c r="D6" s="617" t="s">
+      <c r="D6" s="598" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="618"/>
-      <c r="F6" s="618"/>
-      <c r="G6" s="618"/>
-      <c r="H6" s="619"/>
+      <c r="E6" s="599"/>
+      <c r="F6" s="599"/>
+      <c r="G6" s="599"/>
+      <c r="H6" s="600"/>
       <c r="I6" s="473"/>
       <c r="J6" s="474" t="s">
         <v>413</v>
       </c>
-      <c r="K6" s="617"/>
-      <c r="L6" s="618"/>
-      <c r="M6" s="618"/>
-      <c r="N6" s="619"/>
+      <c r="K6" s="598"/>
+      <c r="L6" s="599"/>
+      <c r="M6" s="599"/>
+      <c r="N6" s="600"/>
     </row>
     <row r="7" spans="1:15" ht="16.5" customHeight="1">
       <c r="A7" s="472" t="s">
@@ -16712,21 +16715,21 @@
       </c>
       <c r="B7" s="472"/>
       <c r="C7" s="472"/>
-      <c r="D7" s="617" t="s">
+      <c r="D7" s="598" t="s">
         <v>415</v>
       </c>
-      <c r="E7" s="618"/>
-      <c r="F7" s="618"/>
-      <c r="G7" s="618"/>
-      <c r="H7" s="619"/>
+      <c r="E7" s="599"/>
+      <c r="F7" s="599"/>
+      <c r="G7" s="599"/>
+      <c r="H7" s="600"/>
       <c r="I7" s="473"/>
       <c r="J7" s="474" t="s">
         <v>416</v>
       </c>
-      <c r="K7" s="617"/>
-      <c r="L7" s="618"/>
-      <c r="M7" s="618"/>
-      <c r="N7" s="619"/>
+      <c r="K7" s="598"/>
+      <c r="L7" s="599"/>
+      <c r="M7" s="599"/>
+      <c r="N7" s="600"/>
     </row>
     <row r="8" spans="1:15" ht="16.5" customHeight="1">
       <c r="A8" s="472" t="s">
@@ -16734,22 +16737,22 @@
       </c>
       <c r="B8" s="472"/>
       <c r="C8" s="472"/>
-      <c r="D8" s="620" t="str">
+      <c r="D8" s="604" t="str">
         <f>Sheet1!K16</f>
         <v/>
       </c>
-      <c r="E8" s="621"/>
-      <c r="F8" s="621"/>
-      <c r="G8" s="621"/>
-      <c r="H8" s="622"/>
+      <c r="E8" s="605"/>
+      <c r="F8" s="605"/>
+      <c r="G8" s="605"/>
+      <c r="H8" s="606"/>
       <c r="I8" s="473"/>
       <c r="J8" s="474" t="s">
         <v>418</v>
       </c>
-      <c r="K8" s="617"/>
-      <c r="L8" s="618"/>
-      <c r="M8" s="618"/>
-      <c r="N8" s="619"/>
+      <c r="K8" s="598"/>
+      <c r="L8" s="599"/>
+      <c r="M8" s="599"/>
+      <c r="N8" s="600"/>
     </row>
     <row r="9" spans="1:15" ht="11.25" customHeight="1">
       <c r="A9" s="475"/>
@@ -16763,11 +16766,11 @@
       <c r="A10" s="475" t="s">
         <v>652</v>
       </c>
-      <c r="D10" s="604"/>
-      <c r="E10" s="605"/>
-      <c r="F10" s="605"/>
-      <c r="G10" s="605"/>
-      <c r="H10" s="606"/>
+      <c r="D10" s="608"/>
+      <c r="E10" s="609"/>
+      <c r="F10" s="609"/>
+      <c r="G10" s="609"/>
+      <c r="H10" s="610"/>
       <c r="I10" s="477" t="s">
         <v>653</v>
       </c>
@@ -16793,25 +16796,25 @@
       </c>
       <c r="B12" s="472"/>
       <c r="C12" s="472"/>
-      <c r="D12" s="607" t="s">
+      <c r="D12" s="611" t="s">
         <v>421</v>
       </c>
-      <c r="E12" s="607"/>
-      <c r="F12" s="607"/>
-      <c r="G12" s="607" t="s">
+      <c r="E12" s="611"/>
+      <c r="F12" s="611"/>
+      <c r="G12" s="611" t="s">
         <v>416</v>
       </c>
-      <c r="H12" s="607"/>
-      <c r="I12" s="607" t="s">
+      <c r="H12" s="611"/>
+      <c r="I12" s="611" t="s">
         <v>8</v>
       </c>
-      <c r="J12" s="607"/>
-      <c r="K12" s="607" t="s">
+      <c r="J12" s="611"/>
+      <c r="K12" s="611" t="s">
         <v>419</v>
       </c>
-      <c r="L12" s="607"/>
-      <c r="M12" s="607"/>
-      <c r="N12" s="607"/>
+      <c r="L12" s="611"/>
+      <c r="M12" s="611"/>
+      <c r="N12" s="611"/>
     </row>
     <row r="13" spans="1:15" ht="16.5" customHeight="1" thickTop="1">
       <c r="A13" s="472"/>
@@ -16819,63 +16822,63 @@
       <c r="C13" s="479" t="s">
         <v>422</v>
       </c>
-      <c r="D13" s="608" t="s">
+      <c r="D13" s="612" t="s">
         <v>689</v>
       </c>
-      <c r="E13" s="609"/>
-      <c r="F13" s="610"/>
-      <c r="G13" s="608" t="s">
+      <c r="E13" s="613"/>
+      <c r="F13" s="614"/>
+      <c r="G13" s="612" t="s">
         <v>690</v>
       </c>
-      <c r="H13" s="610"/>
-      <c r="I13" s="611"/>
-      <c r="J13" s="612"/>
-      <c r="K13" s="608" t="s">
+      <c r="H13" s="614"/>
+      <c r="I13" s="615"/>
+      <c r="J13" s="616"/>
+      <c r="K13" s="612" t="s">
         <v>691</v>
       </c>
-      <c r="L13" s="609"/>
-      <c r="M13" s="609"/>
-      <c r="N13" s="610"/>
+      <c r="L13" s="613"/>
+      <c r="M13" s="613"/>
+      <c r="N13" s="614"/>
     </row>
     <row r="14" spans="1:15" ht="16.5" customHeight="1">
       <c r="C14" s="479" t="s">
         <v>423</v>
       </c>
-      <c r="D14" s="613" t="s">
+      <c r="D14" s="617" t="s">
         <v>689</v>
       </c>
-      <c r="E14" s="614"/>
-      <c r="F14" s="615"/>
-      <c r="G14" s="613" t="s">
+      <c r="E14" s="618"/>
+      <c r="F14" s="619"/>
+      <c r="G14" s="617" t="s">
         <v>692</v>
       </c>
-      <c r="H14" s="615"/>
-      <c r="I14" s="604"/>
-      <c r="J14" s="606"/>
-      <c r="K14" s="613" t="s">
+      <c r="H14" s="619"/>
+      <c r="I14" s="608"/>
+      <c r="J14" s="610"/>
+      <c r="K14" s="617" t="s">
         <v>693</v>
       </c>
-      <c r="L14" s="614"/>
-      <c r="M14" s="614"/>
-      <c r="N14" s="615"/>
+      <c r="L14" s="618"/>
+      <c r="M14" s="618"/>
+      <c r="N14" s="619"/>
     </row>
     <row r="15" spans="1:15" s="480" customFormat="1" ht="36" customHeight="1">
-      <c r="A15" s="616" t="s">
+      <c r="A15" s="620" t="s">
         <v>654</v>
       </c>
-      <c r="B15" s="616"/>
-      <c r="C15" s="616"/>
-      <c r="D15" s="616"/>
-      <c r="E15" s="616"/>
-      <c r="F15" s="616"/>
-      <c r="G15" s="616"/>
-      <c r="H15" s="616"/>
-      <c r="I15" s="616"/>
-      <c r="J15" s="616"/>
-      <c r="K15" s="616"/>
-      <c r="L15" s="616"/>
-      <c r="M15" s="616"/>
-      <c r="N15" s="616"/>
+      <c r="B15" s="620"/>
+      <c r="C15" s="620"/>
+      <c r="D15" s="620"/>
+      <c r="E15" s="620"/>
+      <c r="F15" s="620"/>
+      <c r="G15" s="620"/>
+      <c r="H15" s="620"/>
+      <c r="I15" s="620"/>
+      <c r="J15" s="620"/>
+      <c r="K15" s="620"/>
+      <c r="L15" s="620"/>
+      <c r="M15" s="620"/>
+      <c r="N15" s="620"/>
     </row>
     <row r="16" spans="1:15" ht="16.5" customHeight="1">
       <c r="A16" s="475" t="s">
@@ -16937,46 +16940,46 @@
       <c r="L18" s="496"/>
     </row>
     <row r="19" spans="1:15" ht="21" customHeight="1">
-      <c r="A19" s="603" t="s">
+      <c r="A19" s="607" t="s">
         <v>426</v>
       </c>
-      <c r="B19" s="603"/>
-      <c r="C19" s="603"/>
-      <c r="D19" s="603"/>
-      <c r="E19" s="603"/>
-      <c r="F19" s="603"/>
-      <c r="G19" s="603"/>
-      <c r="H19" s="603"/>
-      <c r="I19" s="603"/>
-      <c r="J19" s="603"/>
-      <c r="K19" s="603"/>
-      <c r="L19" s="603"/>
-      <c r="M19" s="603"/>
-      <c r="N19" s="603"/>
+      <c r="B19" s="607"/>
+      <c r="C19" s="607"/>
+      <c r="D19" s="607"/>
+      <c r="E19" s="607"/>
+      <c r="F19" s="607"/>
+      <c r="G19" s="607"/>
+      <c r="H19" s="607"/>
+      <c r="I19" s="607"/>
+      <c r="J19" s="607"/>
+      <c r="K19" s="607"/>
+      <c r="L19" s="607"/>
+      <c r="M19" s="607"/>
+      <c r="N19" s="607"/>
     </row>
     <row r="20" spans="1:15" ht="15" customHeight="1">
-      <c r="A20" s="601" t="s">
+      <c r="A20" s="623" t="s">
         <v>427</v>
       </c>
-      <c r="B20" s="601"/>
-      <c r="C20" s="601"/>
-      <c r="D20" s="601"/>
-      <c r="E20" s="601"/>
-      <c r="F20" s="601"/>
-      <c r="G20" s="601"/>
-      <c r="H20" s="601"/>
-      <c r="I20" s="601"/>
-      <c r="J20" s="601"/>
-      <c r="K20" s="601"/>
-      <c r="L20" s="601"/>
-      <c r="M20" s="601"/>
-      <c r="N20" s="601"/>
+      <c r="B20" s="623"/>
+      <c r="C20" s="623"/>
+      <c r="D20" s="623"/>
+      <c r="E20" s="623"/>
+      <c r="F20" s="623"/>
+      <c r="G20" s="623"/>
+      <c r="H20" s="623"/>
+      <c r="I20" s="623"/>
+      <c r="J20" s="623"/>
+      <c r="K20" s="623"/>
+      <c r="L20" s="623"/>
+      <c r="M20" s="623"/>
+      <c r="N20" s="623"/>
     </row>
     <row r="21" spans="1:15" ht="15" customHeight="1">
-      <c r="M21" s="602" t="s">
+      <c r="M21" s="624" t="s">
         <v>428</v>
       </c>
-      <c r="N21" s="602"/>
+      <c r="N21" s="624"/>
     </row>
     <row r="22" spans="1:15" ht="15.75" customHeight="1">
       <c r="A22" s="497" t="s">
@@ -16993,8 +16996,8 @@
       <c r="J22" s="472"/>
       <c r="K22" s="472"/>
       <c r="L22" s="472"/>
-      <c r="M22" s="598"/>
-      <c r="N22" s="599"/>
+      <c r="M22" s="621"/>
+      <c r="N22" s="622"/>
     </row>
     <row r="23" spans="1:15" ht="15.75" customHeight="1">
       <c r="A23" s="497" t="s">
@@ -17011,8 +17014,8 @@
       <c r="J23" s="472"/>
       <c r="K23" s="472"/>
       <c r="L23" s="472"/>
-      <c r="M23" s="598"/>
-      <c r="N23" s="599"/>
+      <c r="M23" s="621"/>
+      <c r="N23" s="622"/>
     </row>
     <row r="24" spans="1:15" ht="15.75" customHeight="1">
       <c r="A24" s="497" t="s">
@@ -17029,8 +17032,8 @@
       <c r="J24" s="473"/>
       <c r="K24" s="473"/>
       <c r="L24" s="473"/>
-      <c r="M24" s="598"/>
-      <c r="N24" s="599"/>
+      <c r="M24" s="621"/>
+      <c r="N24" s="622"/>
     </row>
     <row r="25" spans="1:15" ht="15.75" customHeight="1">
       <c r="A25" s="497" t="s">
@@ -17047,8 +17050,8 @@
       <c r="J25" s="472"/>
       <c r="K25" s="472"/>
       <c r="L25" s="472"/>
-      <c r="M25" s="598"/>
-      <c r="N25" s="599"/>
+      <c r="M25" s="621"/>
+      <c r="N25" s="622"/>
     </row>
     <row r="26" spans="1:15" ht="15.75" customHeight="1">
       <c r="A26" s="497" t="s">
@@ -17065,8 +17068,8 @@
       <c r="J26" s="472"/>
       <c r="K26" s="472"/>
       <c r="L26" s="472"/>
-      <c r="M26" s="598"/>
-      <c r="N26" s="599"/>
+      <c r="M26" s="621"/>
+      <c r="N26" s="622"/>
     </row>
     <row r="27" spans="1:15" ht="15.75" customHeight="1">
       <c r="A27" s="497" t="s">
@@ -17083,8 +17086,8 @@
       <c r="J27" s="472"/>
       <c r="K27" s="472"/>
       <c r="L27" s="472"/>
-      <c r="M27" s="598"/>
-      <c r="N27" s="599"/>
+      <c r="M27" s="621"/>
+      <c r="N27" s="622"/>
     </row>
     <row r="28" spans="1:15" ht="15.75" customHeight="1">
       <c r="A28" s="497" t="s">
@@ -17101,8 +17104,8 @@
       <c r="J28" s="472"/>
       <c r="K28" s="472"/>
       <c r="L28" s="472"/>
-      <c r="M28" s="598"/>
-      <c r="N28" s="599"/>
+      <c r="M28" s="621"/>
+      <c r="N28" s="622"/>
     </row>
     <row r="29" spans="1:15" ht="15.75" customHeight="1">
       <c r="A29" s="497" t="s">
@@ -17134,8 +17137,8 @@
       <c r="L30" s="502" t="s">
         <v>329</v>
       </c>
-      <c r="M30" s="598"/>
-      <c r="N30" s="599"/>
+      <c r="M30" s="621"/>
+      <c r="N30" s="622"/>
     </row>
     <row r="31" spans="1:15" ht="15.75" customHeight="1">
       <c r="A31" s="472"/>
@@ -17157,8 +17160,8 @@
       <c r="L31" s="502" t="s">
         <v>329</v>
       </c>
-      <c r="M31" s="598"/>
-      <c r="N31" s="599"/>
+      <c r="M31" s="621"/>
+      <c r="N31" s="622"/>
     </row>
     <row r="32" spans="1:15" ht="15.75" customHeight="1">
       <c r="A32" s="472" t="s">
@@ -17175,8 +17178,8 @@
       <c r="J32" s="472"/>
       <c r="K32" s="472"/>
       <c r="L32" s="472"/>
-      <c r="M32" s="598"/>
-      <c r="N32" s="599"/>
+      <c r="M32" s="621"/>
+      <c r="N32" s="622"/>
     </row>
     <row r="33" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
       <c r="A33" s="472" t="s">
@@ -17221,8 +17224,8 @@
       </c>
       <c r="K34" s="476"/>
       <c r="L34" s="476"/>
-      <c r="M34" s="598"/>
-      <c r="N34" s="599"/>
+      <c r="M34" s="621"/>
+      <c r="N34" s="622"/>
     </row>
     <row r="35" spans="1:14" ht="15.75" customHeight="1">
       <c r="C35" s="503" t="s">
@@ -17244,8 +17247,8 @@
         <v>0</v>
       </c>
       <c r="L35" s="476"/>
-      <c r="M35" s="598"/>
-      <c r="N35" s="599"/>
+      <c r="M35" s="621"/>
+      <c r="N35" s="622"/>
     </row>
     <row r="36" spans="1:14" ht="15.75" customHeight="1">
       <c r="A36" s="472" t="s">
@@ -17283,8 +17286,8 @@
       <c r="J37" s="508"/>
       <c r="K37" s="514"/>
       <c r="L37" s="514"/>
-      <c r="M37" s="598"/>
-      <c r="N37" s="599"/>
+      <c r="M37" s="621"/>
+      <c r="N37" s="622"/>
     </row>
     <row r="38" spans="1:14" ht="15.75" customHeight="1">
       <c r="A38" s="472"/>
@@ -17324,8 +17327,8 @@
       <c r="J39" s="508"/>
       <c r="K39" s="514"/>
       <c r="L39" s="514"/>
-      <c r="M39" s="598"/>
-      <c r="N39" s="599"/>
+      <c r="M39" s="621"/>
+      <c r="N39" s="622"/>
     </row>
     <row r="40" spans="1:14" ht="15.75" customHeight="1">
       <c r="A40" s="472" t="s">
@@ -17342,8 +17345,8 @@
       <c r="J40" s="472"/>
       <c r="K40" s="472"/>
       <c r="L40" s="472"/>
-      <c r="M40" s="598"/>
-      <c r="N40" s="599"/>
+      <c r="M40" s="621"/>
+      <c r="N40" s="622"/>
     </row>
     <row r="41" spans="1:14" ht="15.75" customHeight="1">
       <c r="A41" s="472" t="s">
@@ -17360,8 +17363,8 @@
       <c r="J41" s="472"/>
       <c r="K41" s="472"/>
       <c r="L41" s="472"/>
-      <c r="M41" s="598"/>
-      <c r="N41" s="599"/>
+      <c r="M41" s="621"/>
+      <c r="N41" s="622"/>
     </row>
     <row r="42" spans="1:14" ht="15.75" customHeight="1">
       <c r="A42" s="472" t="s">
@@ -17378,8 +17381,8 @@
       <c r="J42" s="472"/>
       <c r="K42" s="472"/>
       <c r="L42" s="472"/>
-      <c r="M42" s="598"/>
-      <c r="N42" s="599"/>
+      <c r="M42" s="621"/>
+      <c r="N42" s="622"/>
     </row>
     <row r="43" spans="1:14" ht="15.75" customHeight="1">
       <c r="A43" s="497" t="s">
@@ -17396,8 +17399,8 @@
       <c r="J43" s="497"/>
       <c r="K43" s="497"/>
       <c r="L43" s="472"/>
-      <c r="M43" s="598"/>
-      <c r="N43" s="600"/>
+      <c r="M43" s="621"/>
+      <c r="N43" s="626"/>
     </row>
     <row r="44" spans="1:14" ht="15.75" customHeight="1">
       <c r="A44" s="472" t="s">
@@ -17414,8 +17417,8 @@
       <c r="J44" s="472"/>
       <c r="K44" s="472"/>
       <c r="L44" s="472"/>
-      <c r="M44" s="598"/>
-      <c r="N44" s="599"/>
+      <c r="M44" s="621"/>
+      <c r="N44" s="622"/>
     </row>
     <row r="45" spans="1:14" ht="15.75" customHeight="1">
       <c r="A45" s="472" t="s">
@@ -17432,8 +17435,8 @@
       <c r="J45" s="472"/>
       <c r="K45" s="472"/>
       <c r="L45" s="472"/>
-      <c r="M45" s="598"/>
-      <c r="N45" s="599"/>
+      <c r="M45" s="621"/>
+      <c r="N45" s="622"/>
     </row>
     <row r="46" spans="1:14" ht="15.75" customHeight="1">
       <c r="A46" s="472" t="s">
@@ -17450,8 +17453,8 @@
       <c r="J46" s="472"/>
       <c r="K46" s="472"/>
       <c r="L46" s="472"/>
-      <c r="M46" s="598"/>
-      <c r="N46" s="599"/>
+      <c r="M46" s="621"/>
+      <c r="N46" s="622"/>
     </row>
     <row r="47" spans="1:14" ht="15.75" customHeight="1">
       <c r="A47" s="472"/>
@@ -17470,37 +17473,49 @@
       <c r="N47" s="514"/>
     </row>
     <row r="48" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A48" s="597" t="s">
+      <c r="A48" s="625" t="s">
         <v>676</v>
       </c>
-      <c r="B48" s="597"/>
-      <c r="C48" s="597"/>
-      <c r="D48" s="597"/>
-      <c r="E48" s="597"/>
-      <c r="F48" s="597"/>
-      <c r="G48" s="597"/>
-      <c r="H48" s="597"/>
-      <c r="I48" s="597"/>
-      <c r="J48" s="597"/>
-      <c r="K48" s="597"/>
-      <c r="L48" s="597"/>
-      <c r="M48" s="597"/>
-      <c r="N48" s="597"/>
+      <c r="B48" s="625"/>
+      <c r="C48" s="625"/>
+      <c r="D48" s="625"/>
+      <c r="E48" s="625"/>
+      <c r="F48" s="625"/>
+      <c r="G48" s="625"/>
+      <c r="H48" s="625"/>
+      <c r="I48" s="625"/>
+      <c r="J48" s="625"/>
+      <c r="K48" s="625"/>
+      <c r="L48" s="625"/>
+      <c r="M48" s="625"/>
+      <c r="N48" s="625"/>
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="A2:N2"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="K4:N4"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="K5:N5"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="K6:N6"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="K7:N7"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="K8:N8"/>
+    <mergeCell ref="A48:N48"/>
+    <mergeCell ref="M34:N34"/>
+    <mergeCell ref="M35:N35"/>
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="M39:N39"/>
+    <mergeCell ref="M40:N40"/>
+    <mergeCell ref="M41:N41"/>
+    <mergeCell ref="M42:N42"/>
+    <mergeCell ref="M43:N43"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="M45:N45"/>
+    <mergeCell ref="M46:N46"/>
+    <mergeCell ref="M32:N32"/>
+    <mergeCell ref="A20:N20"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="M31:N31"/>
     <mergeCell ref="A19:N19"/>
     <mergeCell ref="D10:H10"/>
     <mergeCell ref="D12:F12"/>
@@ -17516,30 +17531,18 @@
     <mergeCell ref="I14:J14"/>
     <mergeCell ref="K14:N14"/>
     <mergeCell ref="A15:N15"/>
-    <mergeCell ref="M32:N32"/>
-    <mergeCell ref="A20:N20"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="M31:N31"/>
-    <mergeCell ref="A48:N48"/>
-    <mergeCell ref="M34:N34"/>
-    <mergeCell ref="M35:N35"/>
-    <mergeCell ref="M37:N37"/>
-    <mergeCell ref="M39:N39"/>
-    <mergeCell ref="M40:N40"/>
-    <mergeCell ref="M41:N41"/>
-    <mergeCell ref="M42:N42"/>
-    <mergeCell ref="M43:N43"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="M45:N45"/>
-    <mergeCell ref="M46:N46"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="K7:N7"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="K8:N8"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="A2:N2"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="K4:N4"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="K5:N5"/>
   </mergeCells>
   <conditionalFormatting sqref="M22:N28 M32:N32 M37:N37 M39:N40 M42:N42 M44:N45 M43">
     <cfRule type="cellIs" dxfId="93" priority="7" stopIfTrue="1" operator="equal">
@@ -17815,69 +17818,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="27" customHeight="1">
-      <c r="A1" s="637" t="s">
+      <c r="A1" s="630" t="s">
         <v>407</v>
       </c>
-      <c r="B1" s="637"/>
-      <c r="C1" s="637"/>
-      <c r="D1" s="637"/>
-      <c r="E1" s="637"/>
-      <c r="F1" s="637"/>
-      <c r="G1" s="637"/>
-      <c r="H1" s="637"/>
-      <c r="I1" s="637"/>
-      <c r="J1" s="637"/>
-      <c r="K1" s="637"/>
-      <c r="L1" s="637"/>
+      <c r="B1" s="630"/>
+      <c r="C1" s="630"/>
+      <c r="D1" s="630"/>
+      <c r="E1" s="630"/>
+      <c r="F1" s="630"/>
+      <c r="G1" s="630"/>
+      <c r="H1" s="630"/>
+      <c r="I1" s="630"/>
+      <c r="J1" s="630"/>
+      <c r="K1" s="630"/>
+      <c r="L1" s="630"/>
     </row>
     <row r="2" spans="1:12" ht="18" customHeight="1">
-      <c r="A2" s="638" t="s">
+      <c r="A2" s="631" t="s">
         <v>677</v>
       </c>
-      <c r="B2" s="639"/>
-      <c r="C2" s="639"/>
-      <c r="D2" s="639"/>
-      <c r="E2" s="639"/>
-      <c r="F2" s="639"/>
-      <c r="G2" s="639"/>
-      <c r="H2" s="639"/>
-      <c r="I2" s="639"/>
-      <c r="J2" s="639"/>
-      <c r="K2" s="639"/>
-      <c r="L2" s="639"/>
+      <c r="B2" s="632"/>
+      <c r="C2" s="632"/>
+      <c r="D2" s="632"/>
+      <c r="E2" s="632"/>
+      <c r="F2" s="632"/>
+      <c r="G2" s="632"/>
+      <c r="H2" s="632"/>
+      <c r="I2" s="632"/>
+      <c r="J2" s="632"/>
+      <c r="K2" s="632"/>
+      <c r="L2" s="632"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1"/>
     <row r="4" spans="1:12" ht="24" customHeight="1">
-      <c r="A4" s="640" t="s">
+      <c r="A4" s="633" t="s">
         <v>442</v>
       </c>
-      <c r="B4" s="640"/>
-      <c r="C4" s="640"/>
-      <c r="D4" s="640"/>
-      <c r="E4" s="640"/>
-      <c r="F4" s="640"/>
-      <c r="G4" s="640"/>
-      <c r="H4" s="640"/>
-      <c r="I4" s="640"/>
-      <c r="J4" s="640"/>
-      <c r="K4" s="640"/>
-      <c r="L4" s="640"/>
+      <c r="B4" s="633"/>
+      <c r="C4" s="633"/>
+      <c r="D4" s="633"/>
+      <c r="E4" s="633"/>
+      <c r="F4" s="633"/>
+      <c r="G4" s="633"/>
+      <c r="H4" s="633"/>
+      <c r="I4" s="633"/>
+      <c r="J4" s="633"/>
+      <c r="K4" s="633"/>
+      <c r="L4" s="633"/>
     </row>
     <row r="5" spans="1:12" ht="42" customHeight="1">
-      <c r="A5" s="641" t="s">
+      <c r="A5" s="634" t="s">
         <v>678</v>
       </c>
-      <c r="B5" s="641"/>
-      <c r="C5" s="641"/>
-      <c r="D5" s="641"/>
-      <c r="E5" s="641"/>
-      <c r="F5" s="641"/>
-      <c r="G5" s="641"/>
-      <c r="H5" s="641"/>
-      <c r="I5" s="641"/>
-      <c r="J5" s="641"/>
-      <c r="K5" s="641"/>
-      <c r="L5" s="641"/>
+      <c r="B5" s="634"/>
+      <c r="C5" s="634"/>
+      <c r="D5" s="634"/>
+      <c r="E5" s="634"/>
+      <c r="F5" s="634"/>
+      <c r="G5" s="634"/>
+      <c r="H5" s="634"/>
+      <c r="I5" s="634"/>
+      <c r="J5" s="634"/>
+      <c r="K5" s="634"/>
+      <c r="L5" s="634"/>
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1">
       <c r="A6" s="517" t="s">
@@ -17912,9 +17915,9 @@
       <c r="L7" s="524"/>
     </row>
     <row r="8" spans="1:12" ht="15" customHeight="1">
-      <c r="J8" s="642"/>
-      <c r="K8" s="642"/>
-      <c r="L8" s="642"/>
+      <c r="J8" s="635"/>
+      <c r="K8" s="635"/>
+      <c r="L8" s="635"/>
     </row>
     <row r="9" spans="1:12" ht="15" customHeight="1">
       <c r="A9" s="476"/>
@@ -17923,11 +17926,11 @@
         <v>443</v>
       </c>
       <c r="I9" s="493"/>
-      <c r="J9" s="643" t="s">
+      <c r="J9" s="636" t="s">
         <v>428</v>
       </c>
-      <c r="K9" s="643"/>
-      <c r="L9" s="643"/>
+      <c r="K9" s="636"/>
+      <c r="L9" s="636"/>
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1">
       <c r="A10" s="526" t="s">
@@ -18118,52 +18121,52 @@
     </row>
     <row r="23" spans="1:12" ht="15.75" customHeight="1"/>
     <row r="24" spans="1:12" ht="24" customHeight="1">
-      <c r="A24" s="630" t="s">
+      <c r="A24" s="637" t="s">
         <v>468</v>
       </c>
-      <c r="B24" s="630"/>
-      <c r="C24" s="630"/>
-      <c r="D24" s="630"/>
-      <c r="E24" s="630"/>
-      <c r="F24" s="630"/>
-      <c r="G24" s="630"/>
-      <c r="H24" s="630"/>
-      <c r="I24" s="630"/>
-      <c r="J24" s="630"/>
-      <c r="K24" s="630"/>
-      <c r="L24" s="630"/>
+      <c r="B24" s="637"/>
+      <c r="C24" s="637"/>
+      <c r="D24" s="637"/>
+      <c r="E24" s="637"/>
+      <c r="F24" s="637"/>
+      <c r="G24" s="637"/>
+      <c r="H24" s="637"/>
+      <c r="I24" s="637"/>
+      <c r="J24" s="637"/>
+      <c r="K24" s="637"/>
+      <c r="L24" s="637"/>
     </row>
     <row r="25" spans="1:12" ht="15" customHeight="1"/>
     <row r="26" spans="1:12" ht="241.5" customHeight="1">
-      <c r="A26" s="631"/>
-      <c r="B26" s="632"/>
-      <c r="C26" s="632"/>
-      <c r="D26" s="632"/>
-      <c r="E26" s="632"/>
-      <c r="F26" s="632"/>
-      <c r="G26" s="632"/>
-      <c r="H26" s="632"/>
-      <c r="I26" s="632"/>
-      <c r="J26" s="632"/>
-      <c r="K26" s="632"/>
-      <c r="L26" s="633"/>
+      <c r="A26" s="638"/>
+      <c r="B26" s="639"/>
+      <c r="C26" s="639"/>
+      <c r="D26" s="639"/>
+      <c r="E26" s="639"/>
+      <c r="F26" s="639"/>
+      <c r="G26" s="639"/>
+      <c r="H26" s="639"/>
+      <c r="I26" s="639"/>
+      <c r="J26" s="639"/>
+      <c r="K26" s="639"/>
+      <c r="L26" s="640"/>
     </row>
     <row r="27" spans="1:12" ht="15" customHeight="1" thickBot="1"/>
     <row r="28" spans="1:12" ht="204.75" customHeight="1" thickBot="1">
-      <c r="A28" s="634" t="s">
+      <c r="A28" s="641" t="s">
         <v>688</v>
       </c>
-      <c r="B28" s="635"/>
-      <c r="C28" s="635"/>
-      <c r="D28" s="635"/>
-      <c r="E28" s="635"/>
-      <c r="F28" s="635"/>
-      <c r="G28" s="635"/>
-      <c r="H28" s="635"/>
-      <c r="I28" s="635"/>
-      <c r="J28" s="635"/>
-      <c r="K28" s="635"/>
-      <c r="L28" s="636"/>
+      <c r="B28" s="642"/>
+      <c r="C28" s="642"/>
+      <c r="D28" s="642"/>
+      <c r="E28" s="642"/>
+      <c r="F28" s="642"/>
+      <c r="G28" s="642"/>
+      <c r="H28" s="642"/>
+      <c r="I28" s="642"/>
+      <c r="J28" s="642"/>
+      <c r="K28" s="642"/>
+      <c r="L28" s="643"/>
     </row>
     <row r="33" spans="2:12" ht="18" customHeight="1">
       <c r="B33" s="472"/>
@@ -18180,6 +18183,16 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="J22:L22"/>
+    <mergeCell ref="A24:L24"/>
+    <mergeCell ref="A26:L26"/>
+    <mergeCell ref="A28:L28"/>
+    <mergeCell ref="J16:L16"/>
+    <mergeCell ref="J17:L17"/>
+    <mergeCell ref="J18:L18"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="J20:L20"/>
+    <mergeCell ref="J21:L21"/>
     <mergeCell ref="J15:L15"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A2:L2"/>
@@ -18192,16 +18205,6 @@
     <mergeCell ref="J12:L12"/>
     <mergeCell ref="J13:L13"/>
     <mergeCell ref="J14:L14"/>
-    <mergeCell ref="J22:L22"/>
-    <mergeCell ref="A24:L24"/>
-    <mergeCell ref="A26:L26"/>
-    <mergeCell ref="A28:L28"/>
-    <mergeCell ref="J16:L16"/>
-    <mergeCell ref="J17:L17"/>
-    <mergeCell ref="J18:L18"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="J20:L20"/>
-    <mergeCell ref="J21:L21"/>
   </mergeCells>
   <conditionalFormatting sqref="J22:L22 J20 J10:L19">
     <cfRule type="cellIs" dxfId="86" priority="2" stopIfTrue="1" operator="equal">
@@ -18756,13 +18759,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33" customHeight="1">
-      <c r="A1" s="646" t="s">
+      <c r="A1" s="659" t="s">
         <v>469</v>
       </c>
-      <c r="B1" s="647"/>
-      <c r="C1" s="647"/>
-      <c r="D1" s="647"/>
-      <c r="E1" s="647"/>
+      <c r="B1" s="660"/>
+      <c r="C1" s="660"/>
+      <c r="D1" s="660"/>
+      <c r="E1" s="660"/>
     </row>
     <row r="2" spans="1:5" ht="18" customHeight="1">
       <c r="A2" s="534"/>
@@ -18775,23 +18778,23 @@
       <c r="A3" s="535" t="s">
         <v>470</v>
       </c>
-      <c r="B3" s="648">
+      <c r="B3" s="661">
         <f>'QC Test Summary-Hologic'!C4</f>
         <v>0</v>
       </c>
-      <c r="C3" s="648"/>
-      <c r="D3" s="648"/>
-      <c r="E3" s="648"/>
+      <c r="C3" s="661"/>
+      <c r="D3" s="661"/>
+      <c r="E3" s="661"/>
     </row>
     <row r="4" spans="1:5" ht="16.5" customHeight="1">
       <c r="A4" s="535" t="s">
         <v>471</v>
       </c>
-      <c r="B4" s="649" t="str">
+      <c r="B4" s="662" t="str">
         <f>Sheet1!R17</f>
         <v/>
       </c>
-      <c r="C4" s="649"/>
+      <c r="C4" s="662"/>
       <c r="D4" s="536" t="s">
         <v>23</v>
       </c>
@@ -18821,11 +18824,11 @@
       <c r="A6" s="535" t="s">
         <v>474</v>
       </c>
-      <c r="B6" s="649" t="str">
+      <c r="B6" s="662" t="str">
         <f>Sheet1!X7</f>
         <v>Eugene Mah</v>
       </c>
-      <c r="C6" s="649"/>
+      <c r="C6" s="662"/>
       <c r="D6" s="536" t="s">
         <v>475</v>
       </c>
@@ -18838,8 +18841,8 @@
       <c r="A7" s="535" t="s">
         <v>476</v>
       </c>
-      <c r="B7" s="649"/>
-      <c r="C7" s="649"/>
+      <c r="B7" s="662"/>
+      <c r="C7" s="662"/>
       <c r="D7" s="536" t="s">
         <v>477</v>
       </c>
@@ -18867,7 +18870,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="33" customHeight="1" thickTop="1">
-      <c r="A10" s="644" t="s">
+      <c r="A10" s="658" t="s">
         <v>482</v>
       </c>
       <c r="B10" s="543" t="s">
@@ -18882,7 +18885,7 @@
       <c r="E10" s="546"/>
     </row>
     <row r="11" spans="1:5" ht="25.5" customHeight="1" thickBot="1">
-      <c r="A11" s="645"/>
+      <c r="A11" s="654"/>
       <c r="B11" s="547" t="s">
         <v>486</v>
       </c>
@@ -18895,7 +18898,7 @@
       <c r="E11" s="550"/>
     </row>
     <row r="12" spans="1:5" ht="33.75" customHeight="1">
-      <c r="A12" s="655" t="s">
+      <c r="A12" s="649" t="s">
         <v>488</v>
       </c>
       <c r="B12" s="551" t="s">
@@ -18910,7 +18913,7 @@
       <c r="E12" s="554"/>
     </row>
     <row r="13" spans="1:5" ht="33.75" customHeight="1">
-      <c r="A13" s="656"/>
+      <c r="A13" s="650"/>
       <c r="B13" s="555" t="s">
         <v>492</v>
       </c>
@@ -18923,7 +18926,7 @@
       <c r="E13" s="558"/>
     </row>
     <row r="14" spans="1:5" ht="34.5" customHeight="1" thickBot="1">
-      <c r="A14" s="657"/>
+      <c r="A14" s="651"/>
       <c r="B14" s="559" t="s">
         <v>494</v>
       </c>
@@ -18936,7 +18939,7 @@
       <c r="E14" s="561"/>
     </row>
     <row r="15" spans="1:5" ht="56.25">
-      <c r="A15" s="658" t="s">
+      <c r="A15" s="652" t="s">
         <v>496</v>
       </c>
       <c r="B15" s="562" t="s">
@@ -18951,7 +18954,7 @@
       <c r="E15" s="564"/>
     </row>
     <row r="16" spans="1:5" ht="54.75" customHeight="1" thickBot="1">
-      <c r="A16" s="659"/>
+      <c r="A16" s="653"/>
       <c r="B16" s="547" t="s">
         <v>499</v>
       </c>
@@ -18964,7 +18967,7 @@
       <c r="E16" s="566"/>
     </row>
     <row r="17" spans="1:5" ht="33.75" customHeight="1">
-      <c r="A17" s="650" t="s">
+      <c r="A17" s="644" t="s">
         <v>502</v>
       </c>
       <c r="B17" s="567" t="s">
@@ -18979,7 +18982,7 @@
       <c r="E17" s="568"/>
     </row>
     <row r="18" spans="1:5" ht="33.75" customHeight="1" thickBot="1">
-      <c r="A18" s="645"/>
+      <c r="A18" s="654"/>
       <c r="B18" s="569" t="s">
         <v>505</v>
       </c>
@@ -18992,7 +18995,7 @@
       <c r="E18" s="550"/>
     </row>
     <row r="19" spans="1:5" ht="33.75">
-      <c r="A19" s="660" t="s">
+      <c r="A19" s="655" t="s">
         <v>507</v>
       </c>
       <c r="B19" s="567" t="s">
@@ -19007,7 +19010,7 @@
       <c r="E19" s="568"/>
     </row>
     <row r="20" spans="1:5" ht="33.75" customHeight="1">
-      <c r="A20" s="661"/>
+      <c r="A20" s="656"/>
       <c r="B20" s="571" t="s">
         <v>510</v>
       </c>
@@ -19020,7 +19023,7 @@
       <c r="E20" s="573"/>
     </row>
     <row r="21" spans="1:5" ht="54.75" customHeight="1" thickBot="1">
-      <c r="A21" s="662"/>
+      <c r="A21" s="657"/>
       <c r="B21" s="569" t="s">
         <v>512</v>
       </c>
@@ -19033,7 +19036,7 @@
       <c r="E21" s="550"/>
     </row>
     <row r="22" spans="1:5" ht="33.75" customHeight="1">
-      <c r="A22" s="650" t="s">
+      <c r="A22" s="644" t="s">
         <v>514</v>
       </c>
       <c r="B22" s="567" t="s">
@@ -19048,7 +19051,7 @@
       <c r="E22" s="568"/>
     </row>
     <row r="23" spans="1:5" ht="25.5" customHeight="1" thickBot="1">
-      <c r="A23" s="645"/>
+      <c r="A23" s="654"/>
       <c r="B23" s="547" t="s">
         <v>517</v>
       </c>
@@ -19061,7 +19064,7 @@
       <c r="E23" s="566"/>
     </row>
     <row r="24" spans="1:5" ht="33.75">
-      <c r="A24" s="660" t="s">
+      <c r="A24" s="655" t="s">
         <v>519</v>
       </c>
       <c r="B24" s="567" t="s">
@@ -19076,7 +19079,7 @@
       <c r="E24" s="568"/>
     </row>
     <row r="25" spans="1:5" ht="45.75" customHeight="1">
-      <c r="A25" s="661"/>
+      <c r="A25" s="656"/>
       <c r="B25" s="571" t="s">
         <v>522</v>
       </c>
@@ -19089,7 +19092,7 @@
       <c r="E25" s="573"/>
     </row>
     <row r="26" spans="1:5" ht="46.5" customHeight="1">
-      <c r="A26" s="661"/>
+      <c r="A26" s="656"/>
       <c r="B26" s="574" t="s">
         <v>524</v>
       </c>
@@ -19102,7 +19105,7 @@
       <c r="E26" s="573"/>
     </row>
     <row r="27" spans="1:5" ht="22.5">
-      <c r="A27" s="661"/>
+      <c r="A27" s="656"/>
       <c r="B27" s="574" t="s">
         <v>526</v>
       </c>
@@ -19115,7 +19118,7 @@
       <c r="E27" s="573"/>
     </row>
     <row r="28" spans="1:5" ht="23.25" thickBot="1">
-      <c r="A28" s="662"/>
+      <c r="A28" s="657"/>
       <c r="B28" s="575" t="s">
         <v>528</v>
       </c>
@@ -19128,7 +19131,7 @@
       <c r="E28" s="566"/>
     </row>
     <row r="29" spans="1:5" ht="22.5">
-      <c r="A29" s="650" t="s">
+      <c r="A29" s="644" t="s">
         <v>530</v>
       </c>
       <c r="B29" s="576" t="s">
@@ -19143,7 +19146,7 @@
       <c r="E29" s="568"/>
     </row>
     <row r="30" spans="1:5" ht="54.75" customHeight="1">
-      <c r="A30" s="651"/>
+      <c r="A30" s="645"/>
       <c r="B30" s="574" t="s">
         <v>533</v>
       </c>
@@ -19156,7 +19159,7 @@
       <c r="E30" s="573"/>
     </row>
     <row r="31" spans="1:5" ht="34.5" thickBot="1">
-      <c r="A31" s="652"/>
+      <c r="A31" s="646"/>
       <c r="B31" s="575" t="s">
         <v>535</v>
       </c>
@@ -19169,7 +19172,7 @@
       <c r="E31" s="566"/>
     </row>
     <row r="32" spans="1:5" ht="46.5" customHeight="1">
-      <c r="A32" s="650" t="s">
+      <c r="A32" s="644" t="s">
         <v>537</v>
       </c>
       <c r="B32" s="576" t="s">
@@ -19184,7 +19187,7 @@
       <c r="E32" s="568"/>
     </row>
     <row r="33" spans="1:5" ht="66.75" customHeight="1">
-      <c r="A33" s="651"/>
+      <c r="A33" s="645"/>
       <c r="B33" s="574" t="s">
         <v>540</v>
       </c>
@@ -19197,7 +19200,7 @@
       <c r="E33" s="573"/>
     </row>
     <row r="34" spans="1:5" ht="34.5" thickBot="1">
-      <c r="A34" s="652"/>
+      <c r="A34" s="646"/>
       <c r="B34" s="575" t="s">
         <v>541</v>
       </c>
@@ -19285,13 +19288,13 @@
       <c r="E39" s="550"/>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="653" t="s">
+      <c r="A40" s="647" t="s">
         <v>701</v>
       </c>
-      <c r="B40" s="654"/>
-      <c r="C40" s="654"/>
-      <c r="D40" s="654"/>
-      <c r="E40" s="654"/>
+      <c r="B40" s="648"/>
+      <c r="C40" s="648"/>
+      <c r="D40" s="648"/>
+      <c r="E40" s="648"/>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="585"/>
@@ -19988,6 +19991,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
     <mergeCell ref="A29:A31"/>
     <mergeCell ref="A32:A34"/>
     <mergeCell ref="A40:E40"/>
@@ -19997,12 +20006,6 @@
     <mergeCell ref="A19:A21"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="A24:A28"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation showInputMessage="1" showErrorMessage="1" sqref="E10 JA10 SW10 ACS10 AMO10 AWK10 BGG10 BQC10 BZY10 CJU10 CTQ10 DDM10 DNI10 DXE10 EHA10 EQW10 FAS10 FKO10 FUK10 GEG10 GOC10 GXY10 HHU10 HRQ10 IBM10 ILI10 IVE10 JFA10 JOW10 JYS10 KIO10 KSK10 LCG10 LMC10 LVY10 MFU10 MPQ10 MZM10 NJI10 NTE10 ODA10 OMW10 OWS10 PGO10 PQK10 QAG10 QKC10 QTY10 RDU10 RNQ10 RXM10 SHI10 SRE10 TBA10 TKW10 TUS10 UEO10 UOK10 UYG10 VIC10 VRY10 WBU10 WLQ10 WVM10 E65546 JA65546 SW65546 ACS65546 AMO65546 AWK65546 BGG65546 BQC65546 BZY65546 CJU65546 CTQ65546 DDM65546 DNI65546 DXE65546 EHA65546 EQW65546 FAS65546 FKO65546 FUK65546 GEG65546 GOC65546 GXY65546 HHU65546 HRQ65546 IBM65546 ILI65546 IVE65546 JFA65546 JOW65546 JYS65546 KIO65546 KSK65546 LCG65546 LMC65546 LVY65546 MFU65546 MPQ65546 MZM65546 NJI65546 NTE65546 ODA65546 OMW65546 OWS65546 PGO65546 PQK65546 QAG65546 QKC65546 QTY65546 RDU65546 RNQ65546 RXM65546 SHI65546 SRE65546 TBA65546 TKW65546 TUS65546 UEO65546 UOK65546 UYG65546 VIC65546 VRY65546 WBU65546 WLQ65546 WVM65546 E131082 JA131082 SW131082 ACS131082 AMO131082 AWK131082 BGG131082 BQC131082 BZY131082 CJU131082 CTQ131082 DDM131082 DNI131082 DXE131082 EHA131082 EQW131082 FAS131082 FKO131082 FUK131082 GEG131082 GOC131082 GXY131082 HHU131082 HRQ131082 IBM131082 ILI131082 IVE131082 JFA131082 JOW131082 JYS131082 KIO131082 KSK131082 LCG131082 LMC131082 LVY131082 MFU131082 MPQ131082 MZM131082 NJI131082 NTE131082 ODA131082 OMW131082 OWS131082 PGO131082 PQK131082 QAG131082 QKC131082 QTY131082 RDU131082 RNQ131082 RXM131082 SHI131082 SRE131082 TBA131082 TKW131082 TUS131082 UEO131082 UOK131082 UYG131082 VIC131082 VRY131082 WBU131082 WLQ131082 WVM131082 E196618 JA196618 SW196618 ACS196618 AMO196618 AWK196618 BGG196618 BQC196618 BZY196618 CJU196618 CTQ196618 DDM196618 DNI196618 DXE196618 EHA196618 EQW196618 FAS196618 FKO196618 FUK196618 GEG196618 GOC196618 GXY196618 HHU196618 HRQ196618 IBM196618 ILI196618 IVE196618 JFA196618 JOW196618 JYS196618 KIO196618 KSK196618 LCG196618 LMC196618 LVY196618 MFU196618 MPQ196618 MZM196618 NJI196618 NTE196618 ODA196618 OMW196618 OWS196618 PGO196618 PQK196618 QAG196618 QKC196618 QTY196618 RDU196618 RNQ196618 RXM196618 SHI196618 SRE196618 TBA196618 TKW196618 TUS196618 UEO196618 UOK196618 UYG196618 VIC196618 VRY196618 WBU196618 WLQ196618 WVM196618 E262154 JA262154 SW262154 ACS262154 AMO262154 AWK262154 BGG262154 BQC262154 BZY262154 CJU262154 CTQ262154 DDM262154 DNI262154 DXE262154 EHA262154 EQW262154 FAS262154 FKO262154 FUK262154 GEG262154 GOC262154 GXY262154 HHU262154 HRQ262154 IBM262154 ILI262154 IVE262154 JFA262154 JOW262154 JYS262154 KIO262154 KSK262154 LCG262154 LMC262154 LVY262154 MFU262154 MPQ262154 MZM262154 NJI262154 NTE262154 ODA262154 OMW262154 OWS262154 PGO262154 PQK262154 QAG262154 QKC262154 QTY262154 RDU262154 RNQ262154 RXM262154 SHI262154 SRE262154 TBA262154 TKW262154 TUS262154 UEO262154 UOK262154 UYG262154 VIC262154 VRY262154 WBU262154 WLQ262154 WVM262154 E327690 JA327690 SW327690 ACS327690 AMO327690 AWK327690 BGG327690 BQC327690 BZY327690 CJU327690 CTQ327690 DDM327690 DNI327690 DXE327690 EHA327690 EQW327690 FAS327690 FKO327690 FUK327690 GEG327690 GOC327690 GXY327690 HHU327690 HRQ327690 IBM327690 ILI327690 IVE327690 JFA327690 JOW327690 JYS327690 KIO327690 KSK327690 LCG327690 LMC327690 LVY327690 MFU327690 MPQ327690 MZM327690 NJI327690 NTE327690 ODA327690 OMW327690 OWS327690 PGO327690 PQK327690 QAG327690 QKC327690 QTY327690 RDU327690 RNQ327690 RXM327690 SHI327690 SRE327690 TBA327690 TKW327690 TUS327690 UEO327690 UOK327690 UYG327690 VIC327690 VRY327690 WBU327690 WLQ327690 WVM327690 E393226 JA393226 SW393226 ACS393226 AMO393226 AWK393226 BGG393226 BQC393226 BZY393226 CJU393226 CTQ393226 DDM393226 DNI393226 DXE393226 EHA393226 EQW393226 FAS393226 FKO393226 FUK393226 GEG393226 GOC393226 GXY393226 HHU393226 HRQ393226 IBM393226 ILI393226 IVE393226 JFA393226 JOW393226 JYS393226 KIO393226 KSK393226 LCG393226 LMC393226 LVY393226 MFU393226 MPQ393226 MZM393226 NJI393226 NTE393226 ODA393226 OMW393226 OWS393226 PGO393226 PQK393226 QAG393226 QKC393226 QTY393226 RDU393226 RNQ393226 RXM393226 SHI393226 SRE393226 TBA393226 TKW393226 TUS393226 UEO393226 UOK393226 UYG393226 VIC393226 VRY393226 WBU393226 WLQ393226 WVM393226 E458762 JA458762 SW458762 ACS458762 AMO458762 AWK458762 BGG458762 BQC458762 BZY458762 CJU458762 CTQ458762 DDM458762 DNI458762 DXE458762 EHA458762 EQW458762 FAS458762 FKO458762 FUK458762 GEG458762 GOC458762 GXY458762 HHU458762 HRQ458762 IBM458762 ILI458762 IVE458762 JFA458762 JOW458762 JYS458762 KIO458762 KSK458762 LCG458762 LMC458762 LVY458762 MFU458762 MPQ458762 MZM458762 NJI458762 NTE458762 ODA458762 OMW458762 OWS458762 PGO458762 PQK458762 QAG458762 QKC458762 QTY458762 RDU458762 RNQ458762 RXM458762 SHI458762 SRE458762 TBA458762 TKW458762 TUS458762 UEO458762 UOK458762 UYG458762 VIC458762 VRY458762 WBU458762 WLQ458762 WVM458762 E524298 JA524298 SW524298 ACS524298 AMO524298 AWK524298 BGG524298 BQC524298 BZY524298 CJU524298 CTQ524298 DDM524298 DNI524298 DXE524298 EHA524298 EQW524298 FAS524298 FKO524298 FUK524298 GEG524298 GOC524298 GXY524298 HHU524298 HRQ524298 IBM524298 ILI524298 IVE524298 JFA524298 JOW524298 JYS524298 KIO524298 KSK524298 LCG524298 LMC524298 LVY524298 MFU524298 MPQ524298 MZM524298 NJI524298 NTE524298 ODA524298 OMW524298 OWS524298 PGO524298 PQK524298 QAG524298 QKC524298 QTY524298 RDU524298 RNQ524298 RXM524298 SHI524298 SRE524298 TBA524298 TKW524298 TUS524298 UEO524298 UOK524298 UYG524298 VIC524298 VRY524298 WBU524298 WLQ524298 WVM524298 E589834 JA589834 SW589834 ACS589834 AMO589834 AWK589834 BGG589834 BQC589834 BZY589834 CJU589834 CTQ589834 DDM589834 DNI589834 DXE589834 EHA589834 EQW589834 FAS589834 FKO589834 FUK589834 GEG589834 GOC589834 GXY589834 HHU589834 HRQ589834 IBM589834 ILI589834 IVE589834 JFA589834 JOW589834 JYS589834 KIO589834 KSK589834 LCG589834 LMC589834 LVY589834 MFU589834 MPQ589834 MZM589834 NJI589834 NTE589834 ODA589834 OMW589834 OWS589834 PGO589834 PQK589834 QAG589834 QKC589834 QTY589834 RDU589834 RNQ589834 RXM589834 SHI589834 SRE589834 TBA589834 TKW589834 TUS589834 UEO589834 UOK589834 UYG589834 VIC589834 VRY589834 WBU589834 WLQ589834 WVM589834 E655370 JA655370 SW655370 ACS655370 AMO655370 AWK655370 BGG655370 BQC655370 BZY655370 CJU655370 CTQ655370 DDM655370 DNI655370 DXE655370 EHA655370 EQW655370 FAS655370 FKO655370 FUK655370 GEG655370 GOC655370 GXY655370 HHU655370 HRQ655370 IBM655370 ILI655370 IVE655370 JFA655370 JOW655370 JYS655370 KIO655370 KSK655370 LCG655370 LMC655370 LVY655370 MFU655370 MPQ655370 MZM655370 NJI655370 NTE655370 ODA655370 OMW655370 OWS655370 PGO655370 PQK655370 QAG655370 QKC655370 QTY655370 RDU655370 RNQ655370 RXM655370 SHI655370 SRE655370 TBA655370 TKW655370 TUS655370 UEO655370 UOK655370 UYG655370 VIC655370 VRY655370 WBU655370 WLQ655370 WVM655370 E720906 JA720906 SW720906 ACS720906 AMO720906 AWK720906 BGG720906 BQC720906 BZY720906 CJU720906 CTQ720906 DDM720906 DNI720906 DXE720906 EHA720906 EQW720906 FAS720906 FKO720906 FUK720906 GEG720906 GOC720906 GXY720906 HHU720906 HRQ720906 IBM720906 ILI720906 IVE720906 JFA720906 JOW720906 JYS720906 KIO720906 KSK720906 LCG720906 LMC720906 LVY720906 MFU720906 MPQ720906 MZM720906 NJI720906 NTE720906 ODA720906 OMW720906 OWS720906 PGO720906 PQK720906 QAG720906 QKC720906 QTY720906 RDU720906 RNQ720906 RXM720906 SHI720906 SRE720906 TBA720906 TKW720906 TUS720906 UEO720906 UOK720906 UYG720906 VIC720906 VRY720906 WBU720906 WLQ720906 WVM720906 E786442 JA786442 SW786442 ACS786442 AMO786442 AWK786442 BGG786442 BQC786442 BZY786442 CJU786442 CTQ786442 DDM786442 DNI786442 DXE786442 EHA786442 EQW786442 FAS786442 FKO786442 FUK786442 GEG786442 GOC786442 GXY786442 HHU786442 HRQ786442 IBM786442 ILI786442 IVE786442 JFA786442 JOW786442 JYS786442 KIO786442 KSK786442 LCG786442 LMC786442 LVY786442 MFU786442 MPQ786442 MZM786442 NJI786442 NTE786442 ODA786442 OMW786442 OWS786442 PGO786442 PQK786442 QAG786442 QKC786442 QTY786442 RDU786442 RNQ786442 RXM786442 SHI786442 SRE786442 TBA786442 TKW786442 TUS786442 UEO786442 UOK786442 UYG786442 VIC786442 VRY786442 WBU786442 WLQ786442 WVM786442 E851978 JA851978 SW851978 ACS851978 AMO851978 AWK851978 BGG851978 BQC851978 BZY851978 CJU851978 CTQ851978 DDM851978 DNI851978 DXE851978 EHA851978 EQW851978 FAS851978 FKO851978 FUK851978 GEG851978 GOC851978 GXY851978 HHU851978 HRQ851978 IBM851978 ILI851978 IVE851978 JFA851978 JOW851978 JYS851978 KIO851978 KSK851978 LCG851978 LMC851978 LVY851978 MFU851978 MPQ851978 MZM851978 NJI851978 NTE851978 ODA851978 OMW851978 OWS851978 PGO851978 PQK851978 QAG851978 QKC851978 QTY851978 RDU851978 RNQ851978 RXM851978 SHI851978 SRE851978 TBA851978 TKW851978 TUS851978 UEO851978 UOK851978 UYG851978 VIC851978 VRY851978 WBU851978 WLQ851978 WVM851978 E917514 JA917514 SW917514 ACS917514 AMO917514 AWK917514 BGG917514 BQC917514 BZY917514 CJU917514 CTQ917514 DDM917514 DNI917514 DXE917514 EHA917514 EQW917514 FAS917514 FKO917514 FUK917514 GEG917514 GOC917514 GXY917514 HHU917514 HRQ917514 IBM917514 ILI917514 IVE917514 JFA917514 JOW917514 JYS917514 KIO917514 KSK917514 LCG917514 LMC917514 LVY917514 MFU917514 MPQ917514 MZM917514 NJI917514 NTE917514 ODA917514 OMW917514 OWS917514 PGO917514 PQK917514 QAG917514 QKC917514 QTY917514 RDU917514 RNQ917514 RXM917514 SHI917514 SRE917514 TBA917514 TKW917514 TUS917514 UEO917514 UOK917514 UYG917514 VIC917514 VRY917514 WBU917514 WLQ917514 WVM917514 E983050 JA983050 SW983050 ACS983050 AMO983050 AWK983050 BGG983050 BQC983050 BZY983050 CJU983050 CTQ983050 DDM983050 DNI983050 DXE983050 EHA983050 EQW983050 FAS983050 FKO983050 FUK983050 GEG983050 GOC983050 GXY983050 HHU983050 HRQ983050 IBM983050 ILI983050 IVE983050 JFA983050 JOW983050 JYS983050 KIO983050 KSK983050 LCG983050 LMC983050 LVY983050 MFU983050 MPQ983050 MZM983050 NJI983050 NTE983050 ODA983050 OMW983050 OWS983050 PGO983050 PQK983050 QAG983050 QKC983050 QTY983050 RDU983050 RNQ983050 RXM983050 SHI983050 SRE983050 TBA983050 TKW983050 TUS983050 UEO983050 UOK983050 UYG983050 VIC983050 VRY983050 WBU983050 WLQ983050 WVM983050"/>
@@ -22015,7 +22018,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR465"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="M362" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="Q386" sqref="Q386"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
@@ -22447,21 +22452,21 @@
       <c r="E10" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="686" t="str">
+      <c r="F10" s="663" t="str">
         <f>IF(R10="","",R10)</f>
         <v/>
       </c>
-      <c r="G10" s="686"/>
+      <c r="G10" s="663"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="K10" s="686" t="str">
+      <c r="K10" s="663" t="str">
         <f>IF(V10="","",V10)</f>
         <v/>
       </c>
-      <c r="L10" s="686"/>
+      <c r="L10" s="663"/>
       <c r="M10" s="42"/>
       <c r="N10" s="5"/>
       <c r="O10" s="13"/>
@@ -22531,21 +22536,21 @@
       <c r="E11" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="688" t="str">
+      <c r="F11" s="664" t="str">
         <f>IF(R11="","",R11)</f>
         <v/>
       </c>
-      <c r="G11" s="688"/>
+      <c r="G11" s="664"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="K11" s="686" t="str">
+      <c r="K11" s="663" t="str">
         <f>IF(V11="","",V11)</f>
         <v/>
       </c>
-      <c r="L11" s="686"/>
+      <c r="L11" s="663"/>
       <c r="M11" s="42"/>
       <c r="N11" s="5"/>
       <c r="O11" s="13"/>
@@ -22615,21 +22620,21 @@
       <c r="E12" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="688" t="str">
+      <c r="F12" s="664" t="str">
         <f>IF(R12="","",R12)</f>
         <v/>
       </c>
-      <c r="G12" s="688"/>
+      <c r="G12" s="664"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="K12" s="687" t="str">
+      <c r="K12" s="665" t="str">
         <f>IF(V12="","",V12)</f>
         <v/>
       </c>
-      <c r="L12" s="687"/>
+      <c r="L12" s="665"/>
       <c r="M12" s="42"/>
       <c r="N12" s="5"/>
       <c r="O12" s="13"/>
@@ -22699,21 +22704,21 @@
       <c r="E13" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="688" t="str">
+      <c r="F13" s="664" t="str">
         <f>IF(R13="","",R13)</f>
         <v/>
       </c>
-      <c r="G13" s="688"/>
+      <c r="G13" s="664"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="K13" s="686" t="str">
+      <c r="K13" s="663" t="str">
         <f>IF(V13="","",V13)</f>
         <v/>
       </c>
-      <c r="L13" s="686"/>
+      <c r="L13" s="663"/>
       <c r="M13" s="42"/>
       <c r="N13" s="5"/>
       <c r="O13" s="13"/>
@@ -22923,21 +22928,21 @@
       <c r="E16" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="F16" s="686" t="str">
+      <c r="F16" s="663" t="str">
         <f>IF(R17="","",R17)</f>
         <v/>
       </c>
-      <c r="G16" s="686"/>
+      <c r="G16" s="663"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="K16" s="687" t="str">
+      <c r="K16" s="665" t="str">
         <f>IF(V17="","",V17)</f>
         <v/>
       </c>
-      <c r="L16" s="687"/>
+      <c r="L16" s="665"/>
       <c r="M16" s="42"/>
       <c r="N16" s="5"/>
       <c r="O16" s="13"/>
@@ -22999,21 +23004,21 @@
       <c r="E17" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="F17" s="686" t="str">
+      <c r="F17" s="663" t="str">
         <f>IF(R18="","",R18)</f>
         <v/>
       </c>
-      <c r="G17" s="686"/>
+      <c r="G17" s="663"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="K17" s="686" t="str">
+      <c r="K17" s="663" t="str">
         <f>IF(V18="","",V18)</f>
         <v/>
       </c>
-      <c r="L17" s="686"/>
+      <c r="L17" s="663"/>
       <c r="M17" s="42"/>
       <c r="N17" s="5"/>
       <c r="O17" s="13"/>
@@ -23083,21 +23088,21 @@
       <c r="E18" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="F18" s="686" t="str">
+      <c r="F18" s="663" t="str">
         <f>IF(R19="","",R19)</f>
         <v/>
       </c>
-      <c r="G18" s="686"/>
+      <c r="G18" s="663"/>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="K18" s="686" t="str">
+      <c r="K18" s="663" t="str">
         <f>IF(V19="","",V19)</f>
         <v/>
       </c>
-      <c r="L18" s="686"/>
+      <c r="L18" s="663"/>
       <c r="M18" s="42"/>
       <c r="N18" s="5"/>
       <c r="O18" s="13"/>
@@ -23301,21 +23306,21 @@
       <c r="E21" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="F21" s="686" t="str">
+      <c r="F21" s="663" t="str">
         <f>IF(R22="","",R22)</f>
         <v/>
       </c>
-      <c r="G21" s="686"/>
+      <c r="G21" s="663"/>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
       <c r="J21" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="K21" s="686" t="str">
+      <c r="K21" s="663" t="str">
         <f>IF(V21="","",V21)</f>
         <v/>
       </c>
-      <c r="L21" s="686"/>
+      <c r="L21" s="663"/>
       <c r="M21" s="42"/>
       <c r="N21" s="5"/>
       <c r="O21" s="13"/>
@@ -23382,19 +23387,19 @@
       <c r="E22" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="F22" s="687" t="str">
+      <c r="F22" s="665" t="str">
         <f>IF(R23="","",R23)</f>
         <v/>
       </c>
-      <c r="G22" s="687"/>
+      <c r="G22" s="665"/>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="41"/>
-      <c r="K22" s="686" t="str">
+      <c r="K22" s="663" t="str">
         <f>IF(V22="","",V22)</f>
         <v/>
       </c>
-      <c r="L22" s="686"/>
+      <c r="L22" s="663"/>
       <c r="M22" s="42"/>
       <c r="N22" s="5"/>
       <c r="O22" s="13"/>
@@ -23469,11 +23474,11 @@
       <c r="J23" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="K23" s="686" t="str">
+      <c r="K23" s="663" t="str">
         <f>IF(V24="","",V24)</f>
         <v/>
       </c>
-      <c r="L23" s="686"/>
+      <c r="L23" s="663"/>
       <c r="M23" s="42"/>
       <c r="N23" s="5"/>
       <c r="O23" s="13"/>
@@ -23538,19 +23543,19 @@
       <c r="E24" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="F24" s="686" t="str">
+      <c r="F24" s="663" t="str">
         <f>IF(R25="","",R25)</f>
         <v/>
       </c>
-      <c r="G24" s="686"/>
+      <c r="G24" s="663"/>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
-      <c r="K24" s="686" t="str">
+      <c r="K24" s="663" t="str">
         <f>IF(V25="","",V25)</f>
         <v/>
       </c>
-      <c r="L24" s="686"/>
+      <c r="L24" s="663"/>
       <c r="M24" s="42"/>
       <c r="N24" s="5"/>
       <c r="O24" s="13"/>
@@ -23617,11 +23622,11 @@
       <c r="E25" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="F25" s="686" t="str">
+      <c r="F25" s="663" t="str">
         <f>IF(R26="","",R26)</f>
         <v/>
       </c>
-      <c r="G25" s="686"/>
+      <c r="G25" s="663"/>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
       <c r="J25" s="47"/>
@@ -23694,11 +23699,11 @@
       <c r="E26" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="F26" s="686" t="str">
+      <c r="F26" s="663" t="str">
         <f>IF(R27="","",R27)</f>
         <v/>
       </c>
-      <c r="G26" s="686"/>
+      <c r="G26" s="663"/>
       <c r="H26" s="5"/>
       <c r="I26" s="45" t="s">
         <v>32</v>
@@ -23780,11 +23785,11 @@
       <c r="J27" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="K27" s="686" t="str">
+      <c r="K27" s="663" t="str">
         <f>IF(V28="","",V28)</f>
         <v/>
       </c>
-      <c r="L27" s="686"/>
+      <c r="L27" s="663"/>
       <c r="M27" s="42"/>
       <c r="N27" s="5"/>
       <c r="O27" s="13"/>
@@ -23845,21 +23850,21 @@
       <c r="E28" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="F28" s="686" t="str">
+      <c r="F28" s="663" t="str">
         <f>IF(R29="","",R29)</f>
         <v/>
       </c>
-      <c r="G28" s="686"/>
+      <c r="G28" s="663"/>
       <c r="H28" s="5"/>
       <c r="I28" s="47"/>
       <c r="J28" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="K28" s="686" t="str">
+      <c r="K28" s="663" t="str">
         <f>IF(V29="","",V29)</f>
         <v/>
       </c>
-      <c r="L28" s="686"/>
+      <c r="L28" s="663"/>
       <c r="M28" s="42"/>
       <c r="N28" s="5"/>
       <c r="O28" s="13"/>
@@ -23926,11 +23931,11 @@
       <c r="E29" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="F29" s="686" t="str">
+      <c r="F29" s="663" t="str">
         <f>IF(R30="","",R30)</f>
         <v/>
       </c>
-      <c r="G29" s="686"/>
+      <c r="G29" s="663"/>
       <c r="H29" s="5"/>
       <c r="I29" s="45" t="s">
         <v>36</v>
@@ -23938,11 +23943,11 @@
       <c r="J29" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="K29" s="686" t="str">
+      <c r="K29" s="663" t="str">
         <f>IF(V32="","",V32)</f>
         <v/>
       </c>
-      <c r="L29" s="686"/>
+      <c r="L29" s="663"/>
       <c r="M29" s="42"/>
       <c r="N29" s="5"/>
       <c r="O29" s="13"/>
@@ -24012,21 +24017,21 @@
       <c r="E30" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="F30" s="686" t="str">
+      <c r="F30" s="663" t="str">
         <f>IF(R31="","",R31)</f>
         <v/>
       </c>
-      <c r="G30" s="686"/>
+      <c r="G30" s="663"/>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
       <c r="J30" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="K30" s="686" t="str">
+      <c r="K30" s="663" t="str">
         <f>IF(V33="","",V33)</f>
         <v/>
       </c>
-      <c r="L30" s="686"/>
+      <c r="L30" s="663"/>
       <c r="M30" s="42"/>
       <c r="N30" s="5"/>
       <c r="O30" s="13"/>
@@ -24368,21 +24373,21 @@
       <c r="C35" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="D35" s="683" t="s">
+      <c r="D35" s="666" t="s">
         <v>42</v>
       </c>
-      <c r="E35" s="683"/>
-      <c r="F35" s="683"/>
-      <c r="G35" s="684" t="s">
+      <c r="E35" s="666"/>
+      <c r="F35" s="666"/>
+      <c r="G35" s="667" t="s">
         <v>43</v>
       </c>
-      <c r="H35" s="684"/>
-      <c r="I35" s="684"/>
-      <c r="J35" s="683" t="s">
+      <c r="H35" s="667"/>
+      <c r="I35" s="667"/>
+      <c r="J35" s="666" t="s">
         <v>44</v>
       </c>
-      <c r="K35" s="683"/>
-      <c r="L35" s="683"/>
+      <c r="K35" s="666"/>
+      <c r="L35" s="666"/>
       <c r="M35" s="42"/>
       <c r="N35" s="5"/>
       <c r="O35" s="53">
@@ -24444,15 +24449,15 @@
       <c r="C36" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="D36" s="683"/>
-      <c r="E36" s="683"/>
-      <c r="F36" s="683"/>
-      <c r="G36" s="684"/>
-      <c r="H36" s="684"/>
-      <c r="I36" s="684"/>
-      <c r="J36" s="683"/>
-      <c r="K36" s="683"/>
-      <c r="L36" s="683"/>
+      <c r="D36" s="666"/>
+      <c r="E36" s="666"/>
+      <c r="F36" s="666"/>
+      <c r="G36" s="667"/>
+      <c r="H36" s="667"/>
+      <c r="I36" s="667"/>
+      <c r="J36" s="666"/>
+      <c r="K36" s="666"/>
+      <c r="L36" s="666"/>
       <c r="M36" s="42"/>
       <c r="N36" s="5"/>
       <c r="O36" s="5"/>
@@ -25117,10 +25122,10 @@
       <c r="I44" s="5"/>
       <c r="J44" s="5"/>
       <c r="K44" s="5"/>
-      <c r="L44" s="685" t="s">
+      <c r="L44" s="668" t="s">
         <v>63</v>
       </c>
-      <c r="M44" s="685"/>
+      <c r="M44" s="668"/>
       <c r="N44" s="5"/>
       <c r="O44" s="13"/>
       <c r="P44" s="5"/>
@@ -28900,21 +28905,21 @@
       <c r="O97" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="P97" s="683" t="s">
+      <c r="P97" s="666" t="s">
         <v>42</v>
       </c>
-      <c r="Q97" s="683"/>
-      <c r="R97" s="683"/>
-      <c r="S97" s="684" t="s">
+      <c r="Q97" s="666"/>
+      <c r="R97" s="666"/>
+      <c r="S97" s="667" t="s">
         <v>43</v>
       </c>
-      <c r="T97" s="684"/>
-      <c r="U97" s="684"/>
-      <c r="V97" s="683" t="s">
+      <c r="T97" s="667"/>
+      <c r="U97" s="667"/>
+      <c r="V97" s="666" t="s">
         <v>44</v>
       </c>
-      <c r="W97" s="683"/>
-      <c r="X97" s="683"/>
+      <c r="W97" s="666"/>
+      <c r="X97" s="666"/>
       <c r="Y97" s="15"/>
       <c r="AA97" s="177"/>
       <c r="AB97" s="177"/>
@@ -28972,15 +28977,15 @@
       <c r="O98" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="P98" s="683"/>
-      <c r="Q98" s="683"/>
-      <c r="R98" s="683"/>
-      <c r="S98" s="684"/>
-      <c r="T98" s="684"/>
-      <c r="U98" s="684"/>
-      <c r="V98" s="683"/>
-      <c r="W98" s="683"/>
-      <c r="X98" s="683"/>
+      <c r="P98" s="666"/>
+      <c r="Q98" s="666"/>
+      <c r="R98" s="666"/>
+      <c r="S98" s="667"/>
+      <c r="T98" s="667"/>
+      <c r="U98" s="667"/>
+      <c r="V98" s="666"/>
+      <c r="W98" s="666"/>
+      <c r="X98" s="666"/>
       <c r="Y98" s="15"/>
       <c r="AA98" s="45" t="s">
         <v>394</v>
@@ -29596,21 +29601,21 @@
       <c r="O105" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="P105" s="683" t="s">
+      <c r="P105" s="666" t="s">
         <v>42</v>
       </c>
-      <c r="Q105" s="683"/>
-      <c r="R105" s="683"/>
-      <c r="S105" s="684" t="s">
+      <c r="Q105" s="666"/>
+      <c r="R105" s="666"/>
+      <c r="S105" s="667" t="s">
         <v>43</v>
       </c>
-      <c r="T105" s="684"/>
-      <c r="U105" s="684"/>
-      <c r="V105" s="683" t="s">
+      <c r="T105" s="667"/>
+      <c r="U105" s="667"/>
+      <c r="V105" s="666" t="s">
         <v>44</v>
       </c>
-      <c r="W105" s="683"/>
-      <c r="X105" s="683"/>
+      <c r="W105" s="666"/>
+      <c r="X105" s="666"/>
       <c r="Y105" s="15"/>
       <c r="AA105" s="41" t="s">
         <v>274</v>
@@ -29668,15 +29673,15 @@
       <c r="O106" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="P106" s="683"/>
-      <c r="Q106" s="683"/>
-      <c r="R106" s="683"/>
-      <c r="S106" s="684"/>
-      <c r="T106" s="684"/>
-      <c r="U106" s="684"/>
-      <c r="V106" s="683"/>
-      <c r="W106" s="683"/>
-      <c r="X106" s="683"/>
+      <c r="P106" s="666"/>
+      <c r="Q106" s="666"/>
+      <c r="R106" s="666"/>
+      <c r="S106" s="667"/>
+      <c r="T106" s="667"/>
+      <c r="U106" s="667"/>
+      <c r="V106" s="666"/>
+      <c r="W106" s="666"/>
+      <c r="X106" s="666"/>
       <c r="Y106" s="15"/>
       <c r="AA106" s="41" t="s">
         <v>277</v>
@@ -32241,17 +32246,17 @@
       <c r="M150" s="42"/>
       <c r="N150" s="5"/>
       <c r="O150" s="13"/>
-      <c r="P150" s="672" t="s">
+      <c r="P150" s="669" t="s">
         <v>187</v>
       </c>
-      <c r="Q150" s="672"/>
-      <c r="R150" s="672"/>
-      <c r="S150" s="672"/>
+      <c r="Q150" s="669"/>
+      <c r="R150" s="669"/>
+      <c r="S150" s="669"/>
       <c r="T150" s="133"/>
-      <c r="U150" s="672" t="s">
+      <c r="U150" s="669" t="s">
         <v>188</v>
       </c>
-      <c r="V150" s="672"/>
+      <c r="V150" s="669"/>
       <c r="W150" s="5"/>
       <c r="X150" s="5"/>
       <c r="Y150" s="15"/>
@@ -32300,10 +32305,10 @@
         <v>192</v>
       </c>
       <c r="T151" s="133"/>
-      <c r="U151" s="681" t="s">
+      <c r="U151" s="670" t="s">
         <v>193</v>
       </c>
-      <c r="V151" s="681"/>
+      <c r="V151" s="670"/>
       <c r="W151" s="5"/>
       <c r="X151" s="5"/>
       <c r="Y151" s="15"/>
@@ -32343,11 +32348,11 @@
       <c r="R152" s="136"/>
       <c r="S152" s="137"/>
       <c r="T152" s="133"/>
-      <c r="U152" s="682" t="str">
+      <c r="U152" s="671" t="str">
         <f>IF(OR(R149=2,R149=3),"NA",IF(OR(P152="",Q152="",R152="",S152=""),"",AVERAGE(P152:S152)))</f>
         <v/>
       </c>
-      <c r="V152" s="682"/>
+      <c r="V152" s="671"/>
       <c r="W152" s="5"/>
       <c r="X152" s="41" t="s">
         <v>180</v>
@@ -32493,18 +32498,18 @@
       <c r="M156" s="141"/>
       <c r="N156" s="5"/>
       <c r="O156" s="13"/>
-      <c r="P156" s="675" t="s">
+      <c r="P156" s="672" t="s">
         <v>196</v>
       </c>
-      <c r="Q156" s="679" t="s">
+      <c r="Q156" s="673" t="s">
         <v>197</v>
       </c>
-      <c r="R156" s="679"/>
-      <c r="S156" s="679"/>
+      <c r="R156" s="673"/>
+      <c r="S156" s="673"/>
       <c r="T156" s="142" t="s">
         <v>197</v>
       </c>
-      <c r="U156" s="677" t="s">
+      <c r="U156" s="674" t="s">
         <v>198</v>
       </c>
       <c r="V156" s="77"/>
@@ -32532,7 +32537,7 @@
       <c r="M157" s="42"/>
       <c r="N157" s="5"/>
       <c r="O157" s="13"/>
-      <c r="P157" s="675" t="s">
+      <c r="P157" s="672" t="s">
         <v>196</v>
       </c>
       <c r="Q157" s="142" t="s">
@@ -32547,7 +32552,7 @@
       <c r="T157" s="142" t="s">
         <v>202</v>
       </c>
-      <c r="U157" s="677" t="s">
+      <c r="U157" s="674" t="s">
         <v>196</v>
       </c>
       <c r="V157" s="77"/>
@@ -32897,14 +32902,14 @@
       <c r="M164" s="42"/>
       <c r="N164" s="5"/>
       <c r="O164" s="156"/>
-      <c r="P164" s="675" t="s">
+      <c r="P164" s="672" t="s">
         <v>209</v>
       </c>
-      <c r="Q164" s="675"/>
-      <c r="R164" s="675"/>
-      <c r="S164" s="675"/>
-      <c r="T164" s="675"/>
-      <c r="U164" s="675"/>
+      <c r="Q164" s="672"/>
+      <c r="R164" s="672"/>
+      <c r="S164" s="672"/>
+      <c r="T164" s="672"/>
+      <c r="U164" s="672"/>
       <c r="V164" s="77"/>
       <c r="W164" s="77"/>
       <c r="X164" s="77"/>
@@ -32948,18 +32953,18 @@
       <c r="M165" s="42"/>
       <c r="N165" s="5"/>
       <c r="O165" s="156"/>
-      <c r="P165" s="675" t="s">
+      <c r="P165" s="672" t="s">
         <v>196</v>
       </c>
-      <c r="Q165" s="676" t="s">
+      <c r="Q165" s="675" t="s">
         <v>197</v>
       </c>
-      <c r="R165" s="676"/>
-      <c r="S165" s="676"/>
+      <c r="R165" s="675"/>
+      <c r="S165" s="675"/>
       <c r="T165" s="143" t="s">
         <v>197</v>
       </c>
-      <c r="U165" s="677" t="s">
+      <c r="U165" s="674" t="s">
         <v>198</v>
       </c>
       <c r="V165" s="77"/>
@@ -32989,7 +32994,7 @@
       <c r="M166" s="42"/>
       <c r="N166" s="5"/>
       <c r="O166" s="156"/>
-      <c r="P166" s="675" t="s">
+      <c r="P166" s="672" t="s">
         <v>196</v>
       </c>
       <c r="Q166" s="143" t="s">
@@ -33004,7 +33009,7 @@
       <c r="T166" s="143" t="s">
         <v>202</v>
       </c>
-      <c r="U166" s="677" t="s">
+      <c r="U166" s="674" t="s">
         <v>196</v>
       </c>
       <c r="V166" s="77"/>
@@ -33277,17 +33282,17 @@
       </c>
       <c r="B172" s="39"/>
       <c r="C172" s="5"/>
-      <c r="D172" s="672" t="s">
+      <c r="D172" s="669" t="s">
         <v>187</v>
       </c>
-      <c r="E172" s="672"/>
-      <c r="F172" s="672"/>
-      <c r="G172" s="672"/>
+      <c r="E172" s="669"/>
+      <c r="F172" s="669"/>
+      <c r="G172" s="669"/>
       <c r="H172" s="133"/>
-      <c r="I172" s="672" t="s">
+      <c r="I172" s="669" t="s">
         <v>188</v>
       </c>
-      <c r="J172" s="672"/>
+      <c r="J172" s="669"/>
       <c r="K172" s="5"/>
       <c r="L172" s="5"/>
       <c r="M172" s="42"/>
@@ -33343,10 +33348,10 @@
         <v>192</v>
       </c>
       <c r="H173" s="133"/>
-      <c r="I173" s="681" t="s">
+      <c r="I173" s="670" t="s">
         <v>193</v>
       </c>
-      <c r="J173" s="681"/>
+      <c r="J173" s="670"/>
       <c r="K173" s="5"/>
       <c r="L173" s="5"/>
       <c r="M173" s="42"/>
@@ -33390,11 +33395,11 @@
         <v/>
       </c>
       <c r="H174" s="133"/>
-      <c r="I174" s="674" t="str">
+      <c r="I174" s="677" t="str">
         <f>IF(U152="","",U152)</f>
         <v/>
       </c>
-      <c r="J174" s="674"/>
+      <c r="J174" s="677"/>
       <c r="K174" s="5"/>
       <c r="L174" s="41" t="s">
         <v>180</v>
@@ -33537,18 +33542,18 @@
       <c r="M178" s="42"/>
       <c r="N178" s="5"/>
       <c r="O178" s="13"/>
-      <c r="P178" s="675" t="s">
+      <c r="P178" s="672" t="s">
         <v>196</v>
       </c>
-      <c r="Q178" s="676" t="s">
+      <c r="Q178" s="675" t="s">
         <v>197</v>
       </c>
-      <c r="R178" s="676"/>
-      <c r="S178" s="676"/>
+      <c r="R178" s="675"/>
+      <c r="S178" s="675"/>
       <c r="T178" s="143" t="s">
         <v>196</v>
       </c>
-      <c r="U178" s="677" t="s">
+      <c r="U178" s="674" t="s">
         <v>198</v>
       </c>
       <c r="V178" s="77"/>
@@ -33579,7 +33584,7 @@
       <c r="M179" s="42"/>
       <c r="N179" s="5"/>
       <c r="O179" s="13"/>
-      <c r="P179" s="675" t="s">
+      <c r="P179" s="672" t="s">
         <v>196</v>
       </c>
       <c r="Q179" s="143" t="s">
@@ -33594,7 +33599,7 @@
       <c r="T179" s="143" t="s">
         <v>202</v>
       </c>
-      <c r="U179" s="677" t="s">
+      <c r="U179" s="674" t="s">
         <v>196</v>
       </c>
       <c r="V179" s="77"/>
@@ -33608,18 +33613,18 @@
       </c>
       <c r="B180" s="39"/>
       <c r="C180" s="47"/>
-      <c r="D180" s="675" t="s">
+      <c r="D180" s="672" t="s">
         <v>196</v>
       </c>
-      <c r="E180" s="679" t="s">
+      <c r="E180" s="673" t="s">
         <v>197</v>
       </c>
-      <c r="F180" s="679"/>
-      <c r="G180" s="679"/>
+      <c r="F180" s="673"/>
+      <c r="G180" s="673"/>
       <c r="H180" s="142" t="s">
         <v>196</v>
       </c>
-      <c r="I180" s="680" t="s">
+      <c r="I180" s="679" t="s">
         <v>198</v>
       </c>
       <c r="J180" s="77"/>
@@ -33647,7 +33652,7 @@
       </c>
       <c r="B181" s="39"/>
       <c r="C181" s="47"/>
-      <c r="D181" s="675" t="s">
+      <c r="D181" s="672" t="s">
         <v>196</v>
       </c>
       <c r="E181" s="142" t="s">
@@ -33662,7 +33667,7 @@
       <c r="H181" s="142" t="s">
         <v>202</v>
       </c>
-      <c r="I181" s="680" t="s">
+      <c r="I181" s="679" t="s">
         <v>202</v>
       </c>
       <c r="J181" s="77"/>
@@ -33975,14 +33980,14 @@
       <c r="M187" s="42"/>
       <c r="N187" s="5"/>
       <c r="O187" s="156"/>
-      <c r="P187" s="663" t="s">
+      <c r="P187" s="680" t="s">
         <v>209</v>
       </c>
-      <c r="Q187" s="663"/>
-      <c r="R187" s="663"/>
-      <c r="S187" s="663"/>
-      <c r="T187" s="663"/>
-      <c r="U187" s="663"/>
+      <c r="Q187" s="680"/>
+      <c r="R187" s="680"/>
+      <c r="S187" s="680"/>
+      <c r="T187" s="680"/>
+      <c r="U187" s="680"/>
       <c r="V187" s="77"/>
       <c r="W187" s="77"/>
       <c r="X187" s="77"/>
@@ -34026,18 +34031,18 @@
       <c r="M188" s="42"/>
       <c r="N188" s="5"/>
       <c r="O188" s="156"/>
-      <c r="P188" s="675" t="s">
+      <c r="P188" s="672" t="s">
         <v>196</v>
       </c>
-      <c r="Q188" s="676" t="s">
+      <c r="Q188" s="675" t="s">
         <v>197</v>
       </c>
-      <c r="R188" s="676"/>
-      <c r="S188" s="676"/>
+      <c r="R188" s="675"/>
+      <c r="S188" s="675"/>
       <c r="T188" s="143" t="s">
         <v>196</v>
       </c>
-      <c r="U188" s="677" t="s">
+      <c r="U188" s="674" t="s">
         <v>198</v>
       </c>
       <c r="V188" s="77"/>
@@ -34065,7 +34070,7 @@
       <c r="M189" s="78"/>
       <c r="N189" s="5"/>
       <c r="O189" s="156"/>
-      <c r="P189" s="675" t="s">
+      <c r="P189" s="672" t="s">
         <v>196</v>
       </c>
       <c r="Q189" s="143" t="s">
@@ -34080,7 +34085,7 @@
       <c r="T189" s="143" t="s">
         <v>202</v>
       </c>
-      <c r="U189" s="677"/>
+      <c r="U189" s="674"/>
       <c r="V189" s="77"/>
       <c r="W189" s="77"/>
       <c r="X189" s="77"/>
@@ -36893,11 +36898,11 @@
       <c r="U246" s="47"/>
       <c r="V246" s="5"/>
       <c r="W246" s="5"/>
-      <c r="X246" s="673" t="str">
+      <c r="X246" s="676" t="str">
         <f>IF($O$34=1,AB246,Z246)</f>
         <v>Selenia Dimensions</v>
       </c>
-      <c r="Y246" s="673"/>
+      <c r="Y246" s="676"/>
       <c r="Z246" s="435" t="s">
         <v>602</v>
       </c>
@@ -37582,21 +37587,21 @@
       </c>
       <c r="B259" s="39"/>
       <c r="C259" s="5"/>
-      <c r="D259" s="668" t="s">
+      <c r="D259" s="683" t="s">
         <v>263</v>
       </c>
-      <c r="E259" s="668"/>
+      <c r="E259" s="683"/>
       <c r="F259" s="47"/>
-      <c r="G259" s="668" t="s">
+      <c r="G259" s="683" t="s">
         <v>264</v>
       </c>
-      <c r="H259" s="668"/>
+      <c r="H259" s="683"/>
       <c r="I259" s="5"/>
       <c r="J259" s="47"/>
-      <c r="K259" s="669" t="s">
+      <c r="K259" s="684" t="s">
         <v>265</v>
       </c>
-      <c r="L259" s="669"/>
+      <c r="L259" s="684"/>
       <c r="M259" s="78"/>
       <c r="N259" s="5"/>
       <c r="O259" s="110" t="s">
@@ -39874,14 +39879,14 @@
       <c r="B305" s="175"/>
       <c r="C305" s="77"/>
       <c r="D305" s="77"/>
-      <c r="E305" s="670" t="str">
+      <c r="E305" s="685" t="str">
         <f>O294&amp;" "&amp;P295&amp;" "&amp;Q295</f>
         <v xml:space="preserve">Combo Mode 2D Target/Filter: </v>
       </c>
-      <c r="F305" s="670"/>
-      <c r="G305" s="670"/>
-      <c r="H305" s="670"/>
-      <c r="I305" s="670"/>
+      <c r="F305" s="685"/>
+      <c r="G305" s="685"/>
+      <c r="H305" s="685"/>
+      <c r="I305" s="685"/>
       <c r="J305" s="77"/>
       <c r="K305" s="77"/>
       <c r="L305" s="77"/>
@@ -40442,14 +40447,14 @@
       <c r="B316" s="175"/>
       <c r="C316" s="77"/>
       <c r="D316" s="77"/>
-      <c r="E316" s="671" t="str">
+      <c r="E316" s="686" t="str">
         <f>O306&amp;" "&amp;P307&amp;" "&amp;Q307</f>
         <v xml:space="preserve">Combo Mode 3D Target/Filter: </v>
       </c>
-      <c r="F316" s="671"/>
-      <c r="G316" s="671"/>
-      <c r="H316" s="671"/>
-      <c r="I316" s="671"/>
+      <c r="F316" s="686"/>
+      <c r="G316" s="686"/>
+      <c r="H316" s="686"/>
+      <c r="I316" s="686"/>
       <c r="J316" s="77"/>
       <c r="K316" s="77"/>
       <c r="L316" s="77"/>
@@ -40729,10 +40734,10 @@
       <c r="S321" s="41" t="s">
         <v>305</v>
       </c>
-      <c r="T321" s="665">
+      <c r="T321" s="687">
         <v>43014</v>
       </c>
-      <c r="U321" s="665"/>
+      <c r="U321" s="687"/>
       <c r="V321" s="5"/>
       <c r="W321" s="5"/>
       <c r="X321" s="5"/>
@@ -40786,10 +40791,10 @@
       <c r="S322" s="41" t="s">
         <v>307</v>
       </c>
-      <c r="T322" s="665">
+      <c r="T322" s="687">
         <v>43744</v>
       </c>
-      <c r="U322" s="665"/>
+      <c r="U322" s="687"/>
       <c r="V322" s="5"/>
       <c r="W322" s="5"/>
       <c r="X322" s="5"/>
@@ -40885,13 +40890,13 @@
       <c r="Q324" s="5"/>
       <c r="R324" s="5"/>
       <c r="S324" s="5"/>
-      <c r="T324" s="663" t="s">
+      <c r="T324" s="680" t="s">
         <v>308</v>
       </c>
-      <c r="U324" s="663"/>
-      <c r="V324" s="663"/>
-      <c r="W324" s="663"/>
-      <c r="X324" s="663"/>
+      <c r="U324" s="680"/>
+      <c r="V324" s="680"/>
+      <c r="W324" s="680"/>
+      <c r="X324" s="680"/>
       <c r="Y324" s="15"/>
     </row>
     <row r="325" spans="1:25">
@@ -41496,13 +41501,13 @@
       <c r="Q335" s="5"/>
       <c r="R335" s="5"/>
       <c r="S335" s="41"/>
-      <c r="T335" s="663" t="s">
+      <c r="T335" s="680" t="s">
         <v>308</v>
       </c>
-      <c r="U335" s="663"/>
-      <c r="V335" s="663"/>
-      <c r="W335" s="663"/>
-      <c r="X335" s="663"/>
+      <c r="U335" s="680"/>
+      <c r="V335" s="680"/>
+      <c r="W335" s="680"/>
+      <c r="X335" s="680"/>
       <c r="Y335" s="15"/>
     </row>
     <row r="336" spans="1:25">
@@ -41840,15 +41845,15 @@
         <v>50</v>
       </c>
       <c r="T341" s="209" t="str">
-        <f>IF(AM90="","",AM90)</f>
+        <f t="shared" ref="T341:V342" si="65">IF(AM90="","",AM90)</f>
         <v/>
       </c>
       <c r="U341" s="211" t="str">
-        <f>IF(AN90="","",AN90)</f>
+        <f t="shared" si="65"/>
         <v/>
       </c>
       <c r="V341" s="209" t="str">
-        <f>IF(AO90="","",AO90)</f>
+        <f t="shared" si="65"/>
         <v/>
       </c>
       <c r="W341" s="237" t="str">
@@ -41901,15 +41906,15 @@
         <v>50</v>
       </c>
       <c r="T342" s="209" t="str">
-        <f>IF(AM91="","",AM91)</f>
+        <f t="shared" si="65"/>
         <v/>
       </c>
       <c r="U342" s="211" t="str">
-        <f>IF(AN91="","",AN91)</f>
+        <f t="shared" si="65"/>
         <v/>
       </c>
       <c r="V342" s="209" t="str">
-        <f>IF(AO91="","",AO91)</f>
+        <f t="shared" si="65"/>
         <v/>
       </c>
       <c r="W342" s="237" t="str">
@@ -41940,11 +41945,11 @@
       <c r="H343" s="279" t="s">
         <v>305</v>
       </c>
-      <c r="I343" s="666">
+      <c r="I343" s="681">
         <f>IF(T321="","",T321)</f>
         <v>43014</v>
       </c>
-      <c r="J343" s="666"/>
+      <c r="J343" s="681"/>
       <c r="K343" s="33"/>
       <c r="L343" s="33"/>
       <c r="M343" s="35"/>
@@ -41983,11 +41988,11 @@
       <c r="H344" s="228" t="s">
         <v>307</v>
       </c>
-      <c r="I344" s="667">
+      <c r="I344" s="682">
         <f>IF(T322="","",T322)</f>
         <v>43744</v>
       </c>
-      <c r="J344" s="667"/>
+      <c r="J344" s="682"/>
       <c r="K344" s="47"/>
       <c r="L344" s="5"/>
       <c r="M344" s="42"/>
@@ -42028,13 +42033,13 @@
       <c r="Q345" s="5"/>
       <c r="R345" s="5"/>
       <c r="S345" s="41"/>
-      <c r="T345" s="663" t="s">
+      <c r="T345" s="680" t="s">
         <v>308</v>
       </c>
-      <c r="U345" s="663"/>
-      <c r="V345" s="663"/>
-      <c r="W345" s="663"/>
-      <c r="X345" s="663"/>
+      <c r="U345" s="680"/>
+      <c r="V345" s="680"/>
+      <c r="W345" s="680"/>
+      <c r="X345" s="680"/>
       <c r="Y345" s="15"/>
     </row>
     <row r="346" spans="1:25">
@@ -42389,28 +42394,28 @@
       </c>
       <c r="B351" s="39"/>
       <c r="C351" s="121">
-        <f t="shared" ref="C351:C357" si="65">IF(R326="","",R326)</f>
+        <f t="shared" ref="C351:C357" si="66">IF(R326="","",R326)</f>
         <v>24</v>
       </c>
       <c r="D351" s="209" t="str">
-        <f t="shared" ref="D351:D357" si="66">IF(T326="","",T326)</f>
+        <f t="shared" ref="D351:D357" si="67">IF(T326="","",T326)</f>
         <v/>
       </c>
       <c r="E351" s="286" t="str">
-        <f t="shared" ref="E351:E357" si="67">IF(OR(C351="",D351=""),"",IF(AND(C351&gt;0,D351&gt;0),(D351-C351)/C351,""))</f>
+        <f t="shared" ref="E351:E357" si="68">IF(OR(C351="",D351=""),"",IF(AND(C351&gt;0,D351&gt;0),(D351-C351)/C351,""))</f>
         <v/>
       </c>
       <c r="F351" s="5"/>
       <c r="G351" s="121">
-        <f t="shared" ref="G351:G356" si="68">IF(R337="","",R337)</f>
+        <f t="shared" ref="G351:G356" si="69">IF(R337="","",R337)</f>
         <v>28</v>
       </c>
       <c r="H351" s="209" t="str">
-        <f t="shared" ref="H351:H356" si="69">IF(T337="","",T337)</f>
+        <f t="shared" ref="H351:H356" si="70">IF(T337="","",T337)</f>
         <v/>
       </c>
       <c r="I351" s="286" t="str">
-        <f t="shared" ref="I351:I356" si="70">IF(OR(G351="",H351=""),"",IF(AND(G351&gt;0,H351&gt;0),(H351-G351)/G351,""))</f>
+        <f t="shared" ref="I351:I356" si="71">IF(OR(G351="",H351=""),"",IF(AND(G351&gt;0,H351&gt;0),(H351-G351)/G351,""))</f>
         <v/>
       </c>
       <c r="J351" s="77"/>
@@ -42472,28 +42477,28 @@
       </c>
       <c r="B352" s="39"/>
       <c r="C352" s="121">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>25</v>
       </c>
       <c r="D352" s="209" t="str">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v/>
       </c>
       <c r="E352" s="286" t="str">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v/>
       </c>
       <c r="F352" s="5"/>
       <c r="G352" s="121">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>30</v>
       </c>
       <c r="H352" s="209" t="str">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v/>
       </c>
       <c r="I352" s="286" t="str">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v/>
       </c>
       <c r="J352" s="77"/>
@@ -42532,28 +42537,28 @@
       </c>
       <c r="B353" s="39"/>
       <c r="C353" s="121">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>26</v>
       </c>
       <c r="D353" s="209" t="str">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v/>
       </c>
       <c r="E353" s="286" t="str">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v/>
       </c>
       <c r="F353" s="5"/>
       <c r="G353" s="121">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>32</v>
       </c>
       <c r="H353" s="209" t="str">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v/>
       </c>
       <c r="I353" s="286" t="str">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v/>
       </c>
       <c r="J353" s="77"/>
@@ -42588,28 +42593,28 @@
       </c>
       <c r="B354" s="39"/>
       <c r="C354" s="121">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>28</v>
       </c>
       <c r="D354" s="209" t="str">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v/>
       </c>
       <c r="E354" s="286" t="str">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v/>
       </c>
       <c r="F354" s="5"/>
       <c r="G354" s="121">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>34</v>
       </c>
       <c r="H354" s="209" t="str">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v/>
       </c>
       <c r="I354" s="286" t="str">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v/>
       </c>
       <c r="J354" s="77"/>
@@ -42646,28 +42651,28 @@
       </c>
       <c r="B355" s="39"/>
       <c r="C355" s="121">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>30</v>
       </c>
       <c r="D355" s="209" t="str">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v/>
       </c>
       <c r="E355" s="286" t="str">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v/>
       </c>
       <c r="F355" s="5"/>
       <c r="G355" s="121">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>36</v>
       </c>
       <c r="H355" s="209" t="str">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v/>
       </c>
       <c r="I355" s="286" t="str">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v/>
       </c>
       <c r="J355" s="77"/>
@@ -42702,28 +42707,28 @@
       </c>
       <c r="B356" s="39"/>
       <c r="C356" s="121">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>32</v>
       </c>
       <c r="D356" s="209" t="str">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v/>
       </c>
       <c r="E356" s="286" t="str">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v/>
       </c>
       <c r="F356" s="5"/>
       <c r="G356" s="121">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>38</v>
       </c>
       <c r="H356" s="209" t="str">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v/>
       </c>
       <c r="I356" s="286" t="str">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v/>
       </c>
       <c r="J356" s="77"/>
@@ -42736,13 +42741,13 @@
       <c r="Q356" s="5"/>
       <c r="R356" s="5"/>
       <c r="S356" s="41"/>
-      <c r="T356" s="663" t="s">
+      <c r="T356" s="680" t="s">
         <v>308</v>
       </c>
-      <c r="U356" s="663"/>
-      <c r="V356" s="663"/>
-      <c r="W356" s="663"/>
-      <c r="X356" s="663"/>
+      <c r="U356" s="680"/>
+      <c r="V356" s="680"/>
+      <c r="W356" s="680"/>
+      <c r="X356" s="680"/>
       <c r="Y356" s="15"/>
     </row>
     <row r="357" spans="1:25" ht="16.5" thickBot="1">
@@ -42751,15 +42756,15 @@
       </c>
       <c r="B357" s="39"/>
       <c r="C357" s="121">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>34</v>
       </c>
       <c r="D357" s="209" t="str">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v/>
       </c>
       <c r="E357" s="286" t="str">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v/>
       </c>
       <c r="F357" s="5"/>
@@ -42843,11 +42848,11 @@
         <v/>
       </c>
       <c r="R358" s="121">
-        <f t="shared" ref="R358:S361" si="71">IF(AH28="","",AH28)</f>
+        <f t="shared" ref="R358:S361" si="72">IF(AH28="","",AH28)</f>
         <v>28</v>
       </c>
       <c r="S358" s="121">
-        <f t="shared" si="71"/>
+        <f t="shared" si="72"/>
         <v>50</v>
       </c>
       <c r="T358" s="209" t="str">
@@ -42855,11 +42860,11 @@
         <v/>
       </c>
       <c r="U358" s="211" t="str">
-        <f t="shared" ref="U358:V361" si="72">IF(AN28="","",AN28)</f>
+        <f t="shared" ref="U358:V361" si="73">IF(AN28="","",AN28)</f>
         <v/>
       </c>
       <c r="V358" s="209" t="str">
-        <f t="shared" si="72"/>
+        <f t="shared" si="73"/>
         <v/>
       </c>
       <c r="W358" s="237" t="str">
@@ -42899,23 +42904,23 @@
         <v/>
       </c>
       <c r="R359" s="121">
-        <f t="shared" si="71"/>
+        <f t="shared" si="72"/>
         <v>28</v>
       </c>
       <c r="S359" s="121">
-        <f t="shared" si="71"/>
+        <f t="shared" si="72"/>
         <v>50</v>
       </c>
       <c r="T359" s="209" t="str">
-        <f t="shared" ref="T359:T361" si="73">IF(AM29="","",AM29)</f>
+        <f t="shared" ref="T359:T361" si="74">IF(AM29="","",AM29)</f>
         <v/>
       </c>
       <c r="U359" s="211" t="str">
-        <f t="shared" si="72"/>
+        <f t="shared" si="73"/>
         <v/>
       </c>
       <c r="V359" s="209" t="str">
-        <f t="shared" si="72"/>
+        <f t="shared" si="73"/>
         <v/>
       </c>
       <c r="W359" s="237" t="str">
@@ -42959,23 +42964,23 @@
         <v/>
       </c>
       <c r="R360" s="121">
-        <f t="shared" si="71"/>
+        <f t="shared" si="72"/>
         <v>28</v>
       </c>
       <c r="S360" s="121">
-        <f t="shared" si="71"/>
+        <f t="shared" si="72"/>
         <v>50</v>
       </c>
       <c r="T360" s="209" t="str">
+        <f t="shared" si="74"/>
+        <v/>
+      </c>
+      <c r="U360" s="211" t="str">
         <f t="shared" si="73"/>
         <v/>
       </c>
-      <c r="U360" s="211" t="str">
-        <f t="shared" si="72"/>
-        <v/>
-      </c>
       <c r="V360" s="209" t="str">
-        <f t="shared" si="72"/>
+        <f t="shared" si="73"/>
         <v/>
       </c>
       <c r="W360" s="237" t="str">
@@ -43015,23 +43020,23 @@
         <v/>
       </c>
       <c r="R361" s="121">
-        <f t="shared" si="71"/>
+        <f t="shared" si="72"/>
         <v>28</v>
       </c>
       <c r="S361" s="121">
-        <f t="shared" si="71"/>
+        <f t="shared" si="72"/>
         <v>50</v>
       </c>
       <c r="T361" s="588" t="str">
+        <f t="shared" si="74"/>
+        <v/>
+      </c>
+      <c r="U361" s="589" t="str">
         <f t="shared" si="73"/>
         <v/>
       </c>
-      <c r="U361" s="589" t="str">
-        <f t="shared" si="72"/>
-        <v/>
-      </c>
       <c r="V361" s="588" t="str">
-        <f t="shared" si="72"/>
+        <f t="shared" si="73"/>
         <v/>
       </c>
       <c r="W361" s="590" t="str">
@@ -43293,19 +43298,19 @@
         <v>28</v>
       </c>
       <c r="D367" s="209" t="str">
-        <f t="shared" ref="D367:D373" si="74">IF(T358="","",T358)</f>
+        <f t="shared" ref="D367:D373" si="75">IF(T358="","",T358)</f>
         <v/>
       </c>
       <c r="E367" s="209" t="str">
-        <f t="shared" ref="E367:G373" si="75">IF(V358="","",V358)</f>
+        <f t="shared" ref="E367:G373" si="76">IF(V358="","",V358)</f>
         <v/>
       </c>
       <c r="F367" s="237" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
       <c r="G367" s="209" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
       <c r="H367" s="5"/>
@@ -43336,19 +43341,19 @@
       <c r="B368" s="39"/>
       <c r="C368" s="5"/>
       <c r="D368" s="209" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v/>
       </c>
       <c r="E368" s="209" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
       <c r="F368" s="237" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
       <c r="G368" s="209" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
       <c r="H368" s="5"/>
@@ -43379,19 +43384,19 @@
       <c r="B369" s="39"/>
       <c r="C369" s="5"/>
       <c r="D369" s="209" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v/>
       </c>
       <c r="E369" s="209" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
       <c r="F369" s="237" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
       <c r="G369" s="209" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
       <c r="H369" s="5"/>
@@ -43422,19 +43427,19 @@
       <c r="B370" s="39"/>
       <c r="C370" s="5"/>
       <c r="D370" s="209" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v/>
       </c>
       <c r="E370" s="209" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
       <c r="F370" s="237" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
       <c r="G370" s="209" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
       <c r="H370" s="5"/>
@@ -43449,13 +43454,13 @@
       <c r="Q370" s="5"/>
       <c r="R370" s="5"/>
       <c r="S370" s="5"/>
-      <c r="T370" s="663" t="s">
+      <c r="T370" s="680" t="s">
         <v>308</v>
       </c>
-      <c r="U370" s="663"/>
-      <c r="V370" s="663"/>
-      <c r="W370" s="663"/>
-      <c r="X370" s="663"/>
+      <c r="U370" s="680"/>
+      <c r="V370" s="680"/>
+      <c r="W370" s="680"/>
+      <c r="X370" s="680"/>
       <c r="Y370" s="15"/>
     </row>
     <row r="371" spans="1:25">
@@ -43467,19 +43472,19 @@
         <v>169</v>
       </c>
       <c r="D371" s="209" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v/>
       </c>
       <c r="E371" s="209" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
       <c r="F371" s="237" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
       <c r="G371" s="209" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
       <c r="H371" s="5"/>
@@ -43528,19 +43533,19 @@
         <v>328</v>
       </c>
       <c r="D372" s="209" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v/>
       </c>
       <c r="E372" s="209" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
       <c r="F372" s="237" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
       <c r="G372" s="209" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
       <c r="H372" s="5"/>
@@ -43598,19 +43603,19 @@
         <v>291</v>
       </c>
       <c r="D373" s="286" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v/>
       </c>
       <c r="E373" s="286" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
       <c r="F373" s="286" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
       <c r="G373" s="286" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v/>
       </c>
       <c r="H373" s="5"/>
@@ -43708,15 +43713,15 @@
         <v>100</v>
       </c>
       <c r="T374" s="209" t="str">
-        <f t="shared" ref="T374:V375" si="76">IF(AM38="","",AM38)</f>
+        <f t="shared" ref="T374:V375" si="77">IF(AM38="","",AM38)</f>
         <v/>
       </c>
       <c r="U374" s="211" t="str">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v/>
       </c>
       <c r="V374" s="209" t="str">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v/>
       </c>
       <c r="W374" s="237" t="str">
@@ -43768,15 +43773,15 @@
         <v>300</v>
       </c>
       <c r="T375" s="209" t="str">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v/>
       </c>
       <c r="U375" s="211" t="str">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v/>
       </c>
       <c r="V375" s="209" t="str">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v/>
       </c>
       <c r="W375" s="237" t="str">
@@ -44096,23 +44101,23 @@
       </c>
       <c r="B383" s="39"/>
       <c r="C383" s="121">
-        <f t="shared" ref="C383:D386" si="77">IF(S372="","",S372)</f>
+        <f t="shared" ref="C383:D386" si="78">IF(S372="","",S372)</f>
         <v>20</v>
       </c>
       <c r="D383" s="209" t="str">
-        <f t="shared" si="77"/>
+        <f t="shared" si="78"/>
         <v/>
       </c>
       <c r="E383" s="209" t="str">
-        <f t="shared" ref="E383:G386" si="78">IF(V372="","",V372)</f>
+        <f t="shared" ref="E383:G386" si="79">IF(V372="","",V372)</f>
         <v/>
       </c>
       <c r="F383" s="237" t="str">
-        <f t="shared" si="78"/>
+        <f t="shared" si="79"/>
         <v/>
       </c>
       <c r="G383" s="209" t="str">
-        <f t="shared" si="78"/>
+        <f t="shared" si="79"/>
         <v/>
       </c>
       <c r="H383" s="5"/>
@@ -44126,16 +44131,16 @@
       <c r="P383" s="299" t="s">
         <v>340</v>
       </c>
-      <c r="Q383" s="664" t="s">
+      <c r="Q383" s="688" t="s">
         <v>341</v>
       </c>
-      <c r="R383" s="664"/>
-      <c r="S383" s="664"/>
-      <c r="T383" s="664"/>
-      <c r="U383" s="664"/>
-      <c r="V383" s="664"/>
-      <c r="W383" s="664"/>
-      <c r="X383" s="664"/>
+      <c r="R383" s="688"/>
+      <c r="S383" s="688"/>
+      <c r="T383" s="688"/>
+      <c r="U383" s="688"/>
+      <c r="V383" s="688"/>
+      <c r="W383" s="688"/>
+      <c r="X383" s="688"/>
       <c r="Y383" s="15"/>
     </row>
     <row r="384" spans="1:25">
@@ -44144,23 +44149,23 @@
       </c>
       <c r="B384" s="39"/>
       <c r="C384" s="121">
-        <f t="shared" si="77"/>
+        <f t="shared" si="78"/>
         <v>50</v>
       </c>
       <c r="D384" s="209" t="str">
-        <f t="shared" si="77"/>
+        <f t="shared" si="78"/>
         <v/>
       </c>
       <c r="E384" s="209" t="str">
-        <f t="shared" si="78"/>
+        <f t="shared" si="79"/>
         <v/>
       </c>
       <c r="F384" s="237" t="str">
-        <f t="shared" si="78"/>
+        <f t="shared" si="79"/>
         <v/>
       </c>
       <c r="G384" s="209" t="str">
-        <f t="shared" si="78"/>
+        <f t="shared" si="79"/>
         <v/>
       </c>
       <c r="H384" s="5"/>
@@ -44214,23 +44219,23 @@
       </c>
       <c r="B385" s="39"/>
       <c r="C385" s="121">
-        <f t="shared" si="77"/>
+        <f t="shared" si="78"/>
         <v>100</v>
       </c>
       <c r="D385" s="209" t="str">
-        <f t="shared" si="77"/>
+        <f t="shared" si="78"/>
         <v/>
       </c>
       <c r="E385" s="209" t="str">
-        <f t="shared" si="78"/>
+        <f t="shared" si="79"/>
         <v/>
       </c>
       <c r="F385" s="237" t="str">
-        <f t="shared" si="78"/>
+        <f t="shared" si="79"/>
         <v/>
       </c>
       <c r="G385" s="209" t="str">
-        <f t="shared" si="78"/>
+        <f t="shared" si="79"/>
         <v/>
       </c>
       <c r="H385" s="5"/>
@@ -44284,23 +44289,23 @@
       </c>
       <c r="B386" s="39"/>
       <c r="C386" s="121">
-        <f t="shared" si="77"/>
+        <f t="shared" si="78"/>
         <v>300</v>
       </c>
       <c r="D386" s="209" t="str">
-        <f t="shared" si="77"/>
+        <f t="shared" si="78"/>
         <v/>
       </c>
       <c r="E386" s="209" t="str">
-        <f t="shared" si="78"/>
+        <f t="shared" si="79"/>
         <v/>
       </c>
       <c r="F386" s="237" t="str">
-        <f t="shared" si="78"/>
+        <f t="shared" si="79"/>
         <v/>
       </c>
       <c r="G386" s="209" t="str">
-        <f t="shared" si="78"/>
+        <f t="shared" si="79"/>
         <v/>
       </c>
       <c r="H386" s="5"/>
@@ -44375,35 +44380,35 @@
         <v>343</v>
       </c>
       <c r="Q387" s="461" t="str">
-        <f t="shared" ref="Q387:X387" si="79">IF(OR(Q384="",Q385=""),"",ABS(Q385-Q384)/Q384)</f>
+        <f t="shared" ref="Q387:X387" si="80">IF(OR(Q384="",Q385=""),"",ABS(Q385-Q384)/Q384)</f>
         <v/>
       </c>
       <c r="R387" s="461" t="str">
-        <f t="shared" si="79"/>
+        <f t="shared" si="80"/>
         <v/>
       </c>
       <c r="S387" s="461" t="str">
-        <f t="shared" si="79"/>
+        <f t="shared" si="80"/>
         <v/>
       </c>
       <c r="T387" s="461" t="str">
-        <f t="shared" si="79"/>
+        <f t="shared" si="80"/>
         <v/>
       </c>
       <c r="U387" s="461" t="str">
-        <f t="shared" si="79"/>
+        <f t="shared" si="80"/>
         <v/>
       </c>
       <c r="V387" s="461" t="str">
-        <f t="shared" si="79"/>
+        <f t="shared" si="80"/>
         <v/>
       </c>
       <c r="W387" s="461" t="str">
-        <f t="shared" si="79"/>
+        <f t="shared" si="80"/>
         <v/>
       </c>
       <c r="X387" s="462" t="str">
-        <f t="shared" si="79"/>
+        <f t="shared" si="80"/>
         <v/>
       </c>
       <c r="Y387" s="15"/>
@@ -44434,35 +44439,35 @@
         <v>344</v>
       </c>
       <c r="Q388" s="311">
-        <f t="shared" ref="Q388:X388" si="80">IF($Q$380=1,Q382/100+0.03,Q382/100)</f>
+        <f t="shared" ref="Q388:X388" si="81">IF($Q$380=1,Q382/100+0.03,Q382/100)</f>
         <v>0.27</v>
       </c>
       <c r="R388" s="311">
-        <f t="shared" si="80"/>
+        <f t="shared" si="81"/>
         <v>0.28000000000000003</v>
       </c>
       <c r="S388" s="311">
-        <f t="shared" si="80"/>
+        <f t="shared" si="81"/>
         <v>0.31000000000000005</v>
       </c>
       <c r="T388" s="311">
-        <f t="shared" si="80"/>
+        <f t="shared" si="81"/>
         <v>0.35</v>
       </c>
       <c r="U388" s="311">
-        <f t="shared" si="80"/>
+        <f t="shared" si="81"/>
         <v>0.31000000000000005</v>
       </c>
       <c r="V388" s="311">
-        <f t="shared" si="80"/>
+        <f t="shared" si="81"/>
         <v>0.32999999999999996</v>
       </c>
       <c r="W388" s="311">
-        <f t="shared" si="80"/>
+        <f t="shared" si="81"/>
         <v>0.35</v>
       </c>
       <c r="X388" s="312">
-        <f t="shared" si="80"/>
+        <f t="shared" si="81"/>
         <v>0.37</v>
       </c>
       <c r="Y388" s="15"/>
@@ -44641,35 +44646,35 @@
         <v>240</v>
       </c>
       <c r="D392" s="65">
-        <f t="shared" ref="D392:K392" si="81">Q382</f>
+        <f t="shared" ref="D392:K392" si="82">Q382</f>
         <v>24</v>
       </c>
       <c r="E392" s="65">
-        <f t="shared" si="81"/>
+        <f t="shared" si="82"/>
         <v>25</v>
       </c>
       <c r="F392" s="65">
-        <f t="shared" si="81"/>
+        <f t="shared" si="82"/>
         <v>28</v>
       </c>
       <c r="G392" s="65">
-        <f t="shared" si="81"/>
+        <f t="shared" si="82"/>
         <v>32</v>
       </c>
       <c r="H392" s="65">
-        <f t="shared" si="81"/>
+        <f t="shared" si="82"/>
         <v>28</v>
       </c>
       <c r="I392" s="65">
-        <f t="shared" si="81"/>
+        <f t="shared" si="82"/>
         <v>30</v>
       </c>
       <c r="J392" s="65">
-        <f t="shared" si="81"/>
+        <f t="shared" si="82"/>
         <v>32</v>
       </c>
       <c r="K392" s="65">
-        <f t="shared" si="81"/>
+        <f t="shared" si="82"/>
         <v>34</v>
       </c>
       <c r="L392" s="5"/>
@@ -44700,35 +44705,35 @@
         <v>342</v>
       </c>
       <c r="D393" s="318" t="str">
-        <f t="shared" ref="D393:K394" si="82">IF(Q386="","",Q386)</f>
+        <f t="shared" ref="D393:K394" si="83">IF(Q386="","",Q386)</f>
         <v/>
       </c>
       <c r="E393" s="318" t="str">
-        <f t="shared" si="82"/>
+        <f t="shared" si="83"/>
         <v/>
       </c>
       <c r="F393" s="318" t="str">
-        <f t="shared" si="82"/>
+        <f t="shared" si="83"/>
         <v/>
       </c>
       <c r="G393" s="318" t="str">
-        <f t="shared" si="82"/>
+        <f t="shared" si="83"/>
         <v/>
       </c>
       <c r="H393" s="318" t="str">
-        <f t="shared" si="82"/>
+        <f t="shared" si="83"/>
         <v/>
       </c>
       <c r="I393" s="318" t="str">
-        <f t="shared" si="82"/>
+        <f t="shared" si="83"/>
         <v/>
       </c>
       <c r="J393" s="318" t="str">
-        <f t="shared" si="82"/>
+        <f t="shared" si="83"/>
         <v/>
       </c>
       <c r="K393" s="219" t="str">
-        <f t="shared" si="82"/>
+        <f t="shared" si="83"/>
         <v/>
       </c>
       <c r="L393" s="5"/>
@@ -44757,35 +44762,35 @@
         <v>343</v>
       </c>
       <c r="D394" s="448" t="str">
-        <f t="shared" si="82"/>
+        <f t="shared" si="83"/>
         <v/>
       </c>
       <c r="E394" s="448" t="str">
-        <f t="shared" si="82"/>
+        <f t="shared" si="83"/>
         <v/>
       </c>
       <c r="F394" s="448" t="str">
-        <f t="shared" si="82"/>
+        <f t="shared" si="83"/>
         <v/>
       </c>
       <c r="G394" s="448" t="str">
-        <f t="shared" si="82"/>
+        <f t="shared" si="83"/>
         <v/>
       </c>
       <c r="H394" s="448" t="str">
-        <f t="shared" si="82"/>
+        <f t="shared" si="83"/>
         <v/>
       </c>
       <c r="I394" s="448" t="str">
-        <f t="shared" si="82"/>
+        <f t="shared" si="83"/>
         <v/>
       </c>
       <c r="J394" s="448" t="str">
-        <f t="shared" si="82"/>
+        <f t="shared" si="83"/>
         <v/>
       </c>
       <c r="K394" s="450" t="str">
-        <f t="shared" si="82"/>
+        <f t="shared" si="83"/>
         <v/>
       </c>
       <c r="L394" s="5"/>
@@ -44829,35 +44834,35 @@
         <v>344</v>
       </c>
       <c r="D395" s="318">
-        <f t="shared" ref="D395:K397" si="83">Q388</f>
+        <f t="shared" ref="D395:K397" si="84">Q388</f>
         <v>0.27</v>
       </c>
       <c r="E395" s="318">
-        <f t="shared" si="83"/>
+        <f t="shared" si="84"/>
         <v>0.28000000000000003</v>
       </c>
       <c r="F395" s="318">
-        <f t="shared" si="83"/>
+        <f t="shared" si="84"/>
         <v>0.31000000000000005</v>
       </c>
       <c r="G395" s="318">
-        <f t="shared" si="83"/>
+        <f t="shared" si="84"/>
         <v>0.35</v>
       </c>
       <c r="H395" s="318">
-        <f t="shared" si="83"/>
+        <f t="shared" si="84"/>
         <v>0.31000000000000005</v>
       </c>
       <c r="I395" s="318">
-        <f t="shared" si="83"/>
+        <f t="shared" si="84"/>
         <v>0.32999999999999996</v>
       </c>
       <c r="J395" s="318">
-        <f t="shared" si="83"/>
+        <f t="shared" si="84"/>
         <v>0.35</v>
       </c>
       <c r="K395" s="219">
-        <f t="shared" si="83"/>
+        <f t="shared" si="84"/>
         <v>0.37</v>
       </c>
       <c r="L395" s="5"/>
@@ -44901,35 +44906,35 @@
         <v>345</v>
       </c>
       <c r="D396" s="214">
-        <f t="shared" si="83"/>
+        <f t="shared" si="84"/>
         <v>0.36</v>
       </c>
       <c r="E396" s="214">
-        <f t="shared" si="83"/>
+        <f t="shared" si="84"/>
         <v>0.37</v>
       </c>
       <c r="F396" s="214">
-        <f t="shared" si="83"/>
+        <f t="shared" si="84"/>
         <v>0.4</v>
       </c>
       <c r="G396" s="214">
-        <f t="shared" si="83"/>
+        <f t="shared" si="84"/>
         <v>0.44</v>
       </c>
       <c r="H396" s="214">
-        <f t="shared" si="83"/>
+        <f t="shared" si="84"/>
         <v>0.47000000000000003</v>
       </c>
       <c r="I396" s="214">
-        <f t="shared" si="83"/>
+        <f t="shared" si="84"/>
         <v>0.49</v>
       </c>
       <c r="J396" s="214">
-        <f t="shared" si="83"/>
+        <f t="shared" si="84"/>
         <v>0.51</v>
       </c>
       <c r="K396" s="225">
-        <f t="shared" si="83"/>
+        <f t="shared" si="84"/>
         <v>0.53</v>
       </c>
       <c r="L396" s="5"/>
@@ -44939,13 +44944,13 @@
       <c r="P396" s="299" t="s">
         <v>340</v>
       </c>
-      <c r="Q396" s="664" t="s">
+      <c r="Q396" s="688" t="s">
         <v>341</v>
       </c>
-      <c r="R396" s="664"/>
-      <c r="S396" s="664"/>
-      <c r="T396" s="664"/>
-      <c r="U396" s="664"/>
+      <c r="R396" s="688"/>
+      <c r="S396" s="688"/>
+      <c r="T396" s="688"/>
+      <c r="U396" s="688"/>
       <c r="V396" s="77"/>
       <c r="W396" s="77"/>
       <c r="X396" s="77"/>
@@ -44960,35 +44965,35 @@
         <v>180</v>
       </c>
       <c r="D397" s="171" t="str">
-        <f t="shared" si="83"/>
+        <f t="shared" si="84"/>
         <v/>
       </c>
       <c r="E397" s="172" t="str">
-        <f t="shared" si="83"/>
+        <f t="shared" si="84"/>
         <v/>
       </c>
       <c r="F397" s="172" t="str">
-        <f t="shared" si="83"/>
+        <f t="shared" si="84"/>
         <v/>
       </c>
       <c r="G397" s="172" t="str">
-        <f t="shared" si="83"/>
+        <f t="shared" si="84"/>
         <v/>
       </c>
       <c r="H397" s="172" t="str">
-        <f t="shared" si="83"/>
+        <f t="shared" si="84"/>
         <v/>
       </c>
       <c r="I397" s="172" t="str">
-        <f t="shared" si="83"/>
+        <f t="shared" si="84"/>
         <v/>
       </c>
       <c r="J397" s="172" t="str">
-        <f t="shared" si="83"/>
+        <f t="shared" si="84"/>
         <v/>
       </c>
       <c r="K397" s="174" t="str">
-        <f t="shared" si="83"/>
+        <f t="shared" si="84"/>
         <v/>
       </c>
       <c r="L397" s="5"/>
@@ -45204,23 +45209,23 @@
         <v>342</v>
       </c>
       <c r="D401" s="318" t="str">
-        <f t="shared" ref="D401:H404" si="84">IF(Q399="","",Q399)</f>
+        <f t="shared" ref="D401:H404" si="85">IF(Q399="","",Q399)</f>
         <v/>
       </c>
       <c r="E401" s="318" t="str">
-        <f t="shared" si="84"/>
+        <f t="shared" si="85"/>
         <v/>
       </c>
       <c r="F401" s="318" t="str">
-        <f t="shared" si="84"/>
+        <f t="shared" si="85"/>
         <v/>
       </c>
       <c r="G401" s="318" t="str">
-        <f t="shared" si="84"/>
+        <f t="shared" si="85"/>
         <v/>
       </c>
       <c r="H401" s="318" t="str">
-        <f t="shared" si="84"/>
+        <f t="shared" si="85"/>
         <v/>
       </c>
       <c r="I401" s="5"/>
@@ -45267,23 +45272,23 @@
         <v>343</v>
       </c>
       <c r="D402" s="448" t="str">
-        <f t="shared" si="84"/>
+        <f t="shared" si="85"/>
         <v/>
       </c>
       <c r="E402" s="448" t="str">
-        <f t="shared" si="84"/>
+        <f t="shared" si="85"/>
         <v/>
       </c>
       <c r="F402" s="448" t="str">
-        <f t="shared" si="84"/>
+        <f t="shared" si="85"/>
         <v/>
       </c>
       <c r="G402" s="448" t="str">
-        <f t="shared" si="84"/>
+        <f t="shared" si="85"/>
         <v/>
       </c>
       <c r="H402" s="448" t="str">
-        <f t="shared" si="84"/>
+        <f t="shared" si="85"/>
         <v/>
       </c>
       <c r="I402" s="5"/>
@@ -45330,23 +45335,23 @@
         <v>344</v>
       </c>
       <c r="D403" s="318">
-        <f t="shared" si="84"/>
+        <f t="shared" si="85"/>
         <v>0.31000000000000005</v>
       </c>
       <c r="E403" s="318">
-        <f t="shared" si="84"/>
+        <f t="shared" si="85"/>
         <v>0.32999999999999996</v>
       </c>
       <c r="F403" s="318">
-        <f t="shared" si="84"/>
+        <f t="shared" si="85"/>
         <v>0.35</v>
       </c>
       <c r="G403" s="318">
-        <f t="shared" si="84"/>
+        <f t="shared" si="85"/>
         <v>0.37</v>
       </c>
       <c r="H403" s="318">
-        <f t="shared" si="84"/>
+        <f t="shared" si="85"/>
         <v>0.41000000000000003</v>
       </c>
       <c r="I403" s="5"/>
@@ -45391,23 +45396,23 @@
         <v>345</v>
       </c>
       <c r="D404" s="214">
-        <f t="shared" si="84"/>
+        <f t="shared" si="85"/>
         <v>0.4</v>
       </c>
       <c r="E404" s="214">
-        <f t="shared" si="84"/>
+        <f t="shared" si="85"/>
         <v>0.42</v>
       </c>
       <c r="F404" s="214">
-        <f t="shared" si="84"/>
+        <f t="shared" si="85"/>
         <v>0.44</v>
       </c>
       <c r="G404" s="214">
-        <f t="shared" si="84"/>
+        <f t="shared" si="85"/>
         <v>0.46</v>
       </c>
       <c r="H404" s="214">
-        <f t="shared" si="84"/>
+        <f t="shared" si="85"/>
         <v>0.57000000000000006</v>
       </c>
       <c r="I404" s="5"/>
@@ -45657,7 +45662,7 @@
         <v>0</v>
       </c>
       <c r="R410" s="186" t="str">
-        <f t="shared" ref="R410:R415" si="85">IF(AB99="","",AB99)</f>
+        <f t="shared" ref="R410:R415" si="86">IF(AB99="","",AB99)</f>
         <v/>
       </c>
       <c r="S410" s="5"/>
@@ -45697,7 +45702,7 @@
         <v>0</v>
       </c>
       <c r="R411" s="186" t="str">
-        <f t="shared" si="85"/>
+        <f t="shared" si="86"/>
         <v/>
       </c>
       <c r="S411" s="5"/>
@@ -45734,7 +45739,7 @@
       </c>
       <c r="Q412" s="111"/>
       <c r="R412" s="186" t="str">
-        <f t="shared" si="85"/>
+        <f t="shared" si="86"/>
         <v/>
       </c>
       <c r="S412" s="5"/>
@@ -45771,7 +45776,7 @@
       </c>
       <c r="Q413" s="111"/>
       <c r="R413" s="186" t="str">
-        <f t="shared" si="85"/>
+        <f t="shared" si="86"/>
         <v/>
       </c>
       <c r="S413" s="5"/>
@@ -45808,7 +45813,7 @@
       </c>
       <c r="Q414" s="111"/>
       <c r="R414" s="186" t="str">
-        <f t="shared" si="85"/>
+        <f t="shared" si="86"/>
         <v/>
       </c>
       <c r="S414" s="5"/>
@@ -45843,7 +45848,7 @@
         <v/>
       </c>
       <c r="R415" s="186" t="str">
-        <f t="shared" si="85"/>
+        <f t="shared" si="86"/>
         <v/>
       </c>
       <c r="S415" s="5"/>
@@ -46187,17 +46192,17 @@
         <v>0</v>
       </c>
       <c r="Q426" s="332" t="str">
-        <f t="shared" ref="Q426:Q431" si="86">IF(AB109="","",AB109)</f>
+        <f t="shared" ref="Q426:Q431" si="87">IF(AB109="","",AB109)</f>
         <v/>
       </c>
       <c r="R426" s="198"/>
       <c r="S426" s="332" t="str">
-        <f t="shared" ref="S426:S431" si="87">IF(AB115="","",AB115)</f>
+        <f t="shared" ref="S426:S431" si="88">IF(AB115="","",AB115)</f>
         <v/>
       </c>
       <c r="T426" s="198"/>
       <c r="U426" s="332" t="str">
-        <f t="shared" ref="U426:U431" si="88">IF(AB121="","",AB121)</f>
+        <f t="shared" ref="U426:U431" si="89">IF(AB121="","",AB121)</f>
         <v/>
       </c>
       <c r="V426" s="77"/>
@@ -46228,17 +46233,17 @@
         <v>0</v>
       </c>
       <c r="Q427" s="332" t="str">
-        <f t="shared" si="86"/>
+        <f t="shared" si="87"/>
         <v/>
       </c>
       <c r="R427" s="198"/>
       <c r="S427" s="332" t="str">
-        <f t="shared" si="87"/>
+        <f t="shared" si="88"/>
         <v/>
       </c>
       <c r="T427" s="198"/>
       <c r="U427" s="332" t="str">
-        <f t="shared" si="88"/>
+        <f t="shared" si="89"/>
         <v/>
       </c>
       <c r="V427" s="77"/>
@@ -46269,17 +46274,17 @@
         <v>0</v>
       </c>
       <c r="Q428" s="332" t="str">
-        <f t="shared" si="86"/>
+        <f t="shared" si="87"/>
         <v/>
       </c>
       <c r="R428" s="198"/>
       <c r="S428" s="332" t="str">
-        <f t="shared" si="87"/>
+        <f t="shared" si="88"/>
         <v/>
       </c>
       <c r="T428" s="198"/>
       <c r="U428" s="332" t="str">
-        <f t="shared" si="88"/>
+        <f t="shared" si="89"/>
         <v/>
       </c>
       <c r="V428" s="77"/>
@@ -46307,17 +46312,17 @@
       </c>
       <c r="P429" s="198"/>
       <c r="Q429" s="332" t="str">
-        <f t="shared" si="86"/>
+        <f t="shared" si="87"/>
         <v/>
       </c>
       <c r="R429" s="198"/>
       <c r="S429" s="332" t="str">
-        <f t="shared" si="87"/>
+        <f t="shared" si="88"/>
         <v/>
       </c>
       <c r="T429" s="198"/>
       <c r="U429" s="332" t="str">
-        <f t="shared" si="88"/>
+        <f t="shared" si="89"/>
         <v/>
       </c>
       <c r="V429" s="77"/>
@@ -46345,17 +46350,17 @@
       </c>
       <c r="P430" s="198"/>
       <c r="Q430" s="332" t="str">
-        <f t="shared" si="86"/>
+        <f t="shared" si="87"/>
         <v/>
       </c>
       <c r="R430" s="198"/>
       <c r="S430" s="332" t="str">
-        <f t="shared" si="87"/>
+        <f t="shared" si="88"/>
         <v/>
       </c>
       <c r="T430" s="198"/>
       <c r="U430" s="332" t="str">
-        <f t="shared" si="88"/>
+        <f t="shared" si="89"/>
         <v/>
       </c>
       <c r="V430" s="77"/>
@@ -46383,17 +46388,17 @@
       </c>
       <c r="P431" s="202"/>
       <c r="Q431" s="333" t="str">
-        <f t="shared" si="86"/>
+        <f t="shared" si="87"/>
         <v/>
       </c>
       <c r="R431" s="202"/>
       <c r="S431" s="333" t="str">
-        <f t="shared" si="87"/>
+        <f t="shared" si="88"/>
         <v/>
       </c>
       <c r="T431" s="202"/>
       <c r="U431" s="333" t="str">
-        <f t="shared" si="88"/>
+        <f t="shared" si="89"/>
         <v/>
       </c>
       <c r="V431" s="77"/>
@@ -47495,58 +47500,22 @@
     </row>
   </sheetData>
   <mergeCells count="84">
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="D35:F36"/>
-    <mergeCell ref="G35:I36"/>
-    <mergeCell ref="J35:L36"/>
-    <mergeCell ref="L44:M44"/>
-    <mergeCell ref="P97:R98"/>
-    <mergeCell ref="V97:X98"/>
-    <mergeCell ref="P105:R106"/>
-    <mergeCell ref="S105:U106"/>
-    <mergeCell ref="V105:X106"/>
-    <mergeCell ref="P150:S150"/>
-    <mergeCell ref="U150:V150"/>
-    <mergeCell ref="S97:U98"/>
-    <mergeCell ref="I173:J173"/>
-    <mergeCell ref="U151:V151"/>
-    <mergeCell ref="U152:V152"/>
-    <mergeCell ref="P156:P157"/>
-    <mergeCell ref="Q156:S156"/>
-    <mergeCell ref="U156:U157"/>
-    <mergeCell ref="P164:U164"/>
-    <mergeCell ref="P165:P166"/>
-    <mergeCell ref="Q165:S165"/>
-    <mergeCell ref="U165:U166"/>
+    <mergeCell ref="T356:X356"/>
+    <mergeCell ref="T370:X370"/>
+    <mergeCell ref="Q383:X383"/>
+    <mergeCell ref="Q396:U396"/>
+    <mergeCell ref="T322:U322"/>
+    <mergeCell ref="T324:X324"/>
+    <mergeCell ref="T335:X335"/>
+    <mergeCell ref="I343:J343"/>
+    <mergeCell ref="I344:J344"/>
+    <mergeCell ref="T345:X345"/>
+    <mergeCell ref="D259:E259"/>
+    <mergeCell ref="G259:H259"/>
+    <mergeCell ref="K259:L259"/>
+    <mergeCell ref="E305:I305"/>
+    <mergeCell ref="E316:I316"/>
+    <mergeCell ref="T321:U321"/>
     <mergeCell ref="D172:G172"/>
     <mergeCell ref="I172:J172"/>
     <mergeCell ref="X246:Y246"/>
@@ -47563,22 +47532,58 @@
     <mergeCell ref="Q188:S188"/>
     <mergeCell ref="U188:U189"/>
     <mergeCell ref="D189:I189"/>
-    <mergeCell ref="I343:J343"/>
-    <mergeCell ref="I344:J344"/>
-    <mergeCell ref="T345:X345"/>
-    <mergeCell ref="D259:E259"/>
-    <mergeCell ref="G259:H259"/>
-    <mergeCell ref="K259:L259"/>
-    <mergeCell ref="E305:I305"/>
-    <mergeCell ref="E316:I316"/>
-    <mergeCell ref="T321:U321"/>
-    <mergeCell ref="T356:X356"/>
-    <mergeCell ref="T370:X370"/>
-    <mergeCell ref="Q383:X383"/>
-    <mergeCell ref="Q396:U396"/>
-    <mergeCell ref="T322:U322"/>
-    <mergeCell ref="T324:X324"/>
-    <mergeCell ref="T335:X335"/>
+    <mergeCell ref="I173:J173"/>
+    <mergeCell ref="U151:V151"/>
+    <mergeCell ref="U152:V152"/>
+    <mergeCell ref="P156:P157"/>
+    <mergeCell ref="Q156:S156"/>
+    <mergeCell ref="U156:U157"/>
+    <mergeCell ref="P164:U164"/>
+    <mergeCell ref="P165:P166"/>
+    <mergeCell ref="Q165:S165"/>
+    <mergeCell ref="U165:U166"/>
+    <mergeCell ref="V97:X98"/>
+    <mergeCell ref="P105:R106"/>
+    <mergeCell ref="S105:U106"/>
+    <mergeCell ref="V105:X106"/>
+    <mergeCell ref="P150:S150"/>
+    <mergeCell ref="U150:V150"/>
+    <mergeCell ref="S97:U98"/>
+    <mergeCell ref="D35:F36"/>
+    <mergeCell ref="G35:I36"/>
+    <mergeCell ref="J35:L36"/>
+    <mergeCell ref="L44:M44"/>
+    <mergeCell ref="P97:R98"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="K12:L12"/>
   </mergeCells>
   <conditionalFormatting sqref="P171:U172">
     <cfRule type="cellIs" dxfId="84" priority="87" operator="lessThan">
@@ -47941,9 +47946,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD196"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="J73" sqref="J73"/>
-    </sheetView>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <sheetData>
@@ -53515,9 +53518,9 @@
       <c r="B85">
         <v>24</v>
       </c>
-      <c r="C85" s="433" t="e">
-        <f>AVERAGE(Sheet1!AQ10:AQ11)</f>
-        <v>#DIV/0!</v>
+      <c r="C85" s="433" t="str">
+        <f>Sheet1!Q386</f>
+        <v/>
       </c>
       <c r="D85" t="str">
         <f>G73</f>
@@ -53526,9 +53529,9 @@
       <c r="E85">
         <v>28</v>
       </c>
-      <c r="F85" s="433" t="e">
-        <f>AVERAGE(Sheet1!AQ58:AQ59)</f>
-        <v>#DIV/0!</v>
+      <c r="F85" s="433" t="str">
+        <f>Sheet1!U386</f>
+        <v/>
       </c>
       <c r="G85" t="str">
         <f>M73</f>
@@ -53567,9 +53570,9 @@
       <c r="B86">
         <v>25</v>
       </c>
-      <c r="C86" s="433" t="e">
-        <f>AVERAGE(Sheet1!AQ18:AQ19)</f>
-        <v>#DIV/0!</v>
+      <c r="C86" s="433" t="str">
+        <f>Sheet1!R386</f>
+        <v/>
       </c>
       <c r="D86" t="s">
         <v>239</v>
@@ -53577,9 +53580,9 @@
       <c r="E86">
         <v>30</v>
       </c>
-      <c r="F86" s="433" t="e">
-        <f>AVERAGE(Sheet1!AQ66:AQ67)</f>
-        <v>#DIV/0!</v>
+      <c r="F86" s="433" t="str">
+        <f>Sheet1!V386</f>
+        <v/>
       </c>
       <c r="G86" t="s">
         <v>239</v>
@@ -53629,9 +53632,9 @@
       <c r="E87">
         <v>32</v>
       </c>
-      <c r="F87" s="433" t="e">
-        <f>AVERAGE(Sheet1!AQ74:AQ75)</f>
-        <v>#DIV/0!</v>
+      <c r="F87" s="433" t="str">
+        <f>Sheet1!W386</f>
+        <v/>
       </c>
       <c r="G87" t="str">
         <f>M75</f>
@@ -53667,16 +53670,16 @@
       <c r="B88">
         <v>28</v>
       </c>
-      <c r="C88" s="433" t="e">
-        <f>AVERAGE(Sheet1!AQ27:AQ31)</f>
-        <v>#DIV/0!</v>
+      <c r="C88" s="433" t="str">
+        <f>Sheet1!S386</f>
+        <v/>
       </c>
       <c r="E88">
         <v>34</v>
       </c>
-      <c r="F88" s="433" t="e">
-        <f>AVERAGE(Sheet1!AQ82:AQ83)</f>
-        <v>#DIV/0!</v>
+      <c r="F88" s="433" t="str">
+        <f>Sheet1!X386</f>
+        <v/>
       </c>
       <c r="H88">
         <v>34</v>
@@ -53749,9 +53752,9 @@
       <c r="B90">
         <v>32</v>
       </c>
-      <c r="C90" s="433" t="e">
-        <f>AVERAGE(Sheet1!AQ42:AQ43)</f>
-        <v>#DIV/0!</v>
+      <c r="C90" s="433" t="str">
+        <f>Sheet1!T386</f>
+        <v/>
       </c>
       <c r="E90">
         <v>38</v>
@@ -53784,9 +53787,9 @@
       <c r="E92" t="s">
         <v>608</v>
       </c>
-      <c r="F92" t="e">
+      <c r="F92">
         <f>SLOPE(F85:F90,E85:E90)</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="H92" t="s">
         <v>608</v>
@@ -53825,9 +53828,9 @@
       <c r="E93" t="s">
         <v>609</v>
       </c>
-      <c r="F93" t="e">
+      <c r="F93">
         <f>INTERCEPT(F85:F90,E85:E90)</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="H93" t="s">
         <v>609</v>
@@ -53897,13 +53900,13 @@
       </c>
     </row>
     <row r="95" spans="1:25">
-      <c r="A95" t="s">
+      <c r="A95" s="692" t="s">
         <v>405</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B95" s="692" t="s">
         <v>239</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C95" s="692" t="s">
         <v>611</v>
       </c>
       <c r="E95" t="s">
@@ -53932,13 +53935,13 @@
       </c>
     </row>
     <row r="96" spans="1:25">
-      <c r="A96" t="s">
+      <c r="A96" s="692" t="s">
         <v>614</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B96" s="692" t="s">
         <v>614</v>
       </c>
-      <c r="C96">
+      <c r="C96" s="692">
         <v>0.12</v>
       </c>
       <c r="F96" t="s">
@@ -53964,13 +53967,13 @@
       </c>
     </row>
     <row r="97" spans="1:25">
-      <c r="A97" t="s">
+      <c r="A97" s="692" t="s">
         <v>614</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B97" s="692" t="s">
         <v>616</v>
       </c>
-      <c r="C97">
+      <c r="C97" s="692">
         <v>0.19</v>
       </c>
       <c r="F97" t="s">
@@ -53996,13 +53999,13 @@
       </c>
     </row>
     <row r="98" spans="1:25">
-      <c r="A98" t="s">
+      <c r="A98" s="692" t="s">
         <v>616</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B98" s="692" t="s">
         <v>616</v>
       </c>
-      <c r="C98">
+      <c r="C98" s="692">
         <v>0.22</v>
       </c>
       <c r="T98" t="s">

</xml_diff>